<commit_message>
Cleaning up obs data
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B65190-F0B8-4746-B968-46F7747060CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63D498A-31E0-4F91-9CB9-154D15377937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{FBA18FA7-8D49-4A23-B648-57CB41343816}"/>
   </bookViews>
@@ -170,9 +170,6 @@
     <t>dw_OB</t>
   </si>
   <si>
-    <t>Cotton.Fruit.Wt</t>
-  </si>
-  <si>
     <t>Cotton.Fruit.Nconc</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>Cotton.Leaf.SpecificArea</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.Wt</t>
   </si>
 </sst>
 </file>
@@ -682,10 +682,10 @@
   <dimension ref="A1:BU142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D82" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AS2" sqref="AS2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -928,7 +928,7 @@
         <v>33</v>
       </c>
       <c r="AI1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AJ1" t="s">
         <v>34</v>
@@ -958,96 +958,96 @@
         <v>42</v>
       </c>
       <c r="AS1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>65</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>68</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>69</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>70</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1">
         <v>39783</v>
@@ -1056,16 +1056,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s">
         <v>72</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
         <v>73</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>74</v>
       </c>
       <c r="I2" s="3">
         <v>8.3000000000000007</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1">
         <v>39798</v>
@@ -1170,7 +1170,7 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I3" s="3">
         <v>8.3000000000000007</v>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="4" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1">
         <v>39804</v>
@@ -1257,16 +1257,16 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" t="s">
         <v>75</v>
-      </c>
-      <c r="F4" t="s">
-        <v>76</v>
       </c>
       <c r="G4">
         <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I4" s="3">
         <v>8.3000000000000007</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="1">
         <v>39806</v>
@@ -1355,7 +1355,7 @@
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I5" s="3">
         <v>8.3000000000000007</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="6" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1">
         <v>39813</v>
@@ -1444,7 +1444,7 @@
         <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I6" s="3">
         <v>8.3000000000000007</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="7" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="1">
         <v>39818</v>
@@ -1533,7 +1533,7 @@
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I7" s="3">
         <v>8.3000000000000007</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="8" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="1">
         <v>39819</v>
@@ -1654,7 +1654,7 @@
         <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I8" s="3">
         <v>8.3000000000000007</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="9" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1">
         <v>39825</v>
@@ -1741,16 +1741,16 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" t="s">
         <v>77</v>
-      </c>
-      <c r="F9" t="s">
-        <v>78</v>
       </c>
       <c r="G9">
         <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I9" s="3">
         <v>8.3000000000000007</v>
@@ -1866,7 +1866,7 @@
     </row>
     <row r="10" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1">
         <v>39827</v>
@@ -1877,7 +1877,7 @@
         <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I10" s="3">
         <v>8.3000000000000007</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="11" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="1">
         <v>39833</v>
@@ -1966,7 +1966,7 @@
         <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I11" s="3">
         <v>8.3000000000000007</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="12" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" s="1">
         <v>39840</v>
@@ -2055,7 +2055,7 @@
         <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I12" s="3">
         <v>8.3000000000000007</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="13" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1">
         <v>39841</v>
@@ -2144,7 +2144,7 @@
         <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I13" s="3">
         <v>8.3000000000000007</v>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="14" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="1">
         <v>39848</v>
@@ -2269,7 +2269,7 @@
         <v>65</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I14" s="3">
         <v>8.3000000000000007</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="15" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" s="1">
         <v>39853</v>
@@ -2356,16 +2356,16 @@
         <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
         <v>79</v>
-      </c>
-      <c r="F15" t="s">
-        <v>80</v>
       </c>
       <c r="G15">
         <v>70</v>
       </c>
       <c r="H15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I15" s="3">
         <v>8.3000000000000007</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="16" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1">
         <v>39854</v>
@@ -2490,7 +2490,7 @@
         <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I16" s="3">
         <v>8.3000000000000007</v>
@@ -2568,7 +2568,7 @@
     </row>
     <row r="17" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1">
         <v>39860</v>
@@ -2579,7 +2579,7 @@
         <v>77</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I17" s="3">
         <v>8.3000000000000007</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="18" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" s="1">
         <v>39874</v>
@@ -2668,7 +2668,7 @@
         <v>91</v>
       </c>
       <c r="H18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I18" s="3">
         <v>8.3000000000000007</v>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="19" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="1">
         <v>39875</v>
@@ -2757,7 +2757,7 @@
         <v>92</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I19" s="3">
         <v>8.3000000000000007</v>
@@ -2871,7 +2871,7 @@
     </row>
     <row r="20" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1">
         <v>39877</v>
@@ -2880,16 +2880,16 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" t="s">
         <v>81</v>
-      </c>
-      <c r="F20" t="s">
-        <v>82</v>
       </c>
       <c r="G20">
         <v>94</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I20" s="3">
         <v>8.3000000000000007</v>
@@ -2967,7 +2967,7 @@
     </row>
     <row r="21" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1">
         <v>39884</v>
@@ -2978,7 +2978,7 @@
         <v>101</v>
       </c>
       <c r="H21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I21" s="3">
         <v>8.3000000000000007</v>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="22" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="1">
         <v>39889</v>
@@ -3067,7 +3067,7 @@
         <v>106</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I22" s="3">
         <v>8.3000000000000007</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="23" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="1">
         <v>39895</v>
@@ -3192,7 +3192,7 @@
         <v>112</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I23" s="3">
         <v>8.3000000000000007</v>
@@ -3270,7 +3270,7 @@
     </row>
     <row r="24" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1">
         <v>39904</v>
@@ -3281,7 +3281,7 @@
         <v>121</v>
       </c>
       <c r="H24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I24" s="3">
         <v>8.3000000000000007</v>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="25" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1">
         <v>39910</v>
@@ -3372,7 +3372,7 @@
         <v>127</v>
       </c>
       <c r="H25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I25" s="3">
         <v>8.3000000000000007</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="26" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1">
         <v>39911</v>
@@ -3497,7 +3497,7 @@
         <v>128</v>
       </c>
       <c r="H26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I26" s="3">
         <v>8.3000000000000007</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="27" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="1">
         <v>39920</v>
@@ -3588,7 +3588,7 @@
         <v>137</v>
       </c>
       <c r="H27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I27" s="3">
         <v>8.3000000000000007</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="28" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="1">
         <v>39925</v>
@@ -3679,7 +3679,7 @@
         <v>142</v>
       </c>
       <c r="H28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I28" s="3">
         <v>8.3000000000000007</v>
@@ -3759,7 +3759,7 @@
     </row>
     <row r="29" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="1">
         <v>39932</v>
@@ -3770,7 +3770,7 @@
         <v>149</v>
       </c>
       <c r="H29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I29" s="3">
         <v>8.3000000000000007</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="30" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1">
         <v>39939</v>
@@ -3861,7 +3861,7 @@
         <v>156</v>
       </c>
       <c r="H30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I30" s="3">
         <v>8.3000000000000007</v>
@@ -3941,7 +3941,7 @@
     </row>
     <row r="31" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="1">
         <v>39946</v>
@@ -3952,7 +3952,7 @@
         <v>163</v>
       </c>
       <c r="H31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I31" s="3">
         <v>8.3000000000000007</v>
@@ -4032,7 +4032,7 @@
     </row>
     <row r="32" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="1">
         <v>39947</v>
@@ -4041,16 +4041,16 @@
         <v>9</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" t="s">
         <v>83</v>
-      </c>
-      <c r="F32" t="s">
-        <v>84</v>
       </c>
       <c r="G32">
         <v>164</v>
       </c>
       <c r="H32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I32" s="3">
         <v>8.3000000000000007</v>
@@ -4128,7 +4128,7 @@
     </row>
     <row r="33" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" s="1">
         <v>39954</v>
@@ -4139,7 +4139,7 @@
         <v>171</v>
       </c>
       <c r="H33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I33" s="3">
         <v>8.3000000000000007</v>
@@ -4219,7 +4219,7 @@
     </row>
     <row r="34" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" s="1">
         <v>39957</v>
@@ -4228,16 +4228,16 @@
         <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F34" t="s">
         <v>85</v>
-      </c>
-      <c r="F34" t="s">
-        <v>86</v>
       </c>
       <c r="G34">
         <v>174</v>
       </c>
       <c r="H34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I34" s="3">
         <v>8.3000000000000007</v>
@@ -4321,7 +4321,7 @@
     </row>
     <row r="35" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C35" s="1">
         <v>39960</v>
@@ -4332,7 +4332,7 @@
         <v>177</v>
       </c>
       <c r="H35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I35" s="3">
         <v>8.3000000000000007</v>
@@ -4412,7 +4412,7 @@
     </row>
     <row r="36" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="1">
         <v>39801</v>
@@ -4421,16 +4421,16 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" t="s">
         <v>72</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="H36" t="s">
         <v>73</v>
-      </c>
-      <c r="G36" s="2">
-        <v>0</v>
-      </c>
-      <c r="H36" t="s">
-        <v>74</v>
       </c>
       <c r="I36" s="3">
         <v>8.1</v>
@@ -4524,7 +4524,7 @@
     </row>
     <row r="37" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C37" s="1">
         <v>39819</v>
@@ -4535,7 +4535,7 @@
         <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I37" s="3">
         <v>8.1</v>
@@ -4613,7 +4613,7 @@
     </row>
     <row r="38" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" s="1">
         <v>39820</v>
@@ -4624,7 +4624,7 @@
         <v>19</v>
       </c>
       <c r="H38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I38" s="3">
         <v>8.1</v>
@@ -4720,7 +4720,7 @@
     </row>
     <row r="39" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="1">
         <v>39824</v>
@@ -4729,16 +4729,16 @@
         <v>4</v>
       </c>
       <c r="E39" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" t="s">
         <v>75</v>
-      </c>
-      <c r="F39" t="s">
-        <v>76</v>
       </c>
       <c r="G39">
         <v>23</v>
       </c>
       <c r="H39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I39" s="3">
         <v>8.1</v>
@@ -4816,7 +4816,7 @@
     </row>
     <row r="40" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" s="1">
         <v>39827</v>
@@ -4827,7 +4827,7 @@
         <v>26</v>
       </c>
       <c r="H40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I40" s="3">
         <v>8.1</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="41" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C41" s="1">
         <v>39833</v>
@@ -4916,7 +4916,7 @@
         <v>32</v>
       </c>
       <c r="H41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I41" s="3">
         <v>8.1</v>
@@ -5028,7 +5028,7 @@
     </row>
     <row r="42" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42" s="1">
         <v>39840</v>
@@ -5039,7 +5039,7 @@
         <v>39</v>
       </c>
       <c r="H42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I42" s="3">
         <v>8.1</v>
@@ -5117,7 +5117,7 @@
     </row>
     <row r="43" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C43" s="1">
         <v>39848</v>
@@ -5128,7 +5128,7 @@
         <v>47</v>
       </c>
       <c r="H43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I43" s="3">
         <v>8.1</v>
@@ -5244,7 +5244,7 @@
     </row>
     <row r="44" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C44" s="1">
         <v>39849</v>
@@ -5253,16 +5253,16 @@
         <v>4</v>
       </c>
       <c r="E44" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" t="s">
         <v>77</v>
-      </c>
-      <c r="F44" t="s">
-        <v>78</v>
       </c>
       <c r="G44">
         <v>48</v>
       </c>
       <c r="H44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I44" s="3">
         <v>8.1</v>
@@ -5340,7 +5340,7 @@
     </row>
     <row r="45" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" s="1">
         <v>39854</v>
@@ -5351,7 +5351,7 @@
         <v>53</v>
       </c>
       <c r="H45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I45" s="3">
         <v>8.1</v>
@@ -5429,7 +5429,7 @@
     </row>
     <row r="46" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C46" s="1">
         <v>39860</v>
@@ -5438,16 +5438,16 @@
         <v>6</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" t="s">
         <v>79</v>
-      </c>
-      <c r="F46" t="s">
-        <v>80</v>
       </c>
       <c r="G46" s="2">
         <v>59</v>
       </c>
       <c r="H46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I46" s="3">
         <v>8.1</v>
@@ -5563,7 +5563,7 @@
     </row>
     <row r="47" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" s="1">
         <v>39869</v>
@@ -5574,7 +5574,7 @@
         <v>68</v>
       </c>
       <c r="H47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I47" s="3">
         <v>8.1</v>
@@ -5652,7 +5652,7 @@
     </row>
     <row r="48" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C48" s="1">
         <v>39874</v>
@@ -5663,7 +5663,7 @@
         <v>73</v>
       </c>
       <c r="H48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I48" s="3">
         <v>8.1</v>
@@ -5741,7 +5741,7 @@
     </row>
     <row r="49" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C49" s="1">
         <v>39876</v>
@@ -5752,7 +5752,7 @@
         <v>75</v>
       </c>
       <c r="H49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I49" s="3">
         <v>8.1</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="50" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C50" s="1">
         <v>39884</v>
@@ -5877,7 +5877,7 @@
         <v>83</v>
       </c>
       <c r="H50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I50" s="3">
         <v>8.1</v>
@@ -5955,7 +5955,7 @@
     </row>
     <row r="51" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" s="1">
         <v>39888</v>
@@ -5966,7 +5966,7 @@
         <v>87</v>
       </c>
       <c r="H51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I51" s="3">
         <v>8.1</v>
@@ -6080,7 +6080,7 @@
     </row>
     <row r="52" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" s="1">
         <v>39895</v>
@@ -6091,7 +6091,7 @@
         <v>94</v>
       </c>
       <c r="H52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I52" s="3">
         <v>8.1</v>
@@ -6169,7 +6169,7 @@
     </row>
     <row r="53" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C53" s="1">
         <v>39904</v>
@@ -6180,7 +6180,7 @@
         <v>103</v>
       </c>
       <c r="H53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I53" s="3">
         <v>8.1</v>
@@ -6294,7 +6294,7 @@
     </row>
     <row r="54" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" s="1">
         <v>39908</v>
@@ -6305,7 +6305,7 @@
         <v>107</v>
       </c>
       <c r="H54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I54" s="3">
         <v>8.1</v>
@@ -6383,7 +6383,7 @@
     </row>
     <row r="55" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C55" s="1">
         <v>39911</v>
@@ -6394,7 +6394,7 @@
         <v>110</v>
       </c>
       <c r="H55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I55" s="3">
         <v>8.1</v>
@@ -6474,7 +6474,7 @@
     </row>
     <row r="56" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C56" s="1">
         <v>39920</v>
@@ -6485,7 +6485,7 @@
         <v>119</v>
       </c>
       <c r="H56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I56" s="3">
         <v>8.1</v>
@@ -6565,7 +6565,7 @@
     </row>
     <row r="57" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C57" s="1">
         <v>39922</v>
@@ -6574,16 +6574,16 @@
         <v>8</v>
       </c>
       <c r="E57" t="s">
+        <v>80</v>
+      </c>
+      <c r="F57" t="s">
         <v>81</v>
-      </c>
-      <c r="F57" t="s">
-        <v>82</v>
       </c>
       <c r="G57">
         <v>121</v>
       </c>
       <c r="H57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I57" s="3">
         <v>8.1</v>
@@ -6661,7 +6661,7 @@
     </row>
     <row r="58" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58" s="1">
         <v>39925</v>
@@ -6672,7 +6672,7 @@
         <v>124</v>
       </c>
       <c r="H58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I58" s="3">
         <v>8.1</v>
@@ -6752,7 +6752,7 @@
     </row>
     <row r="59" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C59" s="1">
         <v>39932</v>
@@ -6763,7 +6763,7 @@
         <v>131</v>
       </c>
       <c r="H59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I59" s="3">
         <v>8.1</v>
@@ -6881,7 +6881,7 @@
     </row>
     <row r="60" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C60" s="1">
         <v>39939</v>
@@ -6892,7 +6892,7 @@
         <v>138</v>
       </c>
       <c r="H60" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I60" s="3">
         <v>8.1</v>
@@ -6972,7 +6972,7 @@
     </row>
     <row r="61" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C61" s="1">
         <v>39945</v>
@@ -6981,16 +6981,16 @@
         <v>9</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F61" t="s">
         <v>83</v>
-      </c>
-      <c r="F61" t="s">
-        <v>84</v>
       </c>
       <c r="G61">
         <v>144</v>
       </c>
       <c r="H61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I61" s="3">
         <v>8.1</v>
@@ -7068,7 +7068,7 @@
     </row>
     <row r="62" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C62" s="1">
         <v>39946</v>
@@ -7079,7 +7079,7 @@
         <v>145</v>
       </c>
       <c r="H62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I62" s="3">
         <v>8.1</v>
@@ -7159,7 +7159,7 @@
     </row>
     <row r="63" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C63" s="1">
         <v>39954</v>
@@ -7170,7 +7170,7 @@
         <v>153</v>
       </c>
       <c r="H63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I63" s="3">
         <v>8.1</v>
@@ -7250,7 +7250,7 @@
     </row>
     <row r="64" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" s="1">
         <v>39960</v>
@@ -7259,16 +7259,16 @@
         <v>10</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F64" t="s">
         <v>85</v>
-      </c>
-      <c r="F64" t="s">
-        <v>86</v>
       </c>
       <c r="G64">
         <v>159</v>
       </c>
       <c r="H64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I64" s="3">
         <v>8.1</v>
@@ -7356,7 +7356,7 @@
     </row>
     <row r="65" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C65" s="1">
         <v>39820</v>
@@ -7365,16 +7365,16 @@
         <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" t="s">
         <v>72</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" s="2">
+        <v>0</v>
+      </c>
+      <c r="H65" t="s">
         <v>73</v>
-      </c>
-      <c r="G65" s="2">
-        <v>0</v>
-      </c>
-      <c r="H65" t="s">
-        <v>74</v>
       </c>
       <c r="I65" s="3">
         <v>8.3000000000000007</v>
@@ -7468,7 +7468,7 @@
     </row>
     <row r="66" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C66" s="1">
         <v>39846</v>
@@ -7477,16 +7477,16 @@
         <v>4</v>
       </c>
       <c r="E66" t="s">
+        <v>74</v>
+      </c>
+      <c r="F66" t="s">
         <v>75</v>
-      </c>
-      <c r="F66" t="s">
-        <v>76</v>
       </c>
       <c r="G66">
         <v>26</v>
       </c>
       <c r="H66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I66" s="3">
         <v>8.3000000000000007</v>
@@ -7582,7 +7582,7 @@
     </row>
     <row r="67" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C67" s="1">
         <v>39848</v>
@@ -7593,7 +7593,7 @@
         <v>28</v>
       </c>
       <c r="H67" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I67" s="3">
         <v>8.3000000000000007</v>
@@ -7671,7 +7671,7 @@
     </row>
     <row r="68" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C68" s="1">
         <v>39854</v>
@@ -7682,7 +7682,7 @@
         <v>34</v>
       </c>
       <c r="H68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I68" s="3">
         <v>8.3000000000000007</v>
@@ -7760,7 +7760,7 @@
     </row>
     <row r="69" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C69" s="1">
         <v>39860</v>
@@ -7771,7 +7771,7 @@
         <v>40</v>
       </c>
       <c r="H69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I69" s="3">
         <v>8.3000000000000007</v>
@@ -7849,7 +7849,7 @@
     </row>
     <row r="70" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C70" s="1">
         <v>39864</v>
@@ -7860,7 +7860,7 @@
         <v>44</v>
       </c>
       <c r="H70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I70" s="3">
         <v>8.3000000000000007</v>
@@ -7956,7 +7956,7 @@
     </row>
     <row r="71" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C71" s="1">
         <v>39869</v>
@@ -7967,7 +7967,7 @@
         <v>49</v>
       </c>
       <c r="H71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I71" s="3">
         <v>8.3000000000000007</v>
@@ -8045,7 +8045,7 @@
     </row>
     <row r="72" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C72" s="1">
         <v>39874</v>
@@ -8056,7 +8056,7 @@
         <v>54</v>
       </c>
       <c r="H72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I72" s="3">
         <v>8.3000000000000007</v>
@@ -8171,7 +8171,7 @@
     </row>
     <row r="73" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C73" s="1">
         <v>39877</v>
@@ -8180,16 +8180,16 @@
         <v>4</v>
       </c>
       <c r="E73" t="s">
+        <v>76</v>
+      </c>
+      <c r="F73" t="s">
         <v>77</v>
-      </c>
-      <c r="F73" t="s">
-        <v>78</v>
       </c>
       <c r="G73">
         <v>57</v>
       </c>
       <c r="H73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I73" s="3">
         <v>8.3000000000000007</v>
@@ -8267,7 +8267,7 @@
     </row>
     <row r="74" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C74" s="1">
         <v>39884</v>
@@ -8278,7 +8278,7 @@
         <v>64</v>
       </c>
       <c r="H74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I74" s="3">
         <v>8.3000000000000007</v>
@@ -8356,7 +8356,7 @@
     </row>
     <row r="75" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C75" s="1">
         <v>39890</v>
@@ -8367,7 +8367,7 @@
         <v>70</v>
       </c>
       <c r="H75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I75" s="3">
         <v>8.3000000000000007</v>
@@ -8483,7 +8483,7 @@
     </row>
     <row r="76" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C76" s="1">
         <v>39895</v>
@@ -8494,7 +8494,7 @@
         <v>75</v>
       </c>
       <c r="H76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I76" s="3">
         <v>8.3000000000000007</v>
@@ -8572,7 +8572,7 @@
     </row>
     <row r="77" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C77" s="1">
         <v>39903</v>
@@ -8581,16 +8581,16 @@
         <v>6</v>
       </c>
       <c r="E77" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F77" t="s">
         <v>79</v>
-      </c>
-      <c r="F77" t="s">
-        <v>80</v>
       </c>
       <c r="G77">
         <v>83</v>
       </c>
       <c r="H77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I77" s="3">
         <v>8.3000000000000007</v>
@@ -8706,7 +8706,7 @@
     </row>
     <row r="78" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C78" s="1">
         <v>39911</v>
@@ -8717,7 +8717,7 @@
         <v>91</v>
       </c>
       <c r="H78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I78" s="3">
         <v>8.3000000000000007</v>
@@ -8795,7 +8795,7 @@
     </row>
     <row r="79" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C79" s="1">
         <v>39919</v>
@@ -8806,7 +8806,7 @@
         <v>99</v>
       </c>
       <c r="H79" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I79" s="3">
         <v>8.3000000000000007</v>
@@ -8920,7 +8920,7 @@
     </row>
     <row r="80" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C80" s="1">
         <v>39928</v>
@@ -8931,7 +8931,7 @@
         <v>108</v>
       </c>
       <c r="H80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I80" s="3">
         <v>8.3000000000000007</v>
@@ -9009,7 +9009,7 @@
     </row>
     <row r="81" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C81" s="1">
         <v>39938</v>
@@ -9018,16 +9018,16 @@
         <v>8</v>
       </c>
       <c r="E81" t="s">
+        <v>80</v>
+      </c>
+      <c r="F81" t="s">
         <v>81</v>
-      </c>
-      <c r="F81" t="s">
-        <v>82</v>
       </c>
       <c r="G81">
         <v>118</v>
       </c>
       <c r="H81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I81" s="3">
         <v>8.3000000000000007</v>
@@ -9143,7 +9143,7 @@
     </row>
     <row r="82" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C82" s="1">
         <v>39954</v>
@@ -9154,7 +9154,7 @@
         <v>134</v>
       </c>
       <c r="H82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I82" s="3">
         <v>8.3000000000000007</v>
@@ -9234,7 +9234,7 @@
     </row>
     <row r="83" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C83" s="1">
         <v>39960</v>
@@ -9245,7 +9245,7 @@
         <v>140</v>
       </c>
       <c r="H83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I83" s="3">
         <v>8.3000000000000007</v>
@@ -9325,7 +9325,7 @@
     </row>
     <row r="84" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C84" s="1">
         <v>39966</v>
@@ -9336,7 +9336,7 @@
         <v>146</v>
       </c>
       <c r="H84" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I84" s="3">
         <v>8.3000000000000007</v>
@@ -9450,7 +9450,7 @@
     </row>
     <row r="85" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C85" s="1">
         <v>39969</v>
@@ -9461,7 +9461,7 @@
         <v>149</v>
       </c>
       <c r="H85" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I85" s="3">
         <v>8.3000000000000007</v>
@@ -9541,7 +9541,7 @@
     </row>
     <row r="86" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C86" s="1">
         <v>39974</v>
@@ -9550,16 +9550,16 @@
         <v>9</v>
       </c>
       <c r="E86" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F86" t="s">
         <v>83</v>
-      </c>
-      <c r="F86" t="s">
-        <v>84</v>
       </c>
       <c r="G86">
         <v>154</v>
       </c>
       <c r="H86" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I86" s="3">
         <v>8.3000000000000007</v>
@@ -9637,7 +9637,7 @@
     </row>
     <row r="87" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C87" s="1">
         <v>39976</v>
@@ -9648,7 +9648,7 @@
         <v>156</v>
       </c>
       <c r="H87" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I87" s="3">
         <v>8.3000000000000007</v>
@@ -9728,7 +9728,7 @@
     </row>
     <row r="88" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C88" s="1">
         <v>39983</v>
@@ -9739,7 +9739,7 @@
         <v>163</v>
       </c>
       <c r="H88" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I88" s="3">
         <v>8.3000000000000007</v>
@@ -9819,7 +9819,7 @@
     </row>
     <row r="89" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C89" s="1">
         <v>39990</v>
@@ -9830,7 +9830,7 @@
         <v>170</v>
       </c>
       <c r="H89" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I89" s="3">
         <v>8.3000000000000007</v>
@@ -9910,7 +9910,7 @@
     </row>
     <row r="90" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C90" s="1">
         <v>39994</v>
@@ -9919,16 +9919,16 @@
         <v>10</v>
       </c>
       <c r="E90" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F90" t="s">
         <v>85</v>
-      </c>
-      <c r="F90" t="s">
-        <v>86</v>
       </c>
       <c r="G90">
         <v>174</v>
       </c>
       <c r="H90" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I90" s="3">
         <v>8.3000000000000007</v>
@@ -10012,7 +10012,7 @@
     </row>
     <row r="91" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C91" s="1">
         <v>39995</v>
@@ -10023,7 +10023,7 @@
         <v>175</v>
       </c>
       <c r="H91" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I91" s="3">
         <v>8.3000000000000007</v>
@@ -10103,7 +10103,7 @@
     </row>
     <row r="92" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C92" s="1">
         <v>40895</v>
@@ -10112,16 +10112,16 @@
         <v>1</v>
       </c>
       <c r="E92" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F92" t="s">
         <v>72</v>
       </c>
-      <c r="F92" t="s">
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92" t="s">
         <v>73</v>
-      </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92" t="s">
-        <v>74</v>
       </c>
       <c r="I92" s="3">
         <v>8</v>
@@ -10215,7 +10215,7 @@
     </row>
     <row r="93" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C93" s="1">
         <v>40924</v>
@@ -10224,16 +10224,16 @@
         <v>4</v>
       </c>
       <c r="E93" t="s">
+        <v>74</v>
+      </c>
+      <c r="F93" t="s">
         <v>75</v>
-      </c>
-      <c r="F93" t="s">
-        <v>76</v>
       </c>
       <c r="G93">
         <v>29</v>
       </c>
       <c r="H93" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I93" s="3">
         <v>8</v>
@@ -10329,7 +10329,7 @@
     </row>
     <row r="94" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C94" s="1">
         <v>40931</v>
@@ -10340,7 +10340,7 @@
         <v>36</v>
       </c>
       <c r="H94" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I94" s="3">
         <v>8</v>
@@ -10418,7 +10418,7 @@
     </row>
     <row r="95" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C95" s="1">
         <v>40938</v>
@@ -10429,7 +10429,7 @@
         <v>43</v>
       </c>
       <c r="H95" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I95" s="3">
         <v>8</v>
@@ -10543,7 +10543,7 @@
     </row>
     <row r="96" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C96" s="1">
         <v>40939</v>
@@ -10554,7 +10554,7 @@
         <v>44</v>
       </c>
       <c r="H96" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I96" s="3">
         <v>8</v>
@@ -10632,7 +10632,7 @@
     </row>
     <row r="97" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C97" s="1">
         <v>40945</v>
@@ -10641,16 +10641,16 @@
         <v>5</v>
       </c>
       <c r="E97" t="s">
+        <v>76</v>
+      </c>
+      <c r="F97" t="s">
         <v>77</v>
-      </c>
-      <c r="F97" t="s">
-        <v>78</v>
       </c>
       <c r="G97">
         <v>50</v>
       </c>
       <c r="H97" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I97" s="3">
         <v>8</v>
@@ -10766,7 +10766,7 @@
     </row>
     <row r="98" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C98" s="1">
         <v>40948</v>
@@ -10777,7 +10777,7 @@
         <v>53</v>
       </c>
       <c r="H98" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I98" s="3">
         <v>8</v>
@@ -10855,7 +10855,7 @@
     </row>
     <row r="99" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C99" s="1">
         <v>40954</v>
@@ -10866,7 +10866,7 @@
         <v>59</v>
       </c>
       <c r="H99" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I99" s="3">
         <v>8</v>
@@ -10944,7 +10944,7 @@
     </row>
     <row r="100" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C100" s="1">
         <v>40959</v>
@@ -10955,7 +10955,7 @@
         <v>64</v>
       </c>
       <c r="H100" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I100" s="3">
         <v>8</v>
@@ -11069,7 +11069,7 @@
     </row>
     <row r="101" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C101" s="1">
         <v>40960</v>
@@ -11080,7 +11080,7 @@
         <v>65</v>
       </c>
       <c r="H101" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I101" s="3">
         <v>8</v>
@@ -11158,7 +11158,7 @@
     </row>
     <row r="102" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C102" s="1">
         <v>40970</v>
@@ -11169,7 +11169,7 @@
         <v>75</v>
       </c>
       <c r="H102" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I102" s="3">
         <v>8</v>
@@ -11247,7 +11247,7 @@
     </row>
     <row r="103" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C103" s="1">
         <v>40976</v>
@@ -11258,7 +11258,7 @@
         <v>81</v>
       </c>
       <c r="H103" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I103" s="3">
         <v>8</v>
@@ -11336,7 +11336,7 @@
     </row>
     <row r="104" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C104" s="1">
         <v>40980</v>
@@ -11345,16 +11345,16 @@
         <v>6</v>
       </c>
       <c r="E104" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F104" t="s">
         <v>79</v>
-      </c>
-      <c r="F104" t="s">
-        <v>80</v>
       </c>
       <c r="G104">
         <v>85</v>
       </c>
       <c r="H104" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I104" s="3">
         <v>8</v>
@@ -11468,7 +11468,7 @@
     </row>
     <row r="105" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C105" s="1">
         <v>40982</v>
@@ -11479,7 +11479,7 @@
         <v>87</v>
       </c>
       <c r="H105" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I105" s="3">
         <v>8</v>
@@ -11557,7 +11557,7 @@
     </row>
     <row r="106" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C106" s="1">
         <v>40997</v>
@@ -11566,16 +11566,16 @@
         <v>8</v>
       </c>
       <c r="E106" t="s">
+        <v>80</v>
+      </c>
+      <c r="F106" t="s">
         <v>81</v>
-      </c>
-      <c r="F106" t="s">
-        <v>82</v>
       </c>
       <c r="G106">
         <v>102</v>
       </c>
       <c r="H106" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I106" s="3">
         <v>8</v>
@@ -11691,7 +11691,7 @@
     </row>
     <row r="107" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C107" s="1">
         <v>41001</v>
@@ -11702,7 +11702,7 @@
         <v>106</v>
       </c>
       <c r="H107" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I107" s="3">
         <v>8</v>
@@ -11780,7 +11780,7 @@
     </row>
     <row r="108" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C108" s="1">
         <v>41009</v>
@@ -11791,7 +11791,7 @@
         <v>114</v>
       </c>
       <c r="H108" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I108" s="3">
         <v>8</v>
@@ -11871,7 +11871,7 @@
     </row>
     <row r="109" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C109" s="1">
         <v>41018</v>
@@ -11882,7 +11882,7 @@
         <v>123</v>
       </c>
       <c r="H109" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I109" s="3">
         <v>8</v>
@@ -11962,7 +11962,7 @@
     </row>
     <row r="110" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C110" s="1">
         <v>41025</v>
@@ -11971,16 +11971,16 @@
         <v>9</v>
       </c>
       <c r="E110" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F110" t="s">
         <v>83</v>
-      </c>
-      <c r="F110" t="s">
-        <v>84</v>
       </c>
       <c r="G110">
         <v>130</v>
       </c>
       <c r="H110" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I110" s="3">
         <v>8</v>
@@ -12062,7 +12062,7 @@
     </row>
     <row r="111" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C111" s="1">
         <v>41032</v>
@@ -12073,7 +12073,7 @@
         <v>137</v>
       </c>
       <c r="H111" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I111" s="3">
         <v>8</v>
@@ -12153,7 +12153,7 @@
     </row>
     <row r="112" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C112" s="1">
         <v>41038</v>
@@ -12164,7 +12164,7 @@
         <v>143</v>
       </c>
       <c r="H112" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I112" s="3">
         <v>8</v>
@@ -12278,7 +12278,7 @@
     </row>
     <row r="113" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C113" s="1">
         <v>41039</v>
@@ -12289,7 +12289,7 @@
         <v>144</v>
       </c>
       <c r="H113" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I113" s="3">
         <v>8</v>
@@ -12369,7 +12369,7 @@
     </row>
     <row r="114" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C114" s="1">
         <v>41043</v>
@@ -12380,7 +12380,7 @@
         <v>148</v>
       </c>
       <c r="H114" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I114" s="3">
         <v>8</v>
@@ -12460,7 +12460,7 @@
     </row>
     <row r="115" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C115" s="1">
         <v>41050</v>
@@ -12471,7 +12471,7 @@
         <v>155</v>
       </c>
       <c r="H115" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I115" s="3">
         <v>8</v>
@@ -12551,7 +12551,7 @@
     </row>
     <row r="116" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C116" s="1">
         <v>41057</v>
@@ -12562,7 +12562,7 @@
         <v>162</v>
       </c>
       <c r="H116" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I116" s="3">
         <v>8</v>
@@ -12642,7 +12642,7 @@
     </row>
     <row r="117" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C117" s="1">
         <v>41065</v>
@@ -12651,16 +12651,16 @@
         <v>10</v>
       </c>
       <c r="E117" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F117" t="s">
         <v>85</v>
-      </c>
-      <c r="F117" t="s">
-        <v>86</v>
       </c>
       <c r="G117">
         <v>170</v>
       </c>
       <c r="H117" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I117" s="3">
         <v>8</v>
@@ -12744,7 +12744,7 @@
     </row>
     <row r="118" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C118" s="1">
         <v>40912</v>
@@ -12753,16 +12753,16 @@
         <v>1</v>
       </c>
       <c r="E118" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F118" t="s">
         <v>72</v>
       </c>
-      <c r="F118" t="s">
+      <c r="G118">
+        <v>0</v>
+      </c>
+      <c r="H118" t="s">
         <v>73</v>
-      </c>
-      <c r="G118">
-        <v>0</v>
-      </c>
-      <c r="H118" t="s">
-        <v>74</v>
       </c>
       <c r="I118" s="3">
         <v>8</v>
@@ -12856,7 +12856,7 @@
     </row>
     <row r="119" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C119" s="1">
         <v>40945</v>
@@ -12867,7 +12867,7 @@
         <v>33</v>
       </c>
       <c r="H119" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I119" s="3">
         <v>8</v>
@@ -12981,7 +12981,7 @@
     </row>
     <row r="120" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C120" s="1">
         <v>40947</v>
@@ -12990,16 +12990,16 @@
         <v>4</v>
       </c>
       <c r="E120" t="s">
+        <v>74</v>
+      </c>
+      <c r="F120" t="s">
         <v>75</v>
-      </c>
-      <c r="F120" t="s">
-        <v>76</v>
       </c>
       <c r="G120">
         <v>35</v>
       </c>
       <c r="H120" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I120" s="3">
         <v>8</v>
@@ -13077,7 +13077,7 @@
     </row>
     <row r="121" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C121" s="1">
         <v>40956</v>
@@ -13088,7 +13088,7 @@
         <v>44</v>
       </c>
       <c r="H121" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I121" s="3">
         <v>8</v>
@@ -13202,7 +13202,7 @@
     </row>
     <row r="122" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C122" s="1">
         <v>40960</v>
@@ -13213,7 +13213,7 @@
         <v>48</v>
       </c>
       <c r="H122" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I122" s="3">
         <v>8</v>
@@ -13291,7 +13291,7 @@
     </row>
     <row r="123" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C123" s="1">
         <v>40963</v>
@@ -13300,16 +13300,16 @@
         <v>5</v>
       </c>
       <c r="E123" t="s">
+        <v>76</v>
+      </c>
+      <c r="F123" t="s">
         <v>77</v>
-      </c>
-      <c r="F123" t="s">
-        <v>78</v>
       </c>
       <c r="G123">
         <v>51</v>
       </c>
       <c r="H123" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I123" s="3">
         <v>8</v>
@@ -13425,7 +13425,7 @@
     </row>
     <row r="124" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C124" s="1">
         <v>40970</v>
@@ -13436,7 +13436,7 @@
         <v>58</v>
       </c>
       <c r="H124" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I124" s="3">
         <v>8</v>
@@ -13514,7 +13514,7 @@
     </row>
     <row r="125" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C125" s="1">
         <v>40976</v>
@@ -13525,7 +13525,7 @@
         <v>64</v>
       </c>
       <c r="H125" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I125" s="3">
         <v>8</v>
@@ -13603,7 +13603,7 @@
     </row>
     <row r="126" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C126" s="1">
         <v>40980</v>
@@ -13612,16 +13612,16 @@
         <v>6</v>
       </c>
       <c r="E126" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F126" t="s">
         <v>79</v>
-      </c>
-      <c r="F126" t="s">
-        <v>80</v>
       </c>
       <c r="G126">
         <v>68</v>
       </c>
       <c r="H126" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I126" s="3">
         <v>8</v>
@@ -13735,7 +13735,7 @@
     </row>
     <row r="127" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C127" s="1">
         <v>40982</v>
@@ -13746,7 +13746,7 @@
         <v>70</v>
       </c>
       <c r="H127" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I127" s="3">
         <v>8</v>
@@ -13824,7 +13824,7 @@
     </row>
     <row r="128" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C128" s="1">
         <v>40994</v>
@@ -13835,7 +13835,7 @@
         <v>82</v>
       </c>
       <c r="H128" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I128" s="3">
         <v>8</v>
@@ -13913,7 +13913,7 @@
     </row>
     <row r="129" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C129" s="1">
         <v>40998</v>
@@ -13922,16 +13922,16 @@
         <v>8</v>
       </c>
       <c r="E129" t="s">
+        <v>80</v>
+      </c>
+      <c r="F129" t="s">
         <v>81</v>
-      </c>
-      <c r="F129" t="s">
-        <v>82</v>
       </c>
       <c r="G129">
         <v>86</v>
       </c>
       <c r="H129" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I129" s="3">
         <v>8</v>
@@ -14009,7 +14009,7 @@
     </row>
     <row r="130" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C130" s="1">
         <v>41001</v>
@@ -14020,7 +14020,7 @@
         <v>89</v>
       </c>
       <c r="H130" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I130" s="3">
         <v>8</v>
@@ -14098,7 +14098,7 @@
     </row>
     <row r="131" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C131" s="1">
         <v>41011</v>
@@ -14109,7 +14109,7 @@
         <v>99</v>
       </c>
       <c r="H131" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I131" s="3">
         <v>8</v>
@@ -14223,7 +14223,7 @@
     </row>
     <row r="132" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C132" s="1">
         <v>41016</v>
@@ -14234,7 +14234,7 @@
         <v>104</v>
       </c>
       <c r="H132" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I132" s="3">
         <v>8</v>
@@ -14312,7 +14312,7 @@
     </row>
     <row r="133" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C133" s="1">
         <v>41029</v>
@@ -14323,7 +14323,7 @@
         <v>117</v>
       </c>
       <c r="H133" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I133" s="3">
         <v>8</v>
@@ -14437,7 +14437,7 @@
     </row>
     <row r="134" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C134" s="1">
         <v>41043</v>
@@ -14448,7 +14448,7 @@
         <v>131</v>
       </c>
       <c r="H134" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I134" s="3">
         <v>8</v>
@@ -14528,7 +14528,7 @@
     </row>
     <row r="135" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C135" s="1">
         <v>41050</v>
@@ -14539,7 +14539,7 @@
         <v>138</v>
       </c>
       <c r="H135" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I135" s="3">
         <v>8</v>
@@ -14619,7 +14619,7 @@
     </row>
     <row r="136" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C136" s="1">
         <v>41057</v>
@@ -14630,7 +14630,7 @@
         <v>145</v>
       </c>
       <c r="H136" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I136" s="3">
         <v>8</v>
@@ -14710,7 +14710,7 @@
     </row>
     <row r="137" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C137" s="1">
         <v>41064</v>
@@ -14721,7 +14721,7 @@
         <v>152</v>
       </c>
       <c r="H137" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I137" s="3">
         <v>8</v>
@@ -14801,7 +14801,7 @@
     </row>
     <row r="138" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C138" s="1">
         <v>41066</v>
@@ -14812,7 +14812,7 @@
         <v>154</v>
       </c>
       <c r="H138" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I138" s="3">
         <v>8</v>
@@ -14926,7 +14926,7 @@
     </row>
     <row r="139" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C139" s="1">
         <v>41071</v>
@@ -14935,16 +14935,16 @@
         <v>9</v>
       </c>
       <c r="E139" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F139" t="s">
         <v>83</v>
-      </c>
-      <c r="F139" t="s">
-        <v>84</v>
       </c>
       <c r="G139">
         <v>159</v>
       </c>
       <c r="H139" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I139" s="3">
         <v>8</v>
@@ -15022,7 +15022,7 @@
     </row>
     <row r="140" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C140" s="1">
         <v>41072</v>
@@ -15033,7 +15033,7 @@
         <v>160</v>
       </c>
       <c r="H140" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I140" s="3">
         <v>8</v>
@@ -15113,7 +15113,7 @@
     </row>
     <row r="141" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C141" s="1">
         <v>41092</v>
@@ -15124,7 +15124,7 @@
         <v>180</v>
       </c>
       <c r="H141" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I141" s="3">
         <v>8</v>
@@ -15204,7 +15204,7 @@
     </row>
     <row r="142" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C142" s="1">
         <v>41096</v>
@@ -15213,16 +15213,16 @@
         <v>10</v>
       </c>
       <c r="E142" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F142" t="s">
         <v>85</v>
-      </c>
-      <c r="F142" t="s">
-        <v>86</v>
       </c>
       <c r="G142">
         <v>184</v>
       </c>
       <c r="H142" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I142" s="3">
         <v>8</v>

</xml_diff>

<commit_message>
Getting SLA Data reading for modelling
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63D498A-31E0-4F91-9CB9-154D15377937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FEFF5B-E4A5-4B7F-AAA9-B69F81F2F839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{FBA18FA7-8D49-4A23-B648-57CB41343816}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FBA18FA7-8D49-4A23-B648-57CB41343816}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -314,10 +314,10 @@
     <t>BDK12P2</t>
   </si>
   <si>
-    <t>Cotton.Leaf.SpecificArea</t>
+    <t>Cotton.Boll.Wt</t>
   </si>
   <si>
-    <t>Cotton.Boll.Wt</t>
+    <t>Cotton.Leaf.SpecificAreaCanopy</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AS2" sqref="AS2"/>
+      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -928,7 +928,7 @@
         <v>33</v>
       </c>
       <c r="AI1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AJ1" t="s">
         <v>34</v>
@@ -958,7 +958,7 @@
         <v>42</v>
       </c>
       <c r="AS1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AT1" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Updated Phenology DAS in observed files
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FEFF5B-E4A5-4B7F-AAA9-B69F81F2F839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CCE800-6E5E-48B8-8C69-D9E505AD1AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FBA18FA7-8D49-4A23-B648-57CB41343816}"/>
+    <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="17640" xr2:uid="{FBA18FA7-8D49-4A23-B648-57CB41343816}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -682,149 +682,149 @@
   <dimension ref="A1:BU142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="P110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
+      <selection pane="bottomRight" activeCell="V118" sqref="V118:V142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="34" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="33" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="30" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="31.59765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.86328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="17" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="24" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.3984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="25.73046875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="26.73046875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="6.73046875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="4.265625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="31.3984375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="32" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="9" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="10" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="6.265625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="12" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="12" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="76" max="77" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="77" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="22" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="12" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="22" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="12" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="22" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="86" max="86" width="12" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="22" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="12" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="22" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="12" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="22" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="22" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="12" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="22" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="12" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="22" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="12" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="23" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="13" bestFit="1" customWidth="1"/>
     <col min="108" max="108" width="23" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="13" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="23" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="113" max="113" width="13" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="131" max="131" width="7" bestFit="1" customWidth="1"/>
     <col min="132" max="139" width="18" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="5.86328125" bestFit="1" customWidth="1"/>
-    <col min="141" max="148" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="141" max="148" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -1082,11 +1082,19 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
+      <c r="R2" s="2">
+        <v>21</v>
+      </c>
+      <c r="S2" s="2">
+        <v>42</v>
+      </c>
       <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
+      <c r="U2" s="2">
+        <v>94</v>
+      </c>
+      <c r="V2" s="2">
+        <v>164</v>
+      </c>
       <c r="W2" s="2"/>
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
@@ -1157,7 +1165,7 @@
       <c r="BT2" s="2"/>
       <c r="BU2" s="2"/>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -1189,11 +1197,19 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
+      <c r="R3" s="2">
+        <v>21</v>
+      </c>
+      <c r="S3" s="2">
+        <v>42</v>
+      </c>
       <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
+      <c r="U3" s="2">
+        <v>94</v>
+      </c>
+      <c r="V3" s="2">
+        <v>164</v>
+      </c>
       <c r="W3" s="2"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
@@ -1246,7 +1262,7 @@
       <c r="BT3" s="2"/>
       <c r="BU3" s="2"/>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1286,10 +1302,16 @@
       <c r="R4" s="2">
         <v>21</v>
       </c>
-      <c r="S4" s="2"/>
+      <c r="S4" s="2">
+        <v>42</v>
+      </c>
       <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
+      <c r="U4" s="2">
+        <v>94</v>
+      </c>
+      <c r="V4" s="2">
+        <v>164</v>
+      </c>
       <c r="W4" s="2"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
@@ -1342,7 +1364,7 @@
       <c r="BT4" s="2"/>
       <c r="BU4" s="2"/>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1374,11 +1396,19 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
+      <c r="R5" s="2">
+        <v>21</v>
+      </c>
+      <c r="S5" s="2">
+        <v>42</v>
+      </c>
       <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
+      <c r="U5" s="2">
+        <v>94</v>
+      </c>
+      <c r="V5" s="2">
+        <v>164</v>
+      </c>
       <c r="W5" s="2"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
@@ -1431,7 +1461,7 @@
       <c r="BT5" s="2"/>
       <c r="BU5" s="2"/>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -1463,11 +1493,19 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+      <c r="R6" s="2">
+        <v>21</v>
+      </c>
+      <c r="S6" s="2">
+        <v>42</v>
+      </c>
       <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
+      <c r="U6" s="2">
+        <v>94</v>
+      </c>
+      <c r="V6" s="2">
+        <v>164</v>
+      </c>
       <c r="W6" s="2"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
@@ -1520,7 +1558,7 @@
       <c r="BT6" s="2"/>
       <c r="BU6" s="2"/>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -1550,11 +1588,19 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="R7" s="2">
+        <v>21</v>
+      </c>
+      <c r="S7" s="2">
+        <v>42</v>
+      </c>
       <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
+      <c r="U7" s="2">
+        <v>94</v>
+      </c>
+      <c r="V7" s="2">
+        <v>164</v>
+      </c>
       <c r="W7" s="2"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
@@ -1641,7 +1687,7 @@
       <c r="BT7" s="2"/>
       <c r="BU7" s="2"/>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -1673,11 +1719,19 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
+      <c r="R8" s="2">
+        <v>21</v>
+      </c>
+      <c r="S8" s="2">
+        <v>42</v>
+      </c>
       <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
+      <c r="U8" s="2">
+        <v>94</v>
+      </c>
+      <c r="V8" s="2">
+        <v>164</v>
+      </c>
       <c r="W8" s="2"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
@@ -1730,7 +1784,7 @@
       <c r="BT8" s="2"/>
       <c r="BU8" s="2"/>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -1767,13 +1821,19 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
+      <c r="R9" s="2">
+        <v>21</v>
+      </c>
       <c r="S9" s="2">
         <v>42</v>
       </c>
       <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
+      <c r="U9" s="2">
+        <v>94</v>
+      </c>
+      <c r="V9" s="2">
+        <v>164</v>
+      </c>
       <c r="W9" s="2"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
@@ -1864,7 +1924,7 @@
       <c r="BT9" s="2"/>
       <c r="BU9" s="2"/>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -1896,11 +1956,19 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
+      <c r="R10" s="2">
+        <v>21</v>
+      </c>
+      <c r="S10" s="2">
+        <v>42</v>
+      </c>
       <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
+      <c r="U10" s="2">
+        <v>94</v>
+      </c>
+      <c r="V10" s="2">
+        <v>164</v>
+      </c>
       <c r="W10" s="2"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
@@ -1953,7 +2021,7 @@
       <c r="BT10" s="2"/>
       <c r="BU10" s="2"/>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -1985,11 +2053,19 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
+      <c r="R11" s="2">
+        <v>21</v>
+      </c>
+      <c r="S11" s="2">
+        <v>42</v>
+      </c>
       <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
+      <c r="U11" s="2">
+        <v>94</v>
+      </c>
+      <c r="V11" s="2">
+        <v>164</v>
+      </c>
       <c r="W11" s="2"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
@@ -2042,7 +2118,7 @@
       <c r="BT11" s="2"/>
       <c r="BU11" s="2"/>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -2074,11 +2150,19 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
+      <c r="R12" s="2">
+        <v>21</v>
+      </c>
+      <c r="S12" s="2">
+        <v>42</v>
+      </c>
       <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
+      <c r="U12" s="2">
+        <v>94</v>
+      </c>
+      <c r="V12" s="2">
+        <v>164</v>
+      </c>
       <c r="W12" s="2"/>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
@@ -2131,7 +2215,7 @@
       <c r="BT12" s="2"/>
       <c r="BU12" s="2"/>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -2161,11 +2245,19 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
+      <c r="R13" s="2">
+        <v>21</v>
+      </c>
+      <c r="S13" s="2">
+        <v>42</v>
+      </c>
       <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
+      <c r="U13" s="2">
+        <v>94</v>
+      </c>
+      <c r="V13" s="2">
+        <v>164</v>
+      </c>
       <c r="W13" s="2"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
@@ -2256,7 +2348,7 @@
       <c r="BT13" s="2"/>
       <c r="BU13" s="2"/>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>86</v>
       </c>
@@ -2288,11 +2380,19 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
+      <c r="R14" s="2">
+        <v>21</v>
+      </c>
+      <c r="S14" s="2">
+        <v>42</v>
+      </c>
       <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
+      <c r="U14" s="2">
+        <v>94</v>
+      </c>
+      <c r="V14" s="2">
+        <v>164</v>
+      </c>
       <c r="W14" s="2"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
@@ -2345,7 +2445,7 @@
       <c r="BT14" s="2"/>
       <c r="BU14" s="2"/>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -2382,11 +2482,19 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
+      <c r="R15" s="2">
+        <v>21</v>
+      </c>
+      <c r="S15" s="2">
+        <v>42</v>
+      </c>
       <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
+      <c r="U15" s="2">
+        <v>94</v>
+      </c>
+      <c r="V15" s="2">
+        <v>164</v>
+      </c>
       <c r="W15" s="2"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
@@ -2477,7 +2585,7 @@
       <c r="BT15" s="2"/>
       <c r="BU15" s="2"/>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -2509,11 +2617,19 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
+      <c r="R16" s="2">
+        <v>21</v>
+      </c>
+      <c r="S16" s="2">
+        <v>42</v>
+      </c>
       <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
+      <c r="U16" s="2">
+        <v>94</v>
+      </c>
+      <c r="V16" s="2">
+        <v>164</v>
+      </c>
       <c r="W16" s="2"/>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
@@ -2566,7 +2682,7 @@
       <c r="BT16" s="2"/>
       <c r="BU16" s="2"/>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -2598,11 +2714,19 @@
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
+      <c r="R17" s="2">
+        <v>21</v>
+      </c>
+      <c r="S17" s="2">
+        <v>42</v>
+      </c>
       <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
+      <c r="U17" s="2">
+        <v>94</v>
+      </c>
+      <c r="V17" s="2">
+        <v>164</v>
+      </c>
       <c r="W17" s="2"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
@@ -2655,7 +2779,7 @@
       <c r="BT17" s="2"/>
       <c r="BU17" s="2"/>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>86</v>
       </c>
@@ -2687,11 +2811,19 @@
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
+      <c r="R18" s="2">
+        <v>21</v>
+      </c>
+      <c r="S18" s="2">
+        <v>42</v>
+      </c>
       <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
+      <c r="U18" s="2">
+        <v>94</v>
+      </c>
+      <c r="V18" s="2">
+        <v>164</v>
+      </c>
       <c r="W18" s="2"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
@@ -2744,7 +2876,7 @@
       <c r="BT18" s="2"/>
       <c r="BU18" s="2"/>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -2774,11 +2906,19 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
+      <c r="R19" s="2">
+        <v>21</v>
+      </c>
+      <c r="S19" s="2">
+        <v>42</v>
+      </c>
       <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
+      <c r="U19" s="2">
+        <v>94</v>
+      </c>
+      <c r="V19" s="2">
+        <v>164</v>
+      </c>
       <c r="W19" s="2"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
@@ -2869,7 +3009,7 @@
       <c r="BT19" s="2"/>
       <c r="BU19" s="2"/>
     </row>
-    <row r="20" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -2906,13 +3046,19 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
+      <c r="R20" s="2">
+        <v>21</v>
+      </c>
+      <c r="S20" s="2">
+        <v>42</v>
+      </c>
       <c r="T20" s="2"/>
       <c r="U20" s="2">
         <v>94</v>
       </c>
-      <c r="V20" s="2"/>
+      <c r="V20" s="2">
+        <v>164</v>
+      </c>
       <c r="W20" s="2"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
@@ -2965,7 +3111,7 @@
       <c r="BT20" s="2"/>
       <c r="BU20" s="2"/>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -2997,11 +3143,19 @@
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
+      <c r="R21" s="2">
+        <v>21</v>
+      </c>
+      <c r="S21" s="2">
+        <v>42</v>
+      </c>
       <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
+      <c r="U21" s="2">
+        <v>94</v>
+      </c>
+      <c r="V21" s="2">
+        <v>164</v>
+      </c>
       <c r="W21" s="2"/>
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
@@ -3054,7 +3208,7 @@
       <c r="BT21" s="2"/>
       <c r="BU21" s="2"/>
     </row>
-    <row r="22" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -3084,11 +3238,19 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
+      <c r="R22" s="2">
+        <v>21</v>
+      </c>
+      <c r="S22" s="2">
+        <v>42</v>
+      </c>
       <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
+      <c r="U22" s="2">
+        <v>94</v>
+      </c>
+      <c r="V22" s="2">
+        <v>164</v>
+      </c>
       <c r="W22" s="2"/>
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
@@ -3179,7 +3341,7 @@
       <c r="BT22" s="2"/>
       <c r="BU22" s="2"/>
     </row>
-    <row r="23" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -3211,11 +3373,19 @@
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
+      <c r="R23" s="2">
+        <v>21</v>
+      </c>
+      <c r="S23" s="2">
+        <v>42</v>
+      </c>
       <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
+      <c r="U23" s="2">
+        <v>94</v>
+      </c>
+      <c r="V23" s="2">
+        <v>164</v>
+      </c>
       <c r="W23" s="2"/>
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
@@ -3268,7 +3438,7 @@
       <c r="BT23" s="2"/>
       <c r="BU23" s="2"/>
     </row>
-    <row r="24" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -3298,11 +3468,19 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
+      <c r="R24" s="2">
+        <v>21</v>
+      </c>
+      <c r="S24" s="2">
+        <v>42</v>
+      </c>
       <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
+      <c r="U24" s="2">
+        <v>94</v>
+      </c>
+      <c r="V24" s="2">
+        <v>164</v>
+      </c>
       <c r="W24" s="2"/>
       <c r="X24" s="4"/>
       <c r="Y24" s="4"/>
@@ -3359,7 +3537,7 @@
       <c r="BT24" s="2"/>
       <c r="BU24" s="2"/>
     </row>
-    <row r="25" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -3389,11 +3567,19 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
+      <c r="R25" s="2">
+        <v>21</v>
+      </c>
+      <c r="S25" s="2">
+        <v>42</v>
+      </c>
       <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
+      <c r="U25" s="2">
+        <v>94</v>
+      </c>
+      <c r="V25" s="2">
+        <v>164</v>
+      </c>
       <c r="W25" s="2"/>
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
@@ -3484,7 +3670,7 @@
       <c r="BT25" s="2"/>
       <c r="BU25" s="2"/>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -3514,11 +3700,19 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
+      <c r="R26" s="2">
+        <v>21</v>
+      </c>
+      <c r="S26" s="2">
+        <v>42</v>
+      </c>
       <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
+      <c r="U26" s="2">
+        <v>94</v>
+      </c>
+      <c r="V26" s="2">
+        <v>164</v>
+      </c>
       <c r="W26" s="2"/>
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
@@ -3575,7 +3769,7 @@
       <c r="BT26" s="2"/>
       <c r="BU26" s="2"/>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -3605,11 +3799,19 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
+      <c r="R27" s="2">
+        <v>21</v>
+      </c>
+      <c r="S27" s="2">
+        <v>42</v>
+      </c>
       <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
+      <c r="U27" s="2">
+        <v>94</v>
+      </c>
+      <c r="V27" s="2">
+        <v>164</v>
+      </c>
       <c r="W27" s="2"/>
       <c r="X27" s="4"/>
       <c r="Y27" s="4"/>
@@ -3666,7 +3868,7 @@
       <c r="BT27" s="2"/>
       <c r="BU27" s="2"/>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -3696,11 +3898,19 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
+      <c r="R28" s="2">
+        <v>21</v>
+      </c>
+      <c r="S28" s="2">
+        <v>42</v>
+      </c>
       <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
+      <c r="U28" s="2">
+        <v>94</v>
+      </c>
+      <c r="V28" s="2">
+        <v>164</v>
+      </c>
       <c r="W28" s="2"/>
       <c r="X28" s="4"/>
       <c r="Y28" s="4"/>
@@ -3757,7 +3967,7 @@
       <c r="BT28" s="2"/>
       <c r="BU28" s="2"/>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -3787,11 +3997,19 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
+      <c r="R29" s="2">
+        <v>21</v>
+      </c>
+      <c r="S29" s="2">
+        <v>42</v>
+      </c>
       <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
+      <c r="U29" s="2">
+        <v>94</v>
+      </c>
+      <c r="V29" s="2">
+        <v>164</v>
+      </c>
       <c r="W29" s="2"/>
       <c r="X29" s="4"/>
       <c r="Y29" s="4"/>
@@ -3848,7 +4066,7 @@
       <c r="BT29" s="2"/>
       <c r="BU29" s="2"/>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>86</v>
       </c>
@@ -3878,11 +4096,19 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
+      <c r="R30" s="2">
+        <v>21</v>
+      </c>
+      <c r="S30" s="2">
+        <v>42</v>
+      </c>
       <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
+      <c r="U30" s="2">
+        <v>94</v>
+      </c>
+      <c r="V30" s="2">
+        <v>164</v>
+      </c>
       <c r="W30" s="2"/>
       <c r="X30" s="4"/>
       <c r="Y30" s="4"/>
@@ -3939,7 +4165,7 @@
       <c r="BT30" s="2"/>
       <c r="BU30" s="2"/>
     </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -3969,11 +4195,19 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
+      <c r="R31" s="2">
+        <v>21</v>
+      </c>
+      <c r="S31" s="2">
+        <v>42</v>
+      </c>
       <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
+      <c r="U31" s="2">
+        <v>94</v>
+      </c>
+      <c r="V31" s="2">
+        <v>164</v>
+      </c>
       <c r="W31" s="2"/>
       <c r="X31" s="4"/>
       <c r="Y31" s="4"/>
@@ -4030,7 +4264,7 @@
       <c r="BT31" s="2"/>
       <c r="BU31" s="2"/>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -4067,10 +4301,16 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
+      <c r="R32" s="2">
+        <v>21</v>
+      </c>
+      <c r="S32" s="2">
+        <v>42</v>
+      </c>
       <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
+      <c r="U32" s="2">
+        <v>94</v>
+      </c>
       <c r="V32" s="2">
         <v>164</v>
       </c>
@@ -4126,7 +4366,7 @@
       <c r="BT32" s="2"/>
       <c r="BU32" s="2"/>
     </row>
-    <row r="33" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -4156,11 +4396,19 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
+      <c r="R33" s="2">
+        <v>21</v>
+      </c>
+      <c r="S33" s="2">
+        <v>42</v>
+      </c>
       <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
+      <c r="U33" s="2">
+        <v>94</v>
+      </c>
+      <c r="V33" s="2">
+        <v>164</v>
+      </c>
       <c r="W33" s="2"/>
       <c r="X33" s="4"/>
       <c r="Y33" s="4"/>
@@ -4217,7 +4465,7 @@
       <c r="BT33" s="2"/>
       <c r="BU33" s="2"/>
     </row>
-    <row r="34" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -4254,11 +4502,19 @@
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
+      <c r="R34" s="2">
+        <v>21</v>
+      </c>
+      <c r="S34" s="2">
+        <v>42</v>
+      </c>
       <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
+      <c r="U34" s="2">
+        <v>94</v>
+      </c>
+      <c r="V34" s="2">
+        <v>164</v>
+      </c>
       <c r="W34" s="2"/>
       <c r="X34" s="4"/>
       <c r="Y34" s="4"/>
@@ -4319,7 +4575,7 @@
       <c r="BT34" s="2"/>
       <c r="BU34" s="2"/>
     </row>
-    <row r="35" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -4349,11 +4605,19 @@
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
+      <c r="R35" s="2">
+        <v>21</v>
+      </c>
+      <c r="S35" s="2">
+        <v>42</v>
+      </c>
       <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
+      <c r="U35" s="2">
+        <v>94</v>
+      </c>
+      <c r="V35" s="2">
+        <v>164</v>
+      </c>
       <c r="W35" s="2"/>
       <c r="X35" s="4"/>
       <c r="Y35" s="4"/>
@@ -4410,7 +4674,7 @@
       <c r="BT35" s="2"/>
       <c r="BU35" s="2"/>
     </row>
-    <row r="36" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>87</v>
       </c>
@@ -4447,11 +4711,19 @@
       <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
+      <c r="R36" s="2">
+        <v>23</v>
+      </c>
+      <c r="S36" s="2">
+        <v>48</v>
+      </c>
       <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
+      <c r="U36" s="2">
+        <v>121</v>
+      </c>
+      <c r="V36" s="2">
+        <v>144</v>
+      </c>
       <c r="W36" s="2"/>
       <c r="X36" s="4"/>
       <c r="Y36" s="4"/>
@@ -4522,7 +4794,7 @@
       <c r="BT36" s="2"/>
       <c r="BU36" s="2"/>
     </row>
-    <row r="37" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -4554,11 +4826,19 @@
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
       <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
+      <c r="R37" s="2">
+        <v>23</v>
+      </c>
+      <c r="S37" s="2">
+        <v>48</v>
+      </c>
       <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
+      <c r="U37" s="2">
+        <v>121</v>
+      </c>
+      <c r="V37" s="2">
+        <v>144</v>
+      </c>
       <c r="W37" s="2"/>
       <c r="X37" s="4"/>
       <c r="Y37" s="4"/>
@@ -4611,7 +4891,7 @@
       <c r="BT37" s="2"/>
       <c r="BU37" s="2"/>
     </row>
-    <row r="38" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -4641,11 +4921,19 @@
       <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
+      <c r="R38" s="2">
+        <v>23</v>
+      </c>
+      <c r="S38" s="2">
+        <v>48</v>
+      </c>
       <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
+      <c r="U38" s="2">
+        <v>121</v>
+      </c>
+      <c r="V38" s="2">
+        <v>144</v>
+      </c>
       <c r="W38" s="2"/>
       <c r="X38" s="4"/>
       <c r="Y38" s="4"/>
@@ -4718,7 +5006,7 @@
       <c r="BT38" s="2"/>
       <c r="BU38" s="2"/>
     </row>
-    <row r="39" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -4758,10 +5046,16 @@
       <c r="R39" s="2">
         <v>23</v>
       </c>
-      <c r="S39" s="2"/>
+      <c r="S39" s="2">
+        <v>48</v>
+      </c>
       <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
+      <c r="U39" s="2">
+        <v>121</v>
+      </c>
+      <c r="V39" s="2">
+        <v>144</v>
+      </c>
       <c r="W39" s="2"/>
       <c r="X39" s="4"/>
       <c r="Y39" s="4"/>
@@ -4814,7 +5108,7 @@
       <c r="BT39" s="2"/>
       <c r="BU39" s="2"/>
     </row>
-    <row r="40" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -4846,11 +5140,19 @@
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
+      <c r="R40" s="2">
+        <v>23</v>
+      </c>
+      <c r="S40" s="2">
+        <v>48</v>
+      </c>
       <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
+      <c r="U40" s="2">
+        <v>121</v>
+      </c>
+      <c r="V40" s="2">
+        <v>144</v>
+      </c>
       <c r="W40" s="2"/>
       <c r="X40" s="4"/>
       <c r="Y40" s="4"/>
@@ -4903,7 +5205,7 @@
       <c r="BT40" s="2"/>
       <c r="BU40" s="2"/>
     </row>
-    <row r="41" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>87</v>
       </c>
@@ -4935,11 +5237,19 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="2"/>
-      <c r="R41" s="2"/>
-      <c r="S41" s="2"/>
+      <c r="R41" s="2">
+        <v>23</v>
+      </c>
+      <c r="S41" s="2">
+        <v>48</v>
+      </c>
       <c r="T41" s="2"/>
-      <c r="U41" s="2"/>
-      <c r="V41" s="2"/>
+      <c r="U41" s="2">
+        <v>121</v>
+      </c>
+      <c r="V41" s="2">
+        <v>144</v>
+      </c>
       <c r="W41" s="2"/>
       <c r="X41" s="4"/>
       <c r="Y41" s="4"/>
@@ -5026,7 +5336,7 @@
       <c r="BT41" s="2"/>
       <c r="BU41" s="2"/>
     </row>
-    <row r="42" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -5058,11 +5368,19 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
       <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
+      <c r="R42" s="2">
+        <v>23</v>
+      </c>
+      <c r="S42" s="2">
+        <v>48</v>
+      </c>
       <c r="T42" s="2"/>
-      <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
+      <c r="U42" s="2">
+        <v>121</v>
+      </c>
+      <c r="V42" s="2">
+        <v>144</v>
+      </c>
       <c r="W42" s="2"/>
       <c r="X42" s="4"/>
       <c r="Y42" s="4"/>
@@ -5115,7 +5433,7 @@
       <c r="BT42" s="2"/>
       <c r="BU42" s="2"/>
     </row>
-    <row r="43" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -5147,11 +5465,19 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
       <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
+      <c r="R43" s="2">
+        <v>23</v>
+      </c>
+      <c r="S43" s="2">
+        <v>48</v>
+      </c>
       <c r="T43" s="2"/>
-      <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
+      <c r="U43" s="2">
+        <v>121</v>
+      </c>
+      <c r="V43" s="2">
+        <v>144</v>
+      </c>
       <c r="W43" s="2"/>
       <c r="X43" s="4"/>
       <c r="Y43" s="4"/>
@@ -5242,7 +5568,7 @@
       <c r="BT43" s="2"/>
       <c r="BU43" s="2"/>
     </row>
-    <row r="44" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -5279,13 +5605,19 @@
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
+      <c r="R44" s="2">
+        <v>23</v>
+      </c>
       <c r="S44" s="2">
         <v>48</v>
       </c>
       <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
+      <c r="U44" s="2">
+        <v>121</v>
+      </c>
+      <c r="V44" s="2">
+        <v>144</v>
+      </c>
       <c r="W44" s="2"/>
       <c r="X44" s="4"/>
       <c r="Y44" s="4"/>
@@ -5338,7 +5670,7 @@
       <c r="BT44" s="2"/>
       <c r="BU44" s="2"/>
     </row>
-    <row r="45" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -5370,11 +5702,19 @@
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
       <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
+      <c r="R45" s="2">
+        <v>23</v>
+      </c>
+      <c r="S45" s="2">
+        <v>48</v>
+      </c>
       <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
+      <c r="U45" s="2">
+        <v>121</v>
+      </c>
+      <c r="V45" s="2">
+        <v>144</v>
+      </c>
       <c r="W45" s="2"/>
       <c r="X45" s="4"/>
       <c r="Y45" s="4"/>
@@ -5427,7 +5767,7 @@
       <c r="BT45" s="2"/>
       <c r="BU45" s="2"/>
     </row>
-    <row r="46" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -5466,11 +5806,19 @@
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
-      <c r="S46" s="2"/>
+      <c r="R46" s="2">
+        <v>23</v>
+      </c>
+      <c r="S46" s="2">
+        <v>48</v>
+      </c>
       <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
+      <c r="U46" s="2">
+        <v>121</v>
+      </c>
+      <c r="V46" s="2">
+        <v>144</v>
+      </c>
       <c r="W46" s="2"/>
       <c r="X46" s="4"/>
       <c r="Y46" s="4"/>
@@ -5561,7 +5909,7 @@
       <c r="BT46" s="2"/>
       <c r="BU46" s="2"/>
     </row>
-    <row r="47" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -5593,11 +5941,19 @@
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="2"/>
-      <c r="S47" s="2"/>
+      <c r="R47" s="2">
+        <v>23</v>
+      </c>
+      <c r="S47" s="2">
+        <v>48</v>
+      </c>
       <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
+      <c r="U47" s="2">
+        <v>121</v>
+      </c>
+      <c r="V47" s="2">
+        <v>144</v>
+      </c>
       <c r="W47" s="2"/>
       <c r="X47" s="4"/>
       <c r="Y47" s="4"/>
@@ -5650,7 +6006,7 @@
       <c r="BT47" s="2"/>
       <c r="BU47" s="2"/>
     </row>
-    <row r="48" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>87</v>
       </c>
@@ -5682,11 +6038,19 @@
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
+      <c r="R48" s="2">
+        <v>23</v>
+      </c>
+      <c r="S48" s="2">
+        <v>48</v>
+      </c>
       <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
+      <c r="U48" s="2">
+        <v>121</v>
+      </c>
+      <c r="V48" s="2">
+        <v>144</v>
+      </c>
       <c r="W48" s="2"/>
       <c r="X48" s="4"/>
       <c r="Y48" s="4"/>
@@ -5739,7 +6103,7 @@
       <c r="BT48" s="2"/>
       <c r="BU48" s="2"/>
     </row>
-    <row r="49" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -5769,11 +6133,19 @@
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
       <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
+      <c r="R49" s="2">
+        <v>23</v>
+      </c>
+      <c r="S49" s="2">
+        <v>48</v>
+      </c>
       <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
+      <c r="U49" s="2">
+        <v>121</v>
+      </c>
+      <c r="V49" s="2">
+        <v>144</v>
+      </c>
       <c r="W49" s="2"/>
       <c r="X49" s="4"/>
       <c r="Y49" s="4"/>
@@ -5864,7 +6236,7 @@
       <c r="BT49" s="2"/>
       <c r="BU49" s="2"/>
     </row>
-    <row r="50" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -5896,11 +6268,19 @@
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
       <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
-      <c r="S50" s="2"/>
+      <c r="R50" s="2">
+        <v>23</v>
+      </c>
+      <c r="S50" s="2">
+        <v>48</v>
+      </c>
       <c r="T50" s="2"/>
-      <c r="U50" s="2"/>
-      <c r="V50" s="2"/>
+      <c r="U50" s="2">
+        <v>121</v>
+      </c>
+      <c r="V50" s="2">
+        <v>144</v>
+      </c>
       <c r="W50" s="2"/>
       <c r="X50" s="4"/>
       <c r="Y50" s="4"/>
@@ -5953,7 +6333,7 @@
       <c r="BT50" s="2"/>
       <c r="BU50" s="2"/>
     </row>
-    <row r="51" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>87</v>
       </c>
@@ -5983,11 +6363,19 @@
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
       <c r="Q51" s="2"/>
-      <c r="R51" s="2"/>
-      <c r="S51" s="2"/>
+      <c r="R51" s="2">
+        <v>23</v>
+      </c>
+      <c r="S51" s="2">
+        <v>48</v>
+      </c>
       <c r="T51" s="2"/>
-      <c r="U51" s="2"/>
-      <c r="V51" s="2"/>
+      <c r="U51" s="2">
+        <v>121</v>
+      </c>
+      <c r="V51" s="2">
+        <v>144</v>
+      </c>
       <c r="W51" s="2"/>
       <c r="X51" s="4"/>
       <c r="Y51" s="4"/>
@@ -6078,7 +6466,7 @@
       <c r="BT51" s="2"/>
       <c r="BU51" s="2"/>
     </row>
-    <row r="52" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -6110,11 +6498,19 @@
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="2"/>
-      <c r="R52" s="2"/>
-      <c r="S52" s="2"/>
+      <c r="R52" s="2">
+        <v>23</v>
+      </c>
+      <c r="S52" s="2">
+        <v>48</v>
+      </c>
       <c r="T52" s="2"/>
-      <c r="U52" s="2"/>
-      <c r="V52" s="2"/>
+      <c r="U52" s="2">
+        <v>121</v>
+      </c>
+      <c r="V52" s="2">
+        <v>144</v>
+      </c>
       <c r="W52" s="2"/>
       <c r="X52" s="4"/>
       <c r="Y52" s="4"/>
@@ -6167,7 +6563,7 @@
       <c r="BT52" s="2"/>
       <c r="BU52" s="2"/>
     </row>
-    <row r="53" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -6197,11 +6593,19 @@
       <c r="O53" s="4"/>
       <c r="P53" s="4"/>
       <c r="Q53" s="2"/>
-      <c r="R53" s="2"/>
-      <c r="S53" s="2"/>
+      <c r="R53" s="2">
+        <v>23</v>
+      </c>
+      <c r="S53" s="2">
+        <v>48</v>
+      </c>
       <c r="T53" s="2"/>
-      <c r="U53" s="2"/>
-      <c r="V53" s="2"/>
+      <c r="U53" s="2">
+        <v>121</v>
+      </c>
+      <c r="V53" s="2">
+        <v>144</v>
+      </c>
       <c r="W53" s="2"/>
       <c r="X53" s="4"/>
       <c r="Y53" s="4"/>
@@ -6292,7 +6696,7 @@
       <c r="BT53" s="2"/>
       <c r="BU53" s="2"/>
     </row>
-    <row r="54" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>87</v>
       </c>
@@ -6324,11 +6728,19 @@
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
       <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
-      <c r="S54" s="2"/>
+      <c r="R54" s="2">
+        <v>23</v>
+      </c>
+      <c r="S54" s="2">
+        <v>48</v>
+      </c>
       <c r="T54" s="2"/>
-      <c r="U54" s="2"/>
-      <c r="V54" s="2"/>
+      <c r="U54" s="2">
+        <v>121</v>
+      </c>
+      <c r="V54" s="2">
+        <v>144</v>
+      </c>
       <c r="W54" s="2"/>
       <c r="X54" s="4"/>
       <c r="Y54" s="4"/>
@@ -6381,7 +6793,7 @@
       <c r="BT54" s="2"/>
       <c r="BU54" s="2"/>
     </row>
-    <row r="55" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -6411,11 +6823,19 @@
       <c r="O55" s="4"/>
       <c r="P55" s="4"/>
       <c r="Q55" s="2"/>
-      <c r="R55" s="2"/>
-      <c r="S55" s="2"/>
+      <c r="R55" s="2">
+        <v>23</v>
+      </c>
+      <c r="S55" s="2">
+        <v>48</v>
+      </c>
       <c r="T55" s="2"/>
-      <c r="U55" s="2"/>
-      <c r="V55" s="2"/>
+      <c r="U55" s="2">
+        <v>121</v>
+      </c>
+      <c r="V55" s="2">
+        <v>144</v>
+      </c>
       <c r="W55" s="2"/>
       <c r="X55" s="4"/>
       <c r="Y55" s="4"/>
@@ -6472,7 +6892,7 @@
       <c r="BT55" s="2"/>
       <c r="BU55" s="2"/>
     </row>
-    <row r="56" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -6502,11 +6922,19 @@
       <c r="O56" s="4"/>
       <c r="P56" s="4"/>
       <c r="Q56" s="2"/>
-      <c r="R56" s="2"/>
-      <c r="S56" s="2"/>
+      <c r="R56" s="2">
+        <v>23</v>
+      </c>
+      <c r="S56" s="2">
+        <v>48</v>
+      </c>
       <c r="T56" s="2"/>
-      <c r="U56" s="2"/>
-      <c r="V56" s="2"/>
+      <c r="U56" s="2">
+        <v>121</v>
+      </c>
+      <c r="V56" s="2">
+        <v>144</v>
+      </c>
       <c r="W56" s="2"/>
       <c r="X56" s="4"/>
       <c r="Y56" s="4"/>
@@ -6563,7 +6991,7 @@
       <c r="BT56" s="2"/>
       <c r="BU56" s="2"/>
     </row>
-    <row r="57" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -6600,13 +7028,19 @@
       <c r="O57" s="4"/>
       <c r="P57" s="4"/>
       <c r="Q57" s="2"/>
-      <c r="R57" s="2"/>
-      <c r="S57" s="2"/>
+      <c r="R57" s="2">
+        <v>23</v>
+      </c>
+      <c r="S57" s="2">
+        <v>48</v>
+      </c>
       <c r="T57" s="2"/>
       <c r="U57" s="2">
         <v>121</v>
       </c>
-      <c r="V57" s="2"/>
+      <c r="V57" s="2">
+        <v>144</v>
+      </c>
       <c r="W57" s="2"/>
       <c r="X57" s="4"/>
       <c r="Y57" s="4"/>
@@ -6659,7 +7093,7 @@
       <c r="BT57" s="2"/>
       <c r="BU57" s="2"/>
     </row>
-    <row r="58" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>87</v>
       </c>
@@ -6689,11 +7123,19 @@
       <c r="O58" s="4"/>
       <c r="P58" s="4"/>
       <c r="Q58" s="2"/>
-      <c r="R58" s="2"/>
-      <c r="S58" s="2"/>
+      <c r="R58" s="2">
+        <v>23</v>
+      </c>
+      <c r="S58" s="2">
+        <v>48</v>
+      </c>
       <c r="T58" s="2"/>
-      <c r="U58" s="2"/>
-      <c r="V58" s="2"/>
+      <c r="U58" s="2">
+        <v>121</v>
+      </c>
+      <c r="V58" s="2">
+        <v>144</v>
+      </c>
       <c r="W58" s="2"/>
       <c r="X58" s="4"/>
       <c r="Y58" s="4"/>
@@ -6750,7 +7192,7 @@
       <c r="BT58" s="2"/>
       <c r="BU58" s="2"/>
     </row>
-    <row r="59" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>87</v>
       </c>
@@ -6780,11 +7222,19 @@
       <c r="O59" s="4"/>
       <c r="P59" s="4"/>
       <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
-      <c r="S59" s="2"/>
+      <c r="R59" s="2">
+        <v>23</v>
+      </c>
+      <c r="S59" s="2">
+        <v>48</v>
+      </c>
       <c r="T59" s="2"/>
-      <c r="U59" s="2"/>
-      <c r="V59" s="2"/>
+      <c r="U59" s="2">
+        <v>121</v>
+      </c>
+      <c r="V59" s="2">
+        <v>144</v>
+      </c>
       <c r="W59" s="2"/>
       <c r="X59" s="4"/>
       <c r="Y59" s="4"/>
@@ -6879,7 +7329,7 @@
       <c r="BT59" s="2"/>
       <c r="BU59" s="2"/>
     </row>
-    <row r="60" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -6909,11 +7359,19 @@
       <c r="O60" s="4"/>
       <c r="P60" s="4"/>
       <c r="Q60" s="2"/>
-      <c r="R60" s="2"/>
-      <c r="S60" s="2"/>
+      <c r="R60" s="2">
+        <v>23</v>
+      </c>
+      <c r="S60" s="2">
+        <v>48</v>
+      </c>
       <c r="T60" s="2"/>
-      <c r="U60" s="2"/>
-      <c r="V60" s="2"/>
+      <c r="U60" s="2">
+        <v>121</v>
+      </c>
+      <c r="V60" s="2">
+        <v>144</v>
+      </c>
       <c r="W60" s="2"/>
       <c r="X60" s="4"/>
       <c r="Y60" s="4"/>
@@ -6970,7 +7428,7 @@
       <c r="BT60" s="2"/>
       <c r="BU60" s="2"/>
     </row>
-    <row r="61" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>87</v>
       </c>
@@ -7007,10 +7465,16 @@
       <c r="O61" s="4"/>
       <c r="P61" s="4"/>
       <c r="Q61" s="2"/>
-      <c r="R61" s="2"/>
-      <c r="S61" s="2"/>
+      <c r="R61" s="2">
+        <v>23</v>
+      </c>
+      <c r="S61" s="2">
+        <v>48</v>
+      </c>
       <c r="T61" s="2"/>
-      <c r="U61" s="2"/>
+      <c r="U61" s="2">
+        <v>121</v>
+      </c>
       <c r="V61" s="2">
         <v>144</v>
       </c>
@@ -7066,7 +7530,7 @@
       <c r="BT61" s="2"/>
       <c r="BU61" s="2"/>
     </row>
-    <row r="62" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>87</v>
       </c>
@@ -7096,11 +7560,19 @@
       <c r="O62" s="4"/>
       <c r="P62" s="4"/>
       <c r="Q62" s="2"/>
-      <c r="R62" s="2"/>
-      <c r="S62" s="2"/>
+      <c r="R62" s="2">
+        <v>23</v>
+      </c>
+      <c r="S62" s="2">
+        <v>48</v>
+      </c>
       <c r="T62" s="2"/>
-      <c r="U62" s="2"/>
-      <c r="V62" s="2"/>
+      <c r="U62" s="2">
+        <v>121</v>
+      </c>
+      <c r="V62" s="2">
+        <v>144</v>
+      </c>
       <c r="W62" s="2"/>
       <c r="X62" s="4"/>
       <c r="Y62" s="4"/>
@@ -7157,7 +7629,7 @@
       <c r="BT62" s="2"/>
       <c r="BU62" s="2"/>
     </row>
-    <row r="63" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>87</v>
       </c>
@@ -7187,11 +7659,19 @@
       <c r="O63" s="4"/>
       <c r="P63" s="4"/>
       <c r="Q63" s="2"/>
-      <c r="R63" s="2"/>
-      <c r="S63" s="2"/>
+      <c r="R63" s="2">
+        <v>23</v>
+      </c>
+      <c r="S63" s="2">
+        <v>48</v>
+      </c>
       <c r="T63" s="2"/>
-      <c r="U63" s="2"/>
-      <c r="V63" s="2"/>
+      <c r="U63" s="2">
+        <v>121</v>
+      </c>
+      <c r="V63" s="2">
+        <v>144</v>
+      </c>
       <c r="W63" s="2"/>
       <c r="X63" s="4"/>
       <c r="Y63" s="4"/>
@@ -7248,7 +7728,7 @@
       <c r="BT63" s="2"/>
       <c r="BU63" s="2"/>
     </row>
-    <row r="64" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>87</v>
       </c>
@@ -7285,11 +7765,19 @@
       <c r="O64" s="4"/>
       <c r="P64" s="4"/>
       <c r="Q64" s="2"/>
-      <c r="R64" s="2"/>
-      <c r="S64" s="2"/>
+      <c r="R64" s="2">
+        <v>23</v>
+      </c>
+      <c r="S64" s="2">
+        <v>48</v>
+      </c>
       <c r="T64" s="2"/>
-      <c r="U64" s="2"/>
-      <c r="V64" s="2"/>
+      <c r="U64" s="2">
+        <v>121</v>
+      </c>
+      <c r="V64" s="2">
+        <v>144</v>
+      </c>
       <c r="W64" s="2"/>
       <c r="X64" s="4"/>
       <c r="Y64" s="4"/>
@@ -7354,7 +7842,7 @@
       <c r="BT64" s="2"/>
       <c r="BU64" s="2"/>
     </row>
-    <row r="65" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -7391,11 +7879,19 @@
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="2"/>
-      <c r="R65" s="2"/>
-      <c r="S65" s="2"/>
+      <c r="R65" s="2">
+        <v>26</v>
+      </c>
+      <c r="S65" s="2">
+        <v>57</v>
+      </c>
       <c r="T65" s="2"/>
-      <c r="U65" s="2"/>
-      <c r="V65" s="2"/>
+      <c r="U65" s="2">
+        <v>118</v>
+      </c>
+      <c r="V65" s="2">
+        <v>154</v>
+      </c>
       <c r="W65" s="2"/>
       <c r="X65" s="4"/>
       <c r="Y65" s="4"/>
@@ -7466,7 +7962,7 @@
       <c r="BT65" s="2"/>
       <c r="BU65" s="2"/>
     </row>
-    <row r="66" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>88</v>
       </c>
@@ -7506,10 +8002,16 @@
       <c r="R66" s="2">
         <v>26</v>
       </c>
-      <c r="S66" s="2"/>
+      <c r="S66" s="2">
+        <v>57</v>
+      </c>
       <c r="T66" s="2"/>
-      <c r="U66" s="2"/>
-      <c r="V66" s="2"/>
+      <c r="U66" s="2">
+        <v>118</v>
+      </c>
+      <c r="V66" s="2">
+        <v>154</v>
+      </c>
       <c r="W66" s="2"/>
       <c r="X66" s="4"/>
       <c r="Y66" s="4"/>
@@ -7580,7 +8082,7 @@
       <c r="BT66" s="2"/>
       <c r="BU66" s="2"/>
     </row>
-    <row r="67" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>88</v>
       </c>
@@ -7612,11 +8114,19 @@
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
       <c r="Q67" s="2"/>
-      <c r="R67" s="2"/>
-      <c r="S67" s="2"/>
+      <c r="R67" s="2">
+        <v>26</v>
+      </c>
+      <c r="S67" s="2">
+        <v>57</v>
+      </c>
       <c r="T67" s="2"/>
-      <c r="U67" s="2"/>
-      <c r="V67" s="2"/>
+      <c r="U67" s="2">
+        <v>118</v>
+      </c>
+      <c r="V67" s="2">
+        <v>154</v>
+      </c>
       <c r="W67" s="2"/>
       <c r="X67" s="4"/>
       <c r="Y67" s="4"/>
@@ -7669,7 +8179,7 @@
       <c r="BT67" s="2"/>
       <c r="BU67" s="2"/>
     </row>
-    <row r="68" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -7701,11 +8211,19 @@
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
       <c r="Q68" s="2"/>
-      <c r="R68" s="2"/>
-      <c r="S68" s="2"/>
+      <c r="R68" s="2">
+        <v>26</v>
+      </c>
+      <c r="S68" s="2">
+        <v>57</v>
+      </c>
       <c r="T68" s="2"/>
-      <c r="U68" s="2"/>
-      <c r="V68" s="2"/>
+      <c r="U68" s="2">
+        <v>118</v>
+      </c>
+      <c r="V68" s="2">
+        <v>154</v>
+      </c>
       <c r="W68" s="2"/>
       <c r="X68" s="4"/>
       <c r="Y68" s="4"/>
@@ -7758,7 +8276,7 @@
       <c r="BT68" s="2"/>
       <c r="BU68" s="2"/>
     </row>
-    <row r="69" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -7790,11 +8308,19 @@
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
       <c r="Q69" s="2"/>
-      <c r="R69" s="2"/>
-      <c r="S69" s="2"/>
+      <c r="R69" s="2">
+        <v>26</v>
+      </c>
+      <c r="S69" s="2">
+        <v>57</v>
+      </c>
       <c r="T69" s="2"/>
-      <c r="U69" s="2"/>
-      <c r="V69" s="2"/>
+      <c r="U69" s="2">
+        <v>118</v>
+      </c>
+      <c r="V69" s="2">
+        <v>154</v>
+      </c>
       <c r="W69" s="2"/>
       <c r="X69" s="4"/>
       <c r="Y69" s="4"/>
@@ -7847,7 +8373,7 @@
       <c r="BT69" s="2"/>
       <c r="BU69" s="2"/>
     </row>
-    <row r="70" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -7877,11 +8403,19 @@
       <c r="O70" s="4"/>
       <c r="P70" s="4"/>
       <c r="Q70" s="2"/>
-      <c r="R70" s="2"/>
-      <c r="S70" s="2"/>
+      <c r="R70" s="2">
+        <v>26</v>
+      </c>
+      <c r="S70" s="2">
+        <v>57</v>
+      </c>
       <c r="T70" s="2"/>
-      <c r="U70" s="2"/>
-      <c r="V70" s="2"/>
+      <c r="U70" s="2">
+        <v>118</v>
+      </c>
+      <c r="V70" s="2">
+        <v>154</v>
+      </c>
       <c r="W70" s="2"/>
       <c r="X70" s="4"/>
       <c r="Y70" s="4"/>
@@ -7954,7 +8488,7 @@
       <c r="BT70" s="2"/>
       <c r="BU70" s="2"/>
     </row>
-    <row r="71" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>88</v>
       </c>
@@ -7986,11 +8520,19 @@
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
       <c r="Q71" s="2"/>
-      <c r="R71" s="2"/>
-      <c r="S71" s="2"/>
+      <c r="R71" s="2">
+        <v>26</v>
+      </c>
+      <c r="S71" s="2">
+        <v>57</v>
+      </c>
       <c r="T71" s="2"/>
-      <c r="U71" s="2"/>
-      <c r="V71" s="2"/>
+      <c r="U71" s="2">
+        <v>118</v>
+      </c>
+      <c r="V71" s="2">
+        <v>154</v>
+      </c>
       <c r="W71" s="2"/>
       <c r="X71" s="4"/>
       <c r="Y71" s="4"/>
@@ -8043,7 +8585,7 @@
       <c r="BT71" s="2"/>
       <c r="BU71" s="2"/>
     </row>
-    <row r="72" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>88</v>
       </c>
@@ -8075,11 +8617,19 @@
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
       <c r="Q72" s="2"/>
-      <c r="R72" s="2"/>
-      <c r="S72" s="2"/>
+      <c r="R72" s="2">
+        <v>26</v>
+      </c>
+      <c r="S72" s="2">
+        <v>57</v>
+      </c>
       <c r="T72" s="2"/>
-      <c r="U72" s="2"/>
-      <c r="V72" s="2"/>
+      <c r="U72" s="2">
+        <v>118</v>
+      </c>
+      <c r="V72" s="2">
+        <v>154</v>
+      </c>
       <c r="W72" s="2"/>
       <c r="X72" s="4"/>
       <c r="Y72" s="4"/>
@@ -8169,7 +8719,7 @@
       <c r="BT72" s="2"/>
       <c r="BU72" s="2"/>
     </row>
-    <row r="73" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -8206,13 +8756,19 @@
       <c r="O73" s="4"/>
       <c r="P73" s="4"/>
       <c r="Q73" s="2"/>
-      <c r="R73" s="2"/>
+      <c r="R73" s="2">
+        <v>26</v>
+      </c>
       <c r="S73" s="2">
         <v>57</v>
       </c>
       <c r="T73" s="2"/>
-      <c r="U73" s="2"/>
-      <c r="V73" s="2"/>
+      <c r="U73" s="2">
+        <v>118</v>
+      </c>
+      <c r="V73" s="2">
+        <v>154</v>
+      </c>
       <c r="W73" s="2"/>
       <c r="X73" s="4"/>
       <c r="Y73" s="4"/>
@@ -8265,7 +8821,7 @@
       <c r="BT73" s="2"/>
       <c r="BU73" s="2"/>
     </row>
-    <row r="74" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -8297,11 +8853,19 @@
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
       <c r="Q74" s="2"/>
-      <c r="R74" s="2"/>
-      <c r="S74" s="2"/>
+      <c r="R74" s="2">
+        <v>26</v>
+      </c>
+      <c r="S74" s="2">
+        <v>57</v>
+      </c>
       <c r="T74" s="2"/>
-      <c r="U74" s="2"/>
-      <c r="V74" s="2"/>
+      <c r="U74" s="2">
+        <v>118</v>
+      </c>
+      <c r="V74" s="2">
+        <v>154</v>
+      </c>
       <c r="W74" s="2"/>
       <c r="X74" s="4"/>
       <c r="Y74" s="4"/>
@@ -8354,7 +8918,7 @@
       <c r="BT74" s="2"/>
       <c r="BU74" s="2"/>
     </row>
-    <row r="75" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -8386,11 +8950,19 @@
       <c r="O75" s="3"/>
       <c r="P75" s="3"/>
       <c r="Q75" s="2"/>
-      <c r="R75" s="2"/>
-      <c r="S75" s="2"/>
+      <c r="R75" s="2">
+        <v>26</v>
+      </c>
+      <c r="S75" s="2">
+        <v>57</v>
+      </c>
       <c r="T75" s="2"/>
-      <c r="U75" s="2"/>
-      <c r="V75" s="2"/>
+      <c r="U75" s="2">
+        <v>118</v>
+      </c>
+      <c r="V75" s="2">
+        <v>154</v>
+      </c>
       <c r="W75" s="2"/>
       <c r="X75" s="4"/>
       <c r="Y75" s="4"/>
@@ -8481,7 +9053,7 @@
       <c r="BT75" s="2"/>
       <c r="BU75" s="2"/>
     </row>
-    <row r="76" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -8513,11 +9085,19 @@
       <c r="O76" s="3"/>
       <c r="P76" s="3"/>
       <c r="Q76" s="2"/>
-      <c r="R76" s="2"/>
-      <c r="S76" s="2"/>
+      <c r="R76" s="2">
+        <v>26</v>
+      </c>
+      <c r="S76" s="2">
+        <v>57</v>
+      </c>
       <c r="T76" s="2"/>
-      <c r="U76" s="2"/>
-      <c r="V76" s="2"/>
+      <c r="U76" s="2">
+        <v>118</v>
+      </c>
+      <c r="V76" s="2">
+        <v>154</v>
+      </c>
       <c r="W76" s="2"/>
       <c r="X76" s="4"/>
       <c r="Y76" s="4"/>
@@ -8570,7 +9150,7 @@
       <c r="BT76" s="2"/>
       <c r="BU76" s="2"/>
     </row>
-    <row r="77" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -8609,11 +9189,19 @@
       <c r="O77" s="3"/>
       <c r="P77" s="3"/>
       <c r="Q77" s="2"/>
-      <c r="R77" s="2"/>
-      <c r="S77" s="2"/>
+      <c r="R77" s="2">
+        <v>26</v>
+      </c>
+      <c r="S77" s="2">
+        <v>57</v>
+      </c>
       <c r="T77" s="2"/>
-      <c r="U77" s="2"/>
-      <c r="V77" s="2"/>
+      <c r="U77" s="2">
+        <v>118</v>
+      </c>
+      <c r="V77" s="2">
+        <v>154</v>
+      </c>
       <c r="W77" s="2"/>
       <c r="X77" s="4"/>
       <c r="Y77" s="4"/>
@@ -8704,7 +9292,7 @@
       <c r="BT77" s="2"/>
       <c r="BU77" s="2"/>
     </row>
-    <row r="78" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>88</v>
       </c>
@@ -8736,11 +9324,19 @@
       <c r="O78" s="3"/>
       <c r="P78" s="3"/>
       <c r="Q78" s="2"/>
-      <c r="R78" s="2"/>
-      <c r="S78" s="2"/>
+      <c r="R78" s="2">
+        <v>26</v>
+      </c>
+      <c r="S78" s="2">
+        <v>57</v>
+      </c>
       <c r="T78" s="2"/>
-      <c r="U78" s="2"/>
-      <c r="V78" s="2"/>
+      <c r="U78" s="2">
+        <v>118</v>
+      </c>
+      <c r="V78" s="2">
+        <v>154</v>
+      </c>
       <c r="W78" s="2"/>
       <c r="X78" s="4"/>
       <c r="Y78" s="4"/>
@@ -8793,7 +9389,7 @@
       <c r="BT78" s="2"/>
       <c r="BU78" s="2"/>
     </row>
-    <row r="79" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>88</v>
       </c>
@@ -8823,11 +9419,19 @@
       <c r="O79" s="4"/>
       <c r="P79" s="4"/>
       <c r="Q79" s="2"/>
-      <c r="R79" s="2"/>
-      <c r="S79" s="2"/>
+      <c r="R79" s="2">
+        <v>26</v>
+      </c>
+      <c r="S79" s="2">
+        <v>57</v>
+      </c>
       <c r="T79" s="2"/>
-      <c r="U79" s="2"/>
-      <c r="V79" s="2"/>
+      <c r="U79" s="2">
+        <v>118</v>
+      </c>
+      <c r="V79" s="2">
+        <v>154</v>
+      </c>
       <c r="W79" s="2"/>
       <c r="X79" s="4"/>
       <c r="Y79" s="4"/>
@@ -8918,7 +9522,7 @@
       <c r="BT79" s="2"/>
       <c r="BU79" s="2"/>
     </row>
-    <row r="80" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -8950,11 +9554,19 @@
       <c r="O80" s="3"/>
       <c r="P80" s="3"/>
       <c r="Q80" s="2"/>
-      <c r="R80" s="2"/>
-      <c r="S80" s="2"/>
+      <c r="R80" s="2">
+        <v>26</v>
+      </c>
+      <c r="S80" s="2">
+        <v>57</v>
+      </c>
       <c r="T80" s="2"/>
-      <c r="U80" s="2"/>
-      <c r="V80" s="2"/>
+      <c r="U80" s="2">
+        <v>118</v>
+      </c>
+      <c r="V80" s="2">
+        <v>154</v>
+      </c>
       <c r="W80" s="2"/>
       <c r="X80" s="4"/>
       <c r="Y80" s="4"/>
@@ -9007,7 +9619,7 @@
       <c r="BT80" s="2"/>
       <c r="BU80" s="2"/>
     </row>
-    <row r="81" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -9044,13 +9656,19 @@
       <c r="O81" s="4"/>
       <c r="P81" s="4"/>
       <c r="Q81" s="2"/>
-      <c r="R81" s="2"/>
-      <c r="S81" s="2"/>
+      <c r="R81" s="2">
+        <v>26</v>
+      </c>
+      <c r="S81" s="2">
+        <v>57</v>
+      </c>
       <c r="T81" s="2"/>
       <c r="U81" s="2">
         <v>118</v>
       </c>
-      <c r="V81" s="2"/>
+      <c r="V81" s="2">
+        <v>154</v>
+      </c>
       <c r="W81" s="2"/>
       <c r="X81" s="4"/>
       <c r="Y81" s="4"/>
@@ -9141,7 +9759,7 @@
       <c r="BT81" s="2"/>
       <c r="BU81" s="2"/>
     </row>
-    <row r="82" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -9171,11 +9789,19 @@
       <c r="O82" s="4"/>
       <c r="P82" s="4"/>
       <c r="Q82" s="2"/>
-      <c r="R82" s="2"/>
-      <c r="S82" s="2"/>
+      <c r="R82" s="2">
+        <v>26</v>
+      </c>
+      <c r="S82" s="2">
+        <v>57</v>
+      </c>
       <c r="T82" s="2"/>
-      <c r="U82" s="2"/>
-      <c r="V82" s="2"/>
+      <c r="U82" s="2">
+        <v>118</v>
+      </c>
+      <c r="V82" s="2">
+        <v>154</v>
+      </c>
       <c r="W82" s="2"/>
       <c r="X82" s="4"/>
       <c r="Y82" s="4"/>
@@ -9232,7 +9858,7 @@
       <c r="BT82" s="2"/>
       <c r="BU82" s="2"/>
     </row>
-    <row r="83" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -9262,11 +9888,19 @@
       <c r="O83" s="4"/>
       <c r="P83" s="4"/>
       <c r="Q83" s="2"/>
-      <c r="R83" s="2"/>
-      <c r="S83" s="2"/>
+      <c r="R83" s="2">
+        <v>26</v>
+      </c>
+      <c r="S83" s="2">
+        <v>57</v>
+      </c>
       <c r="T83" s="2"/>
-      <c r="U83" s="2"/>
-      <c r="V83" s="2"/>
+      <c r="U83" s="2">
+        <v>118</v>
+      </c>
+      <c r="V83" s="2">
+        <v>154</v>
+      </c>
       <c r="W83" s="2"/>
       <c r="X83" s="4"/>
       <c r="Y83" s="4"/>
@@ -9323,7 +9957,7 @@
       <c r="BT83" s="2"/>
       <c r="BU83" s="2"/>
     </row>
-    <row r="84" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -9353,11 +9987,19 @@
       <c r="O84" s="4"/>
       <c r="P84" s="4"/>
       <c r="Q84" s="2"/>
-      <c r="R84" s="2"/>
-      <c r="S84" s="2"/>
+      <c r="R84" s="2">
+        <v>26</v>
+      </c>
+      <c r="S84" s="2">
+        <v>57</v>
+      </c>
       <c r="T84" s="2"/>
-      <c r="U84" s="2"/>
-      <c r="V84" s="2"/>
+      <c r="U84" s="2">
+        <v>118</v>
+      </c>
+      <c r="V84" s="2">
+        <v>154</v>
+      </c>
       <c r="W84" s="2"/>
       <c r="X84" s="4"/>
       <c r="Y84" s="4"/>
@@ -9448,7 +10090,7 @@
       <c r="BT84" s="2"/>
       <c r="BU84" s="2"/>
     </row>
-    <row r="85" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -9478,11 +10120,19 @@
       <c r="O85" s="4"/>
       <c r="P85" s="4"/>
       <c r="Q85" s="2"/>
-      <c r="R85" s="2"/>
-      <c r="S85" s="2"/>
+      <c r="R85" s="2">
+        <v>26</v>
+      </c>
+      <c r="S85" s="2">
+        <v>57</v>
+      </c>
       <c r="T85" s="2"/>
-      <c r="U85" s="2"/>
-      <c r="V85" s="2"/>
+      <c r="U85" s="2">
+        <v>118</v>
+      </c>
+      <c r="V85" s="2">
+        <v>154</v>
+      </c>
       <c r="W85" s="2"/>
       <c r="X85" s="4"/>
       <c r="Y85" s="4"/>
@@ -9539,7 +10189,7 @@
       <c r="BT85" s="2"/>
       <c r="BU85" s="2"/>
     </row>
-    <row r="86" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -9576,10 +10226,16 @@
       <c r="O86" s="4"/>
       <c r="P86" s="4"/>
       <c r="Q86" s="2"/>
-      <c r="R86" s="2"/>
-      <c r="S86" s="2"/>
+      <c r="R86" s="2">
+        <v>26</v>
+      </c>
+      <c r="S86" s="2">
+        <v>57</v>
+      </c>
       <c r="T86" s="2"/>
-      <c r="U86" s="2"/>
+      <c r="U86" s="2">
+        <v>118</v>
+      </c>
       <c r="V86" s="2">
         <v>154</v>
       </c>
@@ -9635,7 +10291,7 @@
       <c r="BT86" s="2"/>
       <c r="BU86" s="2"/>
     </row>
-    <row r="87" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -9665,11 +10321,19 @@
       <c r="O87" s="4"/>
       <c r="P87" s="4"/>
       <c r="Q87" s="2"/>
-      <c r="R87" s="2"/>
-      <c r="S87" s="2"/>
+      <c r="R87" s="2">
+        <v>26</v>
+      </c>
+      <c r="S87" s="2">
+        <v>57</v>
+      </c>
       <c r="T87" s="2"/>
-      <c r="U87" s="2"/>
-      <c r="V87" s="2"/>
+      <c r="U87" s="2">
+        <v>118</v>
+      </c>
+      <c r="V87" s="2">
+        <v>154</v>
+      </c>
       <c r="W87" s="2"/>
       <c r="X87" s="4"/>
       <c r="Y87" s="4"/>
@@ -9726,7 +10390,7 @@
       <c r="BT87" s="2"/>
       <c r="BU87" s="2"/>
     </row>
-    <row r="88" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -9756,11 +10420,19 @@
       <c r="O88" s="4"/>
       <c r="P88" s="4"/>
       <c r="Q88" s="2"/>
-      <c r="R88" s="2"/>
-      <c r="S88" s="2"/>
+      <c r="R88" s="2">
+        <v>26</v>
+      </c>
+      <c r="S88" s="2">
+        <v>57</v>
+      </c>
       <c r="T88" s="2"/>
-      <c r="U88" s="2"/>
-      <c r="V88" s="2"/>
+      <c r="U88" s="2">
+        <v>118</v>
+      </c>
+      <c r="V88" s="2">
+        <v>154</v>
+      </c>
       <c r="W88" s="2"/>
       <c r="X88" s="4"/>
       <c r="Y88" s="4"/>
@@ -9817,7 +10489,7 @@
       <c r="BT88" s="2"/>
       <c r="BU88" s="2"/>
     </row>
-    <row r="89" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -9847,11 +10519,19 @@
       <c r="O89" s="4"/>
       <c r="P89" s="4"/>
       <c r="Q89" s="2"/>
-      <c r="R89" s="2"/>
-      <c r="S89" s="2"/>
+      <c r="R89" s="2">
+        <v>26</v>
+      </c>
+      <c r="S89" s="2">
+        <v>57</v>
+      </c>
       <c r="T89" s="2"/>
-      <c r="U89" s="2"/>
-      <c r="V89" s="2"/>
+      <c r="U89" s="2">
+        <v>118</v>
+      </c>
+      <c r="V89" s="2">
+        <v>154</v>
+      </c>
       <c r="W89" s="2"/>
       <c r="X89" s="4"/>
       <c r="Y89" s="4"/>
@@ -9908,7 +10588,7 @@
       <c r="BT89" s="2"/>
       <c r="BU89" s="2"/>
     </row>
-    <row r="90" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -9945,11 +10625,19 @@
       <c r="O90" s="4"/>
       <c r="P90" s="4"/>
       <c r="Q90" s="2"/>
-      <c r="R90" s="2"/>
-      <c r="S90" s="2"/>
+      <c r="R90" s="2">
+        <v>26</v>
+      </c>
+      <c r="S90" s="2">
+        <v>57</v>
+      </c>
       <c r="T90" s="2"/>
-      <c r="U90" s="2"/>
-      <c r="V90" s="2"/>
+      <c r="U90" s="2">
+        <v>118</v>
+      </c>
+      <c r="V90" s="2">
+        <v>154</v>
+      </c>
       <c r="W90" s="2"/>
       <c r="X90" s="4"/>
       <c r="Y90" s="4"/>
@@ -10010,7 +10698,7 @@
       <c r="BT90" s="2"/>
       <c r="BU90" s="2"/>
     </row>
-    <row r="91" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>88</v>
       </c>
@@ -10040,11 +10728,19 @@
       <c r="O91" s="4"/>
       <c r="P91" s="4"/>
       <c r="Q91" s="2"/>
-      <c r="R91" s="2"/>
-      <c r="S91" s="2"/>
+      <c r="R91" s="2">
+        <v>26</v>
+      </c>
+      <c r="S91" s="2">
+        <v>57</v>
+      </c>
       <c r="T91" s="2"/>
-      <c r="U91" s="2"/>
-      <c r="V91" s="2"/>
+      <c r="U91" s="2">
+        <v>118</v>
+      </c>
+      <c r="V91" s="2">
+        <v>154</v>
+      </c>
       <c r="W91" s="2"/>
       <c r="X91" s="4"/>
       <c r="Y91" s="4"/>
@@ -10101,7 +10797,7 @@
       <c r="BT91" s="2"/>
       <c r="BU91" s="2"/>
     </row>
-    <row r="92" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>89</v>
       </c>
@@ -10138,11 +10834,19 @@
       <c r="O92" s="4"/>
       <c r="P92" s="4"/>
       <c r="Q92" s="2"/>
-      <c r="R92" s="2"/>
-      <c r="S92" s="2"/>
+      <c r="R92" s="2">
+        <v>29</v>
+      </c>
+      <c r="S92" s="2">
+        <v>50</v>
+      </c>
       <c r="T92" s="2"/>
-      <c r="U92" s="2"/>
-      <c r="V92" s="2"/>
+      <c r="U92" s="2">
+        <v>102</v>
+      </c>
+      <c r="V92" s="2">
+        <v>130</v>
+      </c>
       <c r="W92" s="2"/>
       <c r="X92" s="4"/>
       <c r="Y92" s="4"/>
@@ -10213,7 +10917,7 @@
       <c r="BT92" s="2"/>
       <c r="BU92" s="2"/>
     </row>
-    <row r="93" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>89</v>
       </c>
@@ -10253,10 +10957,16 @@
       <c r="R93" s="2">
         <v>29</v>
       </c>
-      <c r="S93" s="2"/>
+      <c r="S93" s="2">
+        <v>50</v>
+      </c>
       <c r="T93" s="2"/>
-      <c r="U93" s="2"/>
-      <c r="V93" s="2"/>
+      <c r="U93" s="2">
+        <v>102</v>
+      </c>
+      <c r="V93" s="2">
+        <v>130</v>
+      </c>
       <c r="W93" s="2"/>
       <c r="X93" s="4"/>
       <c r="Y93" s="4"/>
@@ -10327,7 +11037,7 @@
       <c r="BT93" s="2"/>
       <c r="BU93" s="2"/>
     </row>
-    <row r="94" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>89</v>
       </c>
@@ -10359,11 +11069,19 @@
       <c r="O94" s="3"/>
       <c r="P94" s="3"/>
       <c r="Q94" s="2"/>
-      <c r="R94" s="2"/>
-      <c r="S94" s="2"/>
+      <c r="R94" s="2">
+        <v>29</v>
+      </c>
+      <c r="S94" s="2">
+        <v>50</v>
+      </c>
       <c r="T94" s="2"/>
-      <c r="U94" s="2"/>
-      <c r="V94" s="2"/>
+      <c r="U94" s="2">
+        <v>102</v>
+      </c>
+      <c r="V94" s="2">
+        <v>130</v>
+      </c>
       <c r="W94" s="2"/>
       <c r="X94" s="4"/>
       <c r="Y94" s="4"/>
@@ -10416,7 +11134,7 @@
       <c r="BT94" s="2"/>
       <c r="BU94" s="2"/>
     </row>
-    <row r="95" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>89</v>
       </c>
@@ -10446,11 +11164,19 @@
       <c r="O95" s="4"/>
       <c r="P95" s="4"/>
       <c r="Q95" s="2"/>
-      <c r="R95" s="2"/>
-      <c r="S95" s="2"/>
+      <c r="R95" s="2">
+        <v>29</v>
+      </c>
+      <c r="S95" s="2">
+        <v>50</v>
+      </c>
       <c r="T95" s="2"/>
-      <c r="U95" s="2"/>
-      <c r="V95" s="2"/>
+      <c r="U95" s="2">
+        <v>102</v>
+      </c>
+      <c r="V95" s="2">
+        <v>130</v>
+      </c>
       <c r="W95" s="2"/>
       <c r="X95" s="4"/>
       <c r="Y95" s="4"/>
@@ -10541,7 +11267,7 @@
       <c r="BT95" s="2"/>
       <c r="BU95" s="2"/>
     </row>
-    <row r="96" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>89</v>
       </c>
@@ -10573,11 +11299,19 @@
       <c r="O96" s="3"/>
       <c r="P96" s="3"/>
       <c r="Q96" s="2"/>
-      <c r="R96" s="2"/>
-      <c r="S96" s="2"/>
+      <c r="R96" s="2">
+        <v>29</v>
+      </c>
+      <c r="S96" s="2">
+        <v>50</v>
+      </c>
       <c r="T96" s="2"/>
-      <c r="U96" s="2"/>
-      <c r="V96" s="2"/>
+      <c r="U96" s="2">
+        <v>102</v>
+      </c>
+      <c r="V96" s="2">
+        <v>130</v>
+      </c>
       <c r="W96" s="2"/>
       <c r="X96" s="4"/>
       <c r="Y96" s="4"/>
@@ -10630,7 +11364,7 @@
       <c r="BT96" s="2"/>
       <c r="BU96" s="2"/>
     </row>
-    <row r="97" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>89</v>
       </c>
@@ -10667,13 +11401,19 @@
       <c r="O97" s="4"/>
       <c r="P97" s="4"/>
       <c r="Q97" s="2"/>
-      <c r="R97" s="2"/>
+      <c r="R97" s="2">
+        <v>29</v>
+      </c>
       <c r="S97" s="2">
         <v>50</v>
       </c>
       <c r="T97" s="2"/>
-      <c r="U97" s="2"/>
-      <c r="V97" s="2"/>
+      <c r="U97" s="2">
+        <v>102</v>
+      </c>
+      <c r="V97" s="2">
+        <v>130</v>
+      </c>
       <c r="W97" s="2"/>
       <c r="X97" s="4"/>
       <c r="Y97" s="4"/>
@@ -10764,7 +11504,7 @@
       <c r="BT97" s="2"/>
       <c r="BU97" s="2"/>
     </row>
-    <row r="98" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>89</v>
       </c>
@@ -10796,11 +11536,19 @@
       <c r="O98" s="3"/>
       <c r="P98" s="3"/>
       <c r="Q98" s="2"/>
-      <c r="R98" s="2"/>
-      <c r="S98" s="2"/>
+      <c r="R98" s="2">
+        <v>29</v>
+      </c>
+      <c r="S98" s="2">
+        <v>50</v>
+      </c>
       <c r="T98" s="2"/>
-      <c r="U98" s="2"/>
-      <c r="V98" s="2"/>
+      <c r="U98" s="2">
+        <v>102</v>
+      </c>
+      <c r="V98" s="2">
+        <v>130</v>
+      </c>
       <c r="W98" s="2"/>
       <c r="X98" s="4"/>
       <c r="Y98" s="4"/>
@@ -10853,7 +11601,7 @@
       <c r="BT98" s="2"/>
       <c r="BU98" s="2"/>
     </row>
-    <row r="99" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>89</v>
       </c>
@@ -10885,11 +11633,19 @@
       <c r="O99" s="3"/>
       <c r="P99" s="3"/>
       <c r="Q99" s="2"/>
-      <c r="R99" s="2"/>
-      <c r="S99" s="2"/>
+      <c r="R99" s="2">
+        <v>29</v>
+      </c>
+      <c r="S99" s="2">
+        <v>50</v>
+      </c>
       <c r="T99" s="2"/>
-      <c r="U99" s="2"/>
-      <c r="V99" s="2"/>
+      <c r="U99" s="2">
+        <v>102</v>
+      </c>
+      <c r="V99" s="2">
+        <v>130</v>
+      </c>
       <c r="W99" s="2"/>
       <c r="X99" s="4"/>
       <c r="Y99" s="4"/>
@@ -10942,7 +11698,7 @@
       <c r="BT99" s="2"/>
       <c r="BU99" s="2"/>
     </row>
-    <row r="100" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>89</v>
       </c>
@@ -10972,11 +11728,19 @@
       <c r="O100" s="4"/>
       <c r="P100" s="4"/>
       <c r="Q100" s="2"/>
-      <c r="R100" s="2"/>
-      <c r="S100" s="2"/>
+      <c r="R100" s="2">
+        <v>29</v>
+      </c>
+      <c r="S100" s="2">
+        <v>50</v>
+      </c>
       <c r="T100" s="2"/>
-      <c r="U100" s="2"/>
-      <c r="V100" s="2"/>
+      <c r="U100" s="2">
+        <v>102</v>
+      </c>
+      <c r="V100" s="2">
+        <v>130</v>
+      </c>
       <c r="W100" s="2"/>
       <c r="X100" s="4"/>
       <c r="Y100" s="4"/>
@@ -11067,7 +11831,7 @@
       <c r="BT100" s="2"/>
       <c r="BU100" s="2"/>
     </row>
-    <row r="101" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>89</v>
       </c>
@@ -11099,11 +11863,19 @@
       <c r="O101" s="3"/>
       <c r="P101" s="3"/>
       <c r="Q101" s="2"/>
-      <c r="R101" s="2"/>
-      <c r="S101" s="2"/>
+      <c r="R101" s="2">
+        <v>29</v>
+      </c>
+      <c r="S101" s="2">
+        <v>50</v>
+      </c>
       <c r="T101" s="2"/>
-      <c r="U101" s="2"/>
-      <c r="V101" s="2"/>
+      <c r="U101" s="2">
+        <v>102</v>
+      </c>
+      <c r="V101" s="2">
+        <v>130</v>
+      </c>
       <c r="W101" s="2"/>
       <c r="X101" s="4"/>
       <c r="Y101" s="4"/>
@@ -11156,7 +11928,7 @@
       <c r="BT101" s="2"/>
       <c r="BU101" s="2"/>
     </row>
-    <row r="102" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>89</v>
       </c>
@@ -11188,11 +11960,19 @@
       <c r="O102" s="3"/>
       <c r="P102" s="3"/>
       <c r="Q102" s="2"/>
-      <c r="R102" s="2"/>
-      <c r="S102" s="2"/>
+      <c r="R102" s="2">
+        <v>29</v>
+      </c>
+      <c r="S102" s="2">
+        <v>50</v>
+      </c>
       <c r="T102" s="2"/>
-      <c r="U102" s="2"/>
-      <c r="V102" s="2"/>
+      <c r="U102" s="2">
+        <v>102</v>
+      </c>
+      <c r="V102" s="2">
+        <v>130</v>
+      </c>
       <c r="W102" s="2"/>
       <c r="X102" s="4"/>
       <c r="Y102" s="4"/>
@@ -11245,7 +12025,7 @@
       <c r="BT102" s="2"/>
       <c r="BU102" s="2"/>
     </row>
-    <row r="103" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>89</v>
       </c>
@@ -11277,11 +12057,19 @@
       <c r="O103" s="3"/>
       <c r="P103" s="3"/>
       <c r="Q103" s="2"/>
-      <c r="R103" s="2"/>
-      <c r="S103" s="2"/>
+      <c r="R103" s="2">
+        <v>29</v>
+      </c>
+      <c r="S103" s="2">
+        <v>50</v>
+      </c>
       <c r="T103" s="2"/>
-      <c r="U103" s="2"/>
-      <c r="V103" s="2"/>
+      <c r="U103" s="2">
+        <v>102</v>
+      </c>
+      <c r="V103" s="2">
+        <v>130</v>
+      </c>
       <c r="W103" s="2"/>
       <c r="X103" s="4"/>
       <c r="Y103" s="4"/>
@@ -11334,7 +12122,7 @@
       <c r="BT103" s="2"/>
       <c r="BU103" s="2"/>
     </row>
-    <row r="104" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>89</v>
       </c>
@@ -11371,11 +12159,19 @@
       <c r="O104" s="4"/>
       <c r="P104" s="4"/>
       <c r="Q104" s="2"/>
-      <c r="R104" s="2"/>
-      <c r="S104" s="2"/>
+      <c r="R104" s="2">
+        <v>29</v>
+      </c>
+      <c r="S104" s="2">
+        <v>50</v>
+      </c>
       <c r="T104" s="2"/>
-      <c r="U104" s="2"/>
-      <c r="V104" s="2"/>
+      <c r="U104" s="2">
+        <v>102</v>
+      </c>
+      <c r="V104" s="2">
+        <v>130</v>
+      </c>
       <c r="W104" s="2"/>
       <c r="X104" s="4"/>
       <c r="Y104" s="4"/>
@@ -11466,7 +12262,7 @@
       <c r="BT104" s="2"/>
       <c r="BU104" s="2"/>
     </row>
-    <row r="105" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>89</v>
       </c>
@@ -11498,11 +12294,19 @@
       <c r="O105" s="3"/>
       <c r="P105" s="3"/>
       <c r="Q105" s="2"/>
-      <c r="R105" s="2"/>
-      <c r="S105" s="2"/>
+      <c r="R105" s="2">
+        <v>29</v>
+      </c>
+      <c r="S105" s="2">
+        <v>50</v>
+      </c>
       <c r="T105" s="2"/>
-      <c r="U105" s="2"/>
-      <c r="V105" s="2"/>
+      <c r="U105" s="2">
+        <v>102</v>
+      </c>
+      <c r="V105" s="2">
+        <v>130</v>
+      </c>
       <c r="W105" s="2"/>
       <c r="X105" s="4"/>
       <c r="Y105" s="4"/>
@@ -11555,7 +12359,7 @@
       <c r="BT105" s="2"/>
       <c r="BU105" s="2"/>
     </row>
-    <row r="106" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>89</v>
       </c>
@@ -11592,13 +12396,19 @@
       <c r="O106" s="4"/>
       <c r="P106" s="4"/>
       <c r="Q106" s="2"/>
-      <c r="R106" s="2"/>
-      <c r="S106" s="2"/>
+      <c r="R106" s="2">
+        <v>29</v>
+      </c>
+      <c r="S106" s="2">
+        <v>50</v>
+      </c>
       <c r="T106" s="2"/>
       <c r="U106" s="2">
         <v>102</v>
       </c>
-      <c r="V106" s="2"/>
+      <c r="V106" s="2">
+        <v>130</v>
+      </c>
       <c r="W106" s="2"/>
       <c r="X106" s="4"/>
       <c r="Y106" s="4"/>
@@ -11689,7 +12499,7 @@
       <c r="BT106" s="2"/>
       <c r="BU106" s="2"/>
     </row>
-    <row r="107" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>89</v>
       </c>
@@ -11721,11 +12531,19 @@
       <c r="O107" s="3"/>
       <c r="P107" s="3"/>
       <c r="Q107" s="2"/>
-      <c r="R107" s="2"/>
-      <c r="S107" s="2"/>
+      <c r="R107" s="2">
+        <v>29</v>
+      </c>
+      <c r="S107" s="2">
+        <v>50</v>
+      </c>
       <c r="T107" s="2"/>
-      <c r="U107" s="2"/>
-      <c r="V107" s="2"/>
+      <c r="U107" s="2">
+        <v>102</v>
+      </c>
+      <c r="V107" s="2">
+        <v>130</v>
+      </c>
       <c r="W107" s="2"/>
       <c r="X107" s="4"/>
       <c r="Y107" s="4"/>
@@ -11778,7 +12596,7 @@
       <c r="BT107" s="2"/>
       <c r="BU107" s="2"/>
     </row>
-    <row r="108" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>89</v>
       </c>
@@ -11808,11 +12626,19 @@
       <c r="O108" s="4"/>
       <c r="P108" s="4"/>
       <c r="Q108" s="2"/>
-      <c r="R108" s="2"/>
-      <c r="S108" s="2"/>
+      <c r="R108" s="2">
+        <v>29</v>
+      </c>
+      <c r="S108" s="2">
+        <v>50</v>
+      </c>
       <c r="T108" s="2"/>
-      <c r="U108" s="2"/>
-      <c r="V108" s="2"/>
+      <c r="U108" s="2">
+        <v>102</v>
+      </c>
+      <c r="V108" s="2">
+        <v>130</v>
+      </c>
       <c r="W108" s="2"/>
       <c r="X108" s="4"/>
       <c r="Y108" s="4"/>
@@ -11869,7 +12695,7 @@
       <c r="BT108" s="2"/>
       <c r="BU108" s="2"/>
     </row>
-    <row r="109" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>89</v>
       </c>
@@ -11899,11 +12725,19 @@
       <c r="O109" s="4"/>
       <c r="P109" s="4"/>
       <c r="Q109" s="2"/>
-      <c r="R109" s="2"/>
-      <c r="S109" s="2"/>
+      <c r="R109" s="2">
+        <v>29</v>
+      </c>
+      <c r="S109" s="2">
+        <v>50</v>
+      </c>
       <c r="T109" s="2"/>
-      <c r="U109" s="2"/>
-      <c r="V109" s="2"/>
+      <c r="U109" s="2">
+        <v>102</v>
+      </c>
+      <c r="V109" s="2">
+        <v>130</v>
+      </c>
       <c r="W109" s="2"/>
       <c r="X109" s="4"/>
       <c r="Y109" s="4"/>
@@ -11960,7 +12794,7 @@
       <c r="BT109" s="2"/>
       <c r="BU109" s="2"/>
     </row>
-    <row r="110" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>89</v>
       </c>
@@ -11997,10 +12831,16 @@
       <c r="O110" s="4"/>
       <c r="P110" s="4"/>
       <c r="Q110" s="2"/>
-      <c r="R110" s="2"/>
-      <c r="S110" s="2"/>
+      <c r="R110" s="2">
+        <v>29</v>
+      </c>
+      <c r="S110" s="2">
+        <v>50</v>
+      </c>
       <c r="T110" s="2"/>
-      <c r="U110" s="2"/>
+      <c r="U110" s="2">
+        <v>102</v>
+      </c>
       <c r="V110" s="2">
         <v>130</v>
       </c>
@@ -12060,7 +12900,7 @@
       <c r="BT110" s="2"/>
       <c r="BU110" s="2"/>
     </row>
-    <row r="111" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>89</v>
       </c>
@@ -12090,11 +12930,19 @@
       <c r="O111" s="4"/>
       <c r="P111" s="4"/>
       <c r="Q111" s="2"/>
-      <c r="R111" s="2"/>
-      <c r="S111" s="2"/>
+      <c r="R111" s="2">
+        <v>29</v>
+      </c>
+      <c r="S111" s="2">
+        <v>50</v>
+      </c>
       <c r="T111" s="2"/>
-      <c r="U111" s="2"/>
-      <c r="V111" s="2"/>
+      <c r="U111" s="2">
+        <v>102</v>
+      </c>
+      <c r="V111" s="2">
+        <v>130</v>
+      </c>
       <c r="W111" s="2"/>
       <c r="X111" s="4"/>
       <c r="Y111" s="4"/>
@@ -12151,7 +12999,7 @@
       <c r="BT111" s="2"/>
       <c r="BU111" s="2"/>
     </row>
-    <row r="112" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>89</v>
       </c>
@@ -12181,11 +13029,19 @@
       <c r="O112" s="4"/>
       <c r="P112" s="4"/>
       <c r="Q112" s="2"/>
-      <c r="R112" s="2"/>
-      <c r="S112" s="2"/>
+      <c r="R112" s="2">
+        <v>29</v>
+      </c>
+      <c r="S112" s="2">
+        <v>50</v>
+      </c>
       <c r="T112" s="2"/>
-      <c r="U112" s="2"/>
-      <c r="V112" s="2"/>
+      <c r="U112" s="2">
+        <v>102</v>
+      </c>
+      <c r="V112" s="2">
+        <v>130</v>
+      </c>
       <c r="W112" s="2"/>
       <c r="X112" s="4"/>
       <c r="Y112" s="4"/>
@@ -12276,7 +13132,7 @@
       <c r="BT112" s="2"/>
       <c r="BU112" s="2"/>
     </row>
-    <row r="113" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>89</v>
       </c>
@@ -12306,11 +13162,19 @@
       <c r="O113" s="4"/>
       <c r="P113" s="4"/>
       <c r="Q113" s="2"/>
-      <c r="R113" s="2"/>
-      <c r="S113" s="2"/>
+      <c r="R113" s="2">
+        <v>29</v>
+      </c>
+      <c r="S113" s="2">
+        <v>50</v>
+      </c>
       <c r="T113" s="2"/>
-      <c r="U113" s="2"/>
-      <c r="V113" s="2"/>
+      <c r="U113" s="2">
+        <v>102</v>
+      </c>
+      <c r="V113" s="2">
+        <v>130</v>
+      </c>
       <c r="W113" s="2"/>
       <c r="X113" s="4"/>
       <c r="Y113" s="4"/>
@@ -12367,7 +13231,7 @@
       <c r="BT113" s="2"/>
       <c r="BU113" s="2"/>
     </row>
-    <row r="114" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>89</v>
       </c>
@@ -12397,11 +13261,19 @@
       <c r="O114" s="4"/>
       <c r="P114" s="4"/>
       <c r="Q114" s="2"/>
-      <c r="R114" s="2"/>
-      <c r="S114" s="2"/>
+      <c r="R114" s="2">
+        <v>29</v>
+      </c>
+      <c r="S114" s="2">
+        <v>50</v>
+      </c>
       <c r="T114" s="2"/>
-      <c r="U114" s="2"/>
-      <c r="V114" s="2"/>
+      <c r="U114" s="2">
+        <v>102</v>
+      </c>
+      <c r="V114" s="2">
+        <v>130</v>
+      </c>
       <c r="W114" s="2"/>
       <c r="X114" s="4"/>
       <c r="Y114" s="4"/>
@@ -12458,7 +13330,7 @@
       <c r="BT114" s="2"/>
       <c r="BU114" s="2"/>
     </row>
-    <row r="115" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>89</v>
       </c>
@@ -12488,11 +13360,19 @@
       <c r="O115" s="4"/>
       <c r="P115" s="4"/>
       <c r="Q115" s="2"/>
-      <c r="R115" s="2"/>
-      <c r="S115" s="2"/>
+      <c r="R115" s="2">
+        <v>29</v>
+      </c>
+      <c r="S115" s="2">
+        <v>50</v>
+      </c>
       <c r="T115" s="2"/>
-      <c r="U115" s="2"/>
-      <c r="V115" s="2"/>
+      <c r="U115" s="2">
+        <v>102</v>
+      </c>
+      <c r="V115" s="2">
+        <v>130</v>
+      </c>
       <c r="W115" s="2"/>
       <c r="X115" s="4"/>
       <c r="Y115" s="4"/>
@@ -12549,7 +13429,7 @@
       <c r="BT115" s="2"/>
       <c r="BU115" s="2"/>
     </row>
-    <row r="116" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>89</v>
       </c>
@@ -12579,11 +13459,19 @@
       <c r="O116" s="4"/>
       <c r="P116" s="4"/>
       <c r="Q116" s="2"/>
-      <c r="R116" s="2"/>
-      <c r="S116" s="2"/>
+      <c r="R116" s="2">
+        <v>29</v>
+      </c>
+      <c r="S116" s="2">
+        <v>50</v>
+      </c>
       <c r="T116" s="2"/>
-      <c r="U116" s="2"/>
-      <c r="V116" s="2"/>
+      <c r="U116" s="2">
+        <v>102</v>
+      </c>
+      <c r="V116" s="2">
+        <v>130</v>
+      </c>
       <c r="W116" s="2"/>
       <c r="X116" s="4"/>
       <c r="Y116" s="4"/>
@@ -12640,7 +13528,7 @@
       <c r="BT116" s="2"/>
       <c r="BU116" s="2"/>
     </row>
-    <row r="117" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>89</v>
       </c>
@@ -12677,11 +13565,19 @@
       <c r="O117" s="4"/>
       <c r="P117" s="4"/>
       <c r="Q117" s="2"/>
-      <c r="R117" s="2"/>
-      <c r="S117" s="2"/>
+      <c r="R117" s="2">
+        <v>29</v>
+      </c>
+      <c r="S117" s="2">
+        <v>50</v>
+      </c>
       <c r="T117" s="2"/>
-      <c r="U117" s="2"/>
-      <c r="V117" s="2"/>
+      <c r="U117" s="2">
+        <v>102</v>
+      </c>
+      <c r="V117" s="2">
+        <v>130</v>
+      </c>
       <c r="W117" s="2"/>
       <c r="X117" s="4"/>
       <c r="Y117" s="4"/>
@@ -12742,7 +13638,7 @@
       <c r="BT117" s="2"/>
       <c r="BU117" s="2"/>
     </row>
-    <row r="118" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>90</v>
       </c>
@@ -12779,11 +13675,19 @@
       <c r="O118" s="4"/>
       <c r="P118" s="4"/>
       <c r="Q118" s="2"/>
-      <c r="R118" s="2"/>
-      <c r="S118" s="2"/>
+      <c r="R118" s="2">
+        <v>35</v>
+      </c>
+      <c r="S118" s="2">
+        <v>51</v>
+      </c>
       <c r="T118" s="2"/>
-      <c r="U118" s="2"/>
-      <c r="V118" s="2"/>
+      <c r="U118" s="2">
+        <v>86</v>
+      </c>
+      <c r="V118" s="2">
+        <v>159</v>
+      </c>
       <c r="W118" s="2"/>
       <c r="X118" s="4"/>
       <c r="Y118" s="4"/>
@@ -12854,7 +13758,7 @@
       <c r="BT118" s="2"/>
       <c r="BU118" s="2"/>
     </row>
-    <row r="119" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>90</v>
       </c>
@@ -12884,11 +13788,19 @@
       <c r="O119" s="4"/>
       <c r="P119" s="4"/>
       <c r="Q119" s="2"/>
-      <c r="R119" s="2"/>
-      <c r="S119" s="2"/>
+      <c r="R119" s="2">
+        <v>35</v>
+      </c>
+      <c r="S119" s="2">
+        <v>51</v>
+      </c>
       <c r="T119" s="2"/>
-      <c r="U119" s="2"/>
-      <c r="V119" s="2"/>
+      <c r="U119" s="2">
+        <v>86</v>
+      </c>
+      <c r="V119" s="2">
+        <v>159</v>
+      </c>
       <c r="W119" s="2"/>
       <c r="X119" s="4"/>
       <c r="Y119" s="4"/>
@@ -12979,7 +13891,7 @@
       <c r="BT119" s="2"/>
       <c r="BU119" s="2"/>
     </row>
-    <row r="120" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>90</v>
       </c>
@@ -13019,10 +13931,16 @@
       <c r="R120" s="2">
         <v>35</v>
       </c>
-      <c r="S120" s="2"/>
+      <c r="S120" s="2">
+        <v>51</v>
+      </c>
       <c r="T120" s="2"/>
-      <c r="U120" s="2"/>
-      <c r="V120" s="2"/>
+      <c r="U120" s="2">
+        <v>86</v>
+      </c>
+      <c r="V120" s="2">
+        <v>159</v>
+      </c>
       <c r="W120" s="2"/>
       <c r="X120" s="4"/>
       <c r="Y120" s="4"/>
@@ -13075,7 +13993,7 @@
       <c r="BT120" s="2"/>
       <c r="BU120" s="2"/>
     </row>
-    <row r="121" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>90</v>
       </c>
@@ -13105,11 +14023,19 @@
       <c r="O121" s="4"/>
       <c r="P121" s="4"/>
       <c r="Q121" s="2"/>
-      <c r="R121" s="2"/>
-      <c r="S121" s="2"/>
+      <c r="R121" s="2">
+        <v>35</v>
+      </c>
+      <c r="S121" s="2">
+        <v>51</v>
+      </c>
       <c r="T121" s="2"/>
-      <c r="U121" s="2"/>
-      <c r="V121" s="2"/>
+      <c r="U121" s="2">
+        <v>86</v>
+      </c>
+      <c r="V121" s="2">
+        <v>159</v>
+      </c>
       <c r="W121" s="2"/>
       <c r="X121" s="4"/>
       <c r="Y121" s="4"/>
@@ -13200,7 +14126,7 @@
       <c r="BT121" s="2"/>
       <c r="BU121" s="2"/>
     </row>
-    <row r="122" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>90</v>
       </c>
@@ -13232,11 +14158,19 @@
       <c r="O122" s="3"/>
       <c r="P122" s="3"/>
       <c r="Q122" s="2"/>
-      <c r="R122" s="2"/>
-      <c r="S122" s="2"/>
+      <c r="R122" s="2">
+        <v>35</v>
+      </c>
+      <c r="S122" s="2">
+        <v>51</v>
+      </c>
       <c r="T122" s="2"/>
-      <c r="U122" s="2"/>
-      <c r="V122" s="2"/>
+      <c r="U122" s="2">
+        <v>86</v>
+      </c>
+      <c r="V122" s="2">
+        <v>159</v>
+      </c>
       <c r="W122" s="2"/>
       <c r="X122" s="4"/>
       <c r="Y122" s="4"/>
@@ -13289,7 +14223,7 @@
       <c r="BT122" s="2"/>
       <c r="BU122" s="2"/>
     </row>
-    <row r="123" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>90</v>
       </c>
@@ -13326,13 +14260,19 @@
       <c r="O123" s="4"/>
       <c r="P123" s="4"/>
       <c r="Q123" s="2"/>
-      <c r="R123" s="2"/>
+      <c r="R123" s="2">
+        <v>35</v>
+      </c>
       <c r="S123" s="2">
         <v>51</v>
       </c>
       <c r="T123" s="2"/>
-      <c r="U123" s="2"/>
-      <c r="V123" s="2"/>
+      <c r="U123" s="2">
+        <v>86</v>
+      </c>
+      <c r="V123" s="2">
+        <v>159</v>
+      </c>
       <c r="W123" s="2"/>
       <c r="X123" s="4"/>
       <c r="Y123" s="4"/>
@@ -13423,7 +14363,7 @@
       <c r="BT123" s="2"/>
       <c r="BU123" s="2"/>
     </row>
-    <row r="124" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>90</v>
       </c>
@@ -13455,11 +14395,19 @@
       <c r="O124" s="3"/>
       <c r="P124" s="3"/>
       <c r="Q124" s="2"/>
-      <c r="R124" s="2"/>
-      <c r="S124" s="2"/>
+      <c r="R124" s="2">
+        <v>35</v>
+      </c>
+      <c r="S124" s="2">
+        <v>51</v>
+      </c>
       <c r="T124" s="2"/>
-      <c r="U124" s="2"/>
-      <c r="V124" s="2"/>
+      <c r="U124" s="2">
+        <v>86</v>
+      </c>
+      <c r="V124" s="2">
+        <v>159</v>
+      </c>
       <c r="W124" s="2"/>
       <c r="X124" s="4"/>
       <c r="Y124" s="4"/>
@@ -13512,7 +14460,7 @@
       <c r="BT124" s="2"/>
       <c r="BU124" s="2"/>
     </row>
-    <row r="125" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>90</v>
       </c>
@@ -13544,11 +14492,19 @@
       <c r="O125" s="3"/>
       <c r="P125" s="3"/>
       <c r="Q125" s="2"/>
-      <c r="R125" s="2"/>
-      <c r="S125" s="2"/>
+      <c r="R125" s="2">
+        <v>35</v>
+      </c>
+      <c r="S125" s="2">
+        <v>51</v>
+      </c>
       <c r="T125" s="2"/>
-      <c r="U125" s="2"/>
-      <c r="V125" s="2"/>
+      <c r="U125" s="2">
+        <v>86</v>
+      </c>
+      <c r="V125" s="2">
+        <v>159</v>
+      </c>
       <c r="W125" s="2"/>
       <c r="X125" s="4"/>
       <c r="Y125" s="4"/>
@@ -13601,7 +14557,7 @@
       <c r="BT125" s="2"/>
       <c r="BU125" s="2"/>
     </row>
-    <row r="126" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>90</v>
       </c>
@@ -13638,11 +14594,19 @@
       <c r="O126" s="4"/>
       <c r="P126" s="4"/>
       <c r="Q126" s="2"/>
-      <c r="R126" s="2"/>
-      <c r="S126" s="2"/>
+      <c r="R126" s="2">
+        <v>35</v>
+      </c>
+      <c r="S126" s="2">
+        <v>51</v>
+      </c>
       <c r="T126" s="2"/>
-      <c r="U126" s="2"/>
-      <c r="V126" s="2"/>
+      <c r="U126" s="2">
+        <v>86</v>
+      </c>
+      <c r="V126" s="2">
+        <v>159</v>
+      </c>
       <c r="W126" s="2"/>
       <c r="X126" s="4"/>
       <c r="Y126" s="4"/>
@@ -13733,7 +14697,7 @@
       <c r="BT126" s="2"/>
       <c r="BU126" s="2"/>
     </row>
-    <row r="127" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>90</v>
       </c>
@@ -13765,11 +14729,19 @@
       <c r="O127" s="3"/>
       <c r="P127" s="3"/>
       <c r="Q127" s="2"/>
-      <c r="R127" s="2"/>
-      <c r="S127" s="2"/>
+      <c r="R127" s="2">
+        <v>35</v>
+      </c>
+      <c r="S127" s="2">
+        <v>51</v>
+      </c>
       <c r="T127" s="2"/>
-      <c r="U127" s="2"/>
-      <c r="V127" s="2"/>
+      <c r="U127" s="2">
+        <v>86</v>
+      </c>
+      <c r="V127" s="2">
+        <v>159</v>
+      </c>
       <c r="W127" s="2"/>
       <c r="X127" s="4"/>
       <c r="Y127" s="4"/>
@@ -13822,7 +14794,7 @@
       <c r="BT127" s="2"/>
       <c r="BU127" s="2"/>
     </row>
-    <row r="128" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>90</v>
       </c>
@@ -13854,11 +14826,19 @@
       <c r="O128" s="3"/>
       <c r="P128" s="3"/>
       <c r="Q128" s="2"/>
-      <c r="R128" s="2"/>
-      <c r="S128" s="2"/>
+      <c r="R128" s="2">
+        <v>35</v>
+      </c>
+      <c r="S128" s="2">
+        <v>51</v>
+      </c>
       <c r="T128" s="2"/>
-      <c r="U128" s="2"/>
-      <c r="V128" s="2"/>
+      <c r="U128" s="2">
+        <v>86</v>
+      </c>
+      <c r="V128" s="2">
+        <v>159</v>
+      </c>
       <c r="W128" s="2"/>
       <c r="X128" s="4"/>
       <c r="Y128" s="4"/>
@@ -13911,7 +14891,7 @@
       <c r="BT128" s="2"/>
       <c r="BU128" s="2"/>
     </row>
-    <row r="129" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>90</v>
       </c>
@@ -13948,13 +14928,19 @@
       <c r="O129" s="4"/>
       <c r="P129" s="4"/>
       <c r="Q129" s="2"/>
-      <c r="R129" s="2"/>
-      <c r="S129" s="2"/>
+      <c r="R129" s="2">
+        <v>35</v>
+      </c>
+      <c r="S129" s="2">
+        <v>51</v>
+      </c>
       <c r="T129" s="2"/>
       <c r="U129" s="2">
         <v>86</v>
       </c>
-      <c r="V129" s="2"/>
+      <c r="V129" s="2">
+        <v>159</v>
+      </c>
       <c r="W129" s="2"/>
       <c r="X129" s="4"/>
       <c r="Y129" s="4"/>
@@ -14007,7 +14993,7 @@
       <c r="BT129" s="2"/>
       <c r="BU129" s="2"/>
     </row>
-    <row r="130" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>90</v>
       </c>
@@ -14039,11 +15025,19 @@
       <c r="O130" s="3"/>
       <c r="P130" s="3"/>
       <c r="Q130" s="2"/>
-      <c r="R130" s="2"/>
-      <c r="S130" s="2"/>
+      <c r="R130" s="2">
+        <v>35</v>
+      </c>
+      <c r="S130" s="2">
+        <v>51</v>
+      </c>
       <c r="T130" s="2"/>
-      <c r="U130" s="2"/>
-      <c r="V130" s="2"/>
+      <c r="U130" s="2">
+        <v>86</v>
+      </c>
+      <c r="V130" s="2">
+        <v>159</v>
+      </c>
       <c r="W130" s="2"/>
       <c r="X130" s="4"/>
       <c r="Y130" s="4"/>
@@ -14096,7 +15090,7 @@
       <c r="BT130" s="2"/>
       <c r="BU130" s="2"/>
     </row>
-    <row r="131" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>90</v>
       </c>
@@ -14126,11 +15120,19 @@
       <c r="O131" s="4"/>
       <c r="P131" s="4"/>
       <c r="Q131" s="2"/>
-      <c r="R131" s="2"/>
-      <c r="S131" s="2"/>
+      <c r="R131" s="2">
+        <v>35</v>
+      </c>
+      <c r="S131" s="2">
+        <v>51</v>
+      </c>
       <c r="T131" s="2"/>
-      <c r="U131" s="2"/>
-      <c r="V131" s="2"/>
+      <c r="U131" s="2">
+        <v>86</v>
+      </c>
+      <c r="V131" s="2">
+        <v>159</v>
+      </c>
       <c r="W131" s="2"/>
       <c r="X131" s="4"/>
       <c r="Y131" s="4"/>
@@ -14221,7 +15223,7 @@
       <c r="BT131" s="2"/>
       <c r="BU131" s="2"/>
     </row>
-    <row r="132" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>90</v>
       </c>
@@ -14253,11 +15255,19 @@
       <c r="O132" s="3"/>
       <c r="P132" s="3"/>
       <c r="Q132" s="2"/>
-      <c r="R132" s="2"/>
-      <c r="S132" s="2"/>
+      <c r="R132" s="2">
+        <v>35</v>
+      </c>
+      <c r="S132" s="2">
+        <v>51</v>
+      </c>
       <c r="T132" s="2"/>
-      <c r="U132" s="2"/>
-      <c r="V132" s="2"/>
+      <c r="U132" s="2">
+        <v>86</v>
+      </c>
+      <c r="V132" s="2">
+        <v>159</v>
+      </c>
       <c r="W132" s="2"/>
       <c r="X132" s="4"/>
       <c r="Y132" s="4"/>
@@ -14310,7 +15320,7 @@
       <c r="BT132" s="2"/>
       <c r="BU132" s="2"/>
     </row>
-    <row r="133" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>90</v>
       </c>
@@ -14340,11 +15350,19 @@
       <c r="O133" s="4"/>
       <c r="P133" s="4"/>
       <c r="Q133" s="2"/>
-      <c r="R133" s="2"/>
-      <c r="S133" s="2"/>
+      <c r="R133" s="2">
+        <v>35</v>
+      </c>
+      <c r="S133" s="2">
+        <v>51</v>
+      </c>
       <c r="T133" s="2"/>
-      <c r="U133" s="2"/>
-      <c r="V133" s="2"/>
+      <c r="U133" s="2">
+        <v>86</v>
+      </c>
+      <c r="V133" s="2">
+        <v>159</v>
+      </c>
       <c r="W133" s="2"/>
       <c r="X133" s="4"/>
       <c r="Y133" s="4"/>
@@ -14435,7 +15453,7 @@
       <c r="BT133" s="2"/>
       <c r="BU133" s="2"/>
     </row>
-    <row r="134" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>90</v>
       </c>
@@ -14465,11 +15483,19 @@
       <c r="O134" s="4"/>
       <c r="P134" s="4"/>
       <c r="Q134" s="2"/>
-      <c r="R134" s="2"/>
-      <c r="S134" s="2"/>
+      <c r="R134" s="2">
+        <v>35</v>
+      </c>
+      <c r="S134" s="2">
+        <v>51</v>
+      </c>
       <c r="T134" s="2"/>
-      <c r="U134" s="2"/>
-      <c r="V134" s="2"/>
+      <c r="U134" s="2">
+        <v>86</v>
+      </c>
+      <c r="V134" s="2">
+        <v>159</v>
+      </c>
       <c r="W134" s="2"/>
       <c r="X134" s="4"/>
       <c r="Y134" s="4"/>
@@ -14526,7 +15552,7 @@
       <c r="BT134" s="2"/>
       <c r="BU134" s="2"/>
     </row>
-    <row r="135" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>90</v>
       </c>
@@ -14556,11 +15582,19 @@
       <c r="O135" s="4"/>
       <c r="P135" s="4"/>
       <c r="Q135" s="2"/>
-      <c r="R135" s="2"/>
-      <c r="S135" s="2"/>
+      <c r="R135" s="2">
+        <v>35</v>
+      </c>
+      <c r="S135" s="2">
+        <v>51</v>
+      </c>
       <c r="T135" s="2"/>
-      <c r="U135" s="2"/>
-      <c r="V135" s="2"/>
+      <c r="U135" s="2">
+        <v>86</v>
+      </c>
+      <c r="V135" s="2">
+        <v>159</v>
+      </c>
       <c r="W135" s="2"/>
       <c r="X135" s="4"/>
       <c r="Y135" s="4"/>
@@ -14617,7 +15651,7 @@
       <c r="BT135" s="2"/>
       <c r="BU135" s="2"/>
     </row>
-    <row r="136" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>90</v>
       </c>
@@ -14647,11 +15681,19 @@
       <c r="O136" s="4"/>
       <c r="P136" s="4"/>
       <c r="Q136" s="2"/>
-      <c r="R136" s="2"/>
-      <c r="S136" s="2"/>
+      <c r="R136" s="2">
+        <v>35</v>
+      </c>
+      <c r="S136" s="2">
+        <v>51</v>
+      </c>
       <c r="T136" s="2"/>
-      <c r="U136" s="2"/>
-      <c r="V136" s="2"/>
+      <c r="U136" s="2">
+        <v>86</v>
+      </c>
+      <c r="V136" s="2">
+        <v>159</v>
+      </c>
       <c r="W136" s="2"/>
       <c r="X136" s="4"/>
       <c r="Y136" s="4"/>
@@ -14708,7 +15750,7 @@
       <c r="BT136" s="2"/>
       <c r="BU136" s="2"/>
     </row>
-    <row r="137" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>90</v>
       </c>
@@ -14738,11 +15780,19 @@
       <c r="O137" s="4"/>
       <c r="P137" s="4"/>
       <c r="Q137" s="2"/>
-      <c r="R137" s="2"/>
-      <c r="S137" s="2"/>
+      <c r="R137" s="2">
+        <v>35</v>
+      </c>
+      <c r="S137" s="2">
+        <v>51</v>
+      </c>
       <c r="T137" s="2"/>
-      <c r="U137" s="2"/>
-      <c r="V137" s="2"/>
+      <c r="U137" s="2">
+        <v>86</v>
+      </c>
+      <c r="V137" s="2">
+        <v>159</v>
+      </c>
       <c r="W137" s="2"/>
       <c r="X137" s="4"/>
       <c r="Y137" s="4"/>
@@ -14799,7 +15849,7 @@
       <c r="BT137" s="2"/>
       <c r="BU137" s="2"/>
     </row>
-    <row r="138" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>90</v>
       </c>
@@ -14829,11 +15879,19 @@
       <c r="O138" s="4"/>
       <c r="P138" s="4"/>
       <c r="Q138" s="2"/>
-      <c r="R138" s="2"/>
-      <c r="S138" s="2"/>
+      <c r="R138" s="2">
+        <v>35</v>
+      </c>
+      <c r="S138" s="2">
+        <v>51</v>
+      </c>
       <c r="T138" s="2"/>
-      <c r="U138" s="2"/>
-      <c r="V138" s="2"/>
+      <c r="U138" s="2">
+        <v>86</v>
+      </c>
+      <c r="V138" s="2">
+        <v>159</v>
+      </c>
       <c r="W138" s="2"/>
       <c r="X138" s="4"/>
       <c r="Y138" s="4"/>
@@ -14924,7 +15982,7 @@
       <c r="BT138" s="2"/>
       <c r="BU138" s="2"/>
     </row>
-    <row r="139" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>90</v>
       </c>
@@ -14961,10 +16019,16 @@
       <c r="O139" s="4"/>
       <c r="P139" s="4"/>
       <c r="Q139" s="2"/>
-      <c r="R139" s="2"/>
-      <c r="S139" s="2"/>
+      <c r="R139" s="2">
+        <v>35</v>
+      </c>
+      <c r="S139" s="2">
+        <v>51</v>
+      </c>
       <c r="T139" s="2"/>
-      <c r="U139" s="2"/>
+      <c r="U139" s="2">
+        <v>86</v>
+      </c>
       <c r="V139" s="2">
         <v>159</v>
       </c>
@@ -15020,7 +16084,7 @@
       <c r="BT139" s="2"/>
       <c r="BU139" s="2"/>
     </row>
-    <row r="140" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>90</v>
       </c>
@@ -15050,11 +16114,19 @@
       <c r="O140" s="4"/>
       <c r="P140" s="4"/>
       <c r="Q140" s="2"/>
-      <c r="R140" s="2"/>
-      <c r="S140" s="2"/>
+      <c r="R140" s="2">
+        <v>35</v>
+      </c>
+      <c r="S140" s="2">
+        <v>51</v>
+      </c>
       <c r="T140" s="2"/>
-      <c r="U140" s="2"/>
-      <c r="V140" s="2"/>
+      <c r="U140" s="2">
+        <v>86</v>
+      </c>
+      <c r="V140" s="2">
+        <v>159</v>
+      </c>
       <c r="W140" s="2"/>
       <c r="X140" s="4"/>
       <c r="Y140" s="4"/>
@@ -15111,7 +16183,7 @@
       <c r="BT140" s="2"/>
       <c r="BU140" s="2"/>
     </row>
-    <row r="141" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>90</v>
       </c>
@@ -15141,11 +16213,19 @@
       <c r="O141" s="4"/>
       <c r="P141" s="4"/>
       <c r="Q141" s="2"/>
-      <c r="R141" s="2"/>
-      <c r="S141" s="2"/>
+      <c r="R141" s="2">
+        <v>35</v>
+      </c>
+      <c r="S141" s="2">
+        <v>51</v>
+      </c>
       <c r="T141" s="2"/>
-      <c r="U141" s="2"/>
-      <c r="V141" s="2"/>
+      <c r="U141" s="2">
+        <v>86</v>
+      </c>
+      <c r="V141" s="2">
+        <v>159</v>
+      </c>
       <c r="W141" s="2"/>
       <c r="X141" s="4"/>
       <c r="Y141" s="4"/>
@@ -15202,7 +16282,7 @@
       <c r="BT141" s="2"/>
       <c r="BU141" s="2"/>
     </row>
-    <row r="142" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>90</v>
       </c>
@@ -15239,11 +16319,19 @@
       <c r="O142" s="4"/>
       <c r="P142" s="4"/>
       <c r="Q142" s="2"/>
-      <c r="R142" s="2"/>
-      <c r="S142" s="2"/>
+      <c r="R142" s="2">
+        <v>35</v>
+      </c>
+      <c r="S142" s="2">
+        <v>51</v>
+      </c>
       <c r="T142" s="2"/>
-      <c r="U142" s="2"/>
-      <c r="V142" s="2"/>
+      <c r="U142" s="2">
+        <v>86</v>
+      </c>
+      <c r="V142" s="2">
+        <v>159</v>
+      </c>
       <c r="W142" s="2"/>
       <c r="X142" s="4"/>
       <c r="Y142" s="4"/>

</xml_diff>

<commit_message>
Cotton - Inconsistent capitalisation between observed files
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FEFF5B-E4A5-4B7F-AAA9-B69F81F2F839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D430014C-BF33-4285-B5C9-17135222526F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FBA18FA7-8D49-4A23-B648-57CB41343816}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FBA18FA7-8D49-4A23-B648-57CB41343816}"/>
   </bookViews>
   <sheets>
     <sheet name="CottonObserved" sheetId="1" r:id="rId1"/>
@@ -170,9 +170,6 @@
     <t>dw_OB</t>
   </si>
   <si>
-    <t>Cotton.Fruit.Nconc</t>
-  </si>
-  <si>
     <t>Cotton.Fruit.N</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>Cotton.Leaf.SpecificAreaCanopy</t>
+  </si>
+  <si>
+    <t>Cotton.Fruit.NConc</t>
   </si>
 </sst>
 </file>
@@ -682,149 +682,149 @@
   <dimension ref="A1:BU142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI2" sqref="AI2"/>
+      <selection pane="bottomRight" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="34" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="33" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="30" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="31.59765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.86328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="21" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.1328125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="17" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="24" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.3984375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="25.73046875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="26.73046875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="6.73046875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="4.265625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="31.3984375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="32" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="9" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="10" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="6.265625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="12" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="10.265625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="12" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="16.73046875" bestFit="1" customWidth="1"/>
-    <col min="76" max="77" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="77" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="22" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="12" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="22" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="12" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="22" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="86" max="86" width="12" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="22" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="12" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="22" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="12" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="22" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="22" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="12" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="22" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="12" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="22" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="12" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="23" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="13" bestFit="1" customWidth="1"/>
     <col min="108" max="108" width="23" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="13" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="23" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="113" max="113" width="13" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="131" max="131" width="7" bestFit="1" customWidth="1"/>
     <col min="132" max="139" width="18" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="5.86328125" bestFit="1" customWidth="1"/>
-    <col min="141" max="148" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="141" max="148" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -928,7 +928,7 @@
         <v>33</v>
       </c>
       <c r="AI1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AJ1" t="s">
         <v>34</v>
@@ -958,96 +958,96 @@
         <v>42</v>
       </c>
       <c r="AS1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AT1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AU1" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>52</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>54</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>55</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>56</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>57</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>58</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>59</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>60</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>61</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>62</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>63</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>64</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>65</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>66</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>67</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>68</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>69</v>
       </c>
-      <c r="BU1" t="s">
-        <v>70</v>
-      </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="1">
         <v>39783</v>
@@ -1056,16 +1056,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
         <v>71</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
         <v>72</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>73</v>
       </c>
       <c r="I2" s="3">
         <v>8.3000000000000007</v>
@@ -1157,9 +1157,9 @@
       <c r="BT2" s="2"/>
       <c r="BU2" s="2"/>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="1">
         <v>39798</v>
@@ -1170,7 +1170,7 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I3" s="3">
         <v>8.3000000000000007</v>
@@ -1246,9 +1246,9 @@
       <c r="BT3" s="2"/>
       <c r="BU3" s="2"/>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1">
         <v>39804</v>
@@ -1257,16 +1257,16 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" t="s">
         <v>74</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
       </c>
       <c r="G4">
         <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I4" s="3">
         <v>8.3000000000000007</v>
@@ -1342,9 +1342,9 @@
       <c r="BT4" s="2"/>
       <c r="BU4" s="2"/>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1">
         <v>39806</v>
@@ -1355,7 +1355,7 @@
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I5" s="3">
         <v>8.3000000000000007</v>
@@ -1431,9 +1431,9 @@
       <c r="BT5" s="2"/>
       <c r="BU5" s="2"/>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1">
         <v>39813</v>
@@ -1444,7 +1444,7 @@
         <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I6" s="3">
         <v>8.3000000000000007</v>
@@ -1520,9 +1520,9 @@
       <c r="BT6" s="2"/>
       <c r="BU6" s="2"/>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="1">
         <v>39818</v>
@@ -1533,7 +1533,7 @@
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I7" s="3">
         <v>8.3000000000000007</v>
@@ -1641,9 +1641,9 @@
       <c r="BT7" s="2"/>
       <c r="BU7" s="2"/>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1">
         <v>39819</v>
@@ -1654,7 +1654,7 @@
         <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I8" s="3">
         <v>8.3000000000000007</v>
@@ -1730,9 +1730,9 @@
       <c r="BT8" s="2"/>
       <c r="BU8" s="2"/>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="1">
         <v>39825</v>
@@ -1741,16 +1741,16 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
         <v>76</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
       </c>
       <c r="G9">
         <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="3">
         <v>8.3000000000000007</v>
@@ -1864,9 +1864,9 @@
       <c r="BT9" s="2"/>
       <c r="BU9" s="2"/>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1">
         <v>39827</v>
@@ -1877,7 +1877,7 @@
         <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I10" s="3">
         <v>8.3000000000000007</v>
@@ -1953,9 +1953,9 @@
       <c r="BT10" s="2"/>
       <c r="BU10" s="2"/>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="1">
         <v>39833</v>
@@ -1966,7 +1966,7 @@
         <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I11" s="3">
         <v>8.3000000000000007</v>
@@ -2042,9 +2042,9 @@
       <c r="BT11" s="2"/>
       <c r="BU11" s="2"/>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1">
         <v>39840</v>
@@ -2055,7 +2055,7 @@
         <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I12" s="3">
         <v>8.3000000000000007</v>
@@ -2131,9 +2131,9 @@
       <c r="BT12" s="2"/>
       <c r="BU12" s="2"/>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1">
         <v>39841</v>
@@ -2144,7 +2144,7 @@
         <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I13" s="3">
         <v>8.3000000000000007</v>
@@ -2256,9 +2256,9 @@
       <c r="BT13" s="2"/>
       <c r="BU13" s="2"/>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="1">
         <v>39848</v>
@@ -2269,7 +2269,7 @@
         <v>65</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I14" s="3">
         <v>8.3000000000000007</v>
@@ -2345,9 +2345,9 @@
       <c r="BT14" s="2"/>
       <c r="BU14" s="2"/>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="1">
         <v>39853</v>
@@ -2356,16 +2356,16 @@
         <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" t="s">
         <v>78</v>
-      </c>
-      <c r="F15" t="s">
-        <v>79</v>
       </c>
       <c r="G15">
         <v>70</v>
       </c>
       <c r="H15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I15" s="3">
         <v>8.3000000000000007</v>
@@ -2477,9 +2477,9 @@
       <c r="BT15" s="2"/>
       <c r="BU15" s="2"/>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="1">
         <v>39854</v>
@@ -2490,7 +2490,7 @@
         <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I16" s="3">
         <v>8.3000000000000007</v>
@@ -2566,9 +2566,9 @@
       <c r="BT16" s="2"/>
       <c r="BU16" s="2"/>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" s="1">
         <v>39860</v>
@@ -2579,7 +2579,7 @@
         <v>77</v>
       </c>
       <c r="H17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I17" s="3">
         <v>8.3000000000000007</v>
@@ -2655,9 +2655,9 @@
       <c r="BT17" s="2"/>
       <c r="BU17" s="2"/>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1">
         <v>39874</v>
@@ -2668,7 +2668,7 @@
         <v>91</v>
       </c>
       <c r="H18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I18" s="3">
         <v>8.3000000000000007</v>
@@ -2744,9 +2744,9 @@
       <c r="BT18" s="2"/>
       <c r="BU18" s="2"/>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="1">
         <v>39875</v>
@@ -2757,7 +2757,7 @@
         <v>92</v>
       </c>
       <c r="H19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I19" s="3">
         <v>8.3000000000000007</v>
@@ -2869,9 +2869,9 @@
       <c r="BT19" s="2"/>
       <c r="BU19" s="2"/>
     </row>
-    <row r="20" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="1">
         <v>39877</v>
@@ -2880,16 +2880,16 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" t="s">
         <v>80</v>
-      </c>
-      <c r="F20" t="s">
-        <v>81</v>
       </c>
       <c r="G20">
         <v>94</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I20" s="3">
         <v>8.3000000000000007</v>
@@ -2965,9 +2965,9 @@
       <c r="BT20" s="2"/>
       <c r="BU20" s="2"/>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="1">
         <v>39884</v>
@@ -2978,7 +2978,7 @@
         <v>101</v>
       </c>
       <c r="H21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I21" s="3">
         <v>8.3000000000000007</v>
@@ -3054,9 +3054,9 @@
       <c r="BT21" s="2"/>
       <c r="BU21" s="2"/>
     </row>
-    <row r="22" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="1">
         <v>39889</v>
@@ -3067,7 +3067,7 @@
         <v>106</v>
       </c>
       <c r="H22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I22" s="3">
         <v>8.3000000000000007</v>
@@ -3179,9 +3179,9 @@
       <c r="BT22" s="2"/>
       <c r="BU22" s="2"/>
     </row>
-    <row r="23" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" s="1">
         <v>39895</v>
@@ -3192,7 +3192,7 @@
         <v>112</v>
       </c>
       <c r="H23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I23" s="3">
         <v>8.3000000000000007</v>
@@ -3268,9 +3268,9 @@
       <c r="BT23" s="2"/>
       <c r="BU23" s="2"/>
     </row>
-    <row r="24" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="1">
         <v>39904</v>
@@ -3281,7 +3281,7 @@
         <v>121</v>
       </c>
       <c r="H24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I24" s="3">
         <v>8.3000000000000007</v>
@@ -3359,9 +3359,9 @@
       <c r="BT24" s="2"/>
       <c r="BU24" s="2"/>
     </row>
-    <row r="25" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" s="1">
         <v>39910</v>
@@ -3372,7 +3372,7 @@
         <v>127</v>
       </c>
       <c r="H25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I25" s="3">
         <v>8.3000000000000007</v>
@@ -3484,9 +3484,9 @@
       <c r="BT25" s="2"/>
       <c r="BU25" s="2"/>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="1">
         <v>39911</v>
@@ -3497,7 +3497,7 @@
         <v>128</v>
       </c>
       <c r="H26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I26" s="3">
         <v>8.3000000000000007</v>
@@ -3575,9 +3575,9 @@
       <c r="BT26" s="2"/>
       <c r="BU26" s="2"/>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="1">
         <v>39920</v>
@@ -3588,7 +3588,7 @@
         <v>137</v>
       </c>
       <c r="H27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I27" s="3">
         <v>8.3000000000000007</v>
@@ -3666,9 +3666,9 @@
       <c r="BT27" s="2"/>
       <c r="BU27" s="2"/>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" s="1">
         <v>39925</v>
@@ -3679,7 +3679,7 @@
         <v>142</v>
       </c>
       <c r="H28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I28" s="3">
         <v>8.3000000000000007</v>
@@ -3757,9 +3757,9 @@
       <c r="BT28" s="2"/>
       <c r="BU28" s="2"/>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1">
         <v>39932</v>
@@ -3770,7 +3770,7 @@
         <v>149</v>
       </c>
       <c r="H29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I29" s="3">
         <v>8.3000000000000007</v>
@@ -3848,9 +3848,9 @@
       <c r="BT29" s="2"/>
       <c r="BU29" s="2"/>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="1">
         <v>39939</v>
@@ -3861,7 +3861,7 @@
         <v>156</v>
       </c>
       <c r="H30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I30" s="3">
         <v>8.3000000000000007</v>
@@ -3939,9 +3939,9 @@
       <c r="BT30" s="2"/>
       <c r="BU30" s="2"/>
     </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" s="1">
         <v>39946</v>
@@ -3952,7 +3952,7 @@
         <v>163</v>
       </c>
       <c r="H31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I31" s="3">
         <v>8.3000000000000007</v>
@@ -4030,9 +4030,9 @@
       <c r="BT31" s="2"/>
       <c r="BU31" s="2"/>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" s="1">
         <v>39947</v>
@@ -4041,16 +4041,16 @@
         <v>9</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" t="s">
         <v>82</v>
-      </c>
-      <c r="F32" t="s">
-        <v>83</v>
       </c>
       <c r="G32">
         <v>164</v>
       </c>
       <c r="H32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I32" s="3">
         <v>8.3000000000000007</v>
@@ -4126,9 +4126,9 @@
       <c r="BT32" s="2"/>
       <c r="BU32" s="2"/>
     </row>
-    <row r="33" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C33" s="1">
         <v>39954</v>
@@ -4139,7 +4139,7 @@
         <v>171</v>
       </c>
       <c r="H33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I33" s="3">
         <v>8.3000000000000007</v>
@@ -4217,9 +4217,9 @@
       <c r="BT33" s="2"/>
       <c r="BU33" s="2"/>
     </row>
-    <row r="34" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C34" s="1">
         <v>39957</v>
@@ -4228,16 +4228,16 @@
         <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" t="s">
         <v>84</v>
-      </c>
-      <c r="F34" t="s">
-        <v>85</v>
       </c>
       <c r="G34">
         <v>174</v>
       </c>
       <c r="H34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I34" s="3">
         <v>8.3000000000000007</v>
@@ -4319,9 +4319,9 @@
       <c r="BT34" s="2"/>
       <c r="BU34" s="2"/>
     </row>
-    <row r="35" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C35" s="1">
         <v>39960</v>
@@ -4332,7 +4332,7 @@
         <v>177</v>
       </c>
       <c r="H35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I35" s="3">
         <v>8.3000000000000007</v>
@@ -4410,9 +4410,9 @@
       <c r="BT35" s="2"/>
       <c r="BU35" s="2"/>
     </row>
-    <row r="36" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C36" s="1">
         <v>39801</v>
@@ -4421,16 +4421,16 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" t="s">
         <v>71</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="H36" t="s">
         <v>72</v>
-      </c>
-      <c r="G36" s="2">
-        <v>0</v>
-      </c>
-      <c r="H36" t="s">
-        <v>73</v>
       </c>
       <c r="I36" s="3">
         <v>8.1</v>
@@ -4522,9 +4522,9 @@
       <c r="BT36" s="2"/>
       <c r="BU36" s="2"/>
     </row>
-    <row r="37" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37" s="1">
         <v>39819</v>
@@ -4535,7 +4535,7 @@
         <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I37" s="3">
         <v>8.1</v>
@@ -4611,9 +4611,9 @@
       <c r="BT37" s="2"/>
       <c r="BU37" s="2"/>
     </row>
-    <row r="38" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" s="1">
         <v>39820</v>
@@ -4624,7 +4624,7 @@
         <v>19</v>
       </c>
       <c r="H38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I38" s="3">
         <v>8.1</v>
@@ -4718,9 +4718,9 @@
       <c r="BT38" s="2"/>
       <c r="BU38" s="2"/>
     </row>
-    <row r="39" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" s="1">
         <v>39824</v>
@@ -4729,16 +4729,16 @@
         <v>4</v>
       </c>
       <c r="E39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" t="s">
         <v>74</v>
-      </c>
-      <c r="F39" t="s">
-        <v>75</v>
       </c>
       <c r="G39">
         <v>23</v>
       </c>
       <c r="H39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I39" s="3">
         <v>8.1</v>
@@ -4814,9 +4814,9 @@
       <c r="BT39" s="2"/>
       <c r="BU39" s="2"/>
     </row>
-    <row r="40" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" s="1">
         <v>39827</v>
@@ -4827,7 +4827,7 @@
         <v>26</v>
       </c>
       <c r="H40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I40" s="3">
         <v>8.1</v>
@@ -4903,9 +4903,9 @@
       <c r="BT40" s="2"/>
       <c r="BU40" s="2"/>
     </row>
-    <row r="41" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C41" s="1">
         <v>39833</v>
@@ -4916,7 +4916,7 @@
         <v>32</v>
       </c>
       <c r="H41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I41" s="3">
         <v>8.1</v>
@@ -5026,9 +5026,9 @@
       <c r="BT41" s="2"/>
       <c r="BU41" s="2"/>
     </row>
-    <row r="42" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C42" s="1">
         <v>39840</v>
@@ -5039,7 +5039,7 @@
         <v>39</v>
       </c>
       <c r="H42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I42" s="3">
         <v>8.1</v>
@@ -5115,9 +5115,9 @@
       <c r="BT42" s="2"/>
       <c r="BU42" s="2"/>
     </row>
-    <row r="43" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C43" s="1">
         <v>39848</v>
@@ -5128,7 +5128,7 @@
         <v>47</v>
       </c>
       <c r="H43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I43" s="3">
         <v>8.1</v>
@@ -5242,9 +5242,9 @@
       <c r="BT43" s="2"/>
       <c r="BU43" s="2"/>
     </row>
-    <row r="44" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C44" s="1">
         <v>39849</v>
@@ -5253,16 +5253,16 @@
         <v>4</v>
       </c>
       <c r="E44" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44" t="s">
         <v>76</v>
-      </c>
-      <c r="F44" t="s">
-        <v>77</v>
       </c>
       <c r="G44">
         <v>48</v>
       </c>
       <c r="H44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I44" s="3">
         <v>8.1</v>
@@ -5338,9 +5338,9 @@
       <c r="BT44" s="2"/>
       <c r="BU44" s="2"/>
     </row>
-    <row r="45" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C45" s="1">
         <v>39854</v>
@@ -5351,7 +5351,7 @@
         <v>53</v>
       </c>
       <c r="H45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I45" s="3">
         <v>8.1</v>
@@ -5427,9 +5427,9 @@
       <c r="BT45" s="2"/>
       <c r="BU45" s="2"/>
     </row>
-    <row r="46" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" s="1">
         <v>39860</v>
@@ -5438,16 +5438,16 @@
         <v>6</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" t="s">
         <v>78</v>
-      </c>
-      <c r="F46" t="s">
-        <v>79</v>
       </c>
       <c r="G46" s="2">
         <v>59</v>
       </c>
       <c r="H46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I46" s="3">
         <v>8.1</v>
@@ -5561,9 +5561,9 @@
       <c r="BT46" s="2"/>
       <c r="BU46" s="2"/>
     </row>
-    <row r="47" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C47" s="1">
         <v>39869</v>
@@ -5574,7 +5574,7 @@
         <v>68</v>
       </c>
       <c r="H47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I47" s="3">
         <v>8.1</v>
@@ -5650,9 +5650,9 @@
       <c r="BT47" s="2"/>
       <c r="BU47" s="2"/>
     </row>
-    <row r="48" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C48" s="1">
         <v>39874</v>
@@ -5663,7 +5663,7 @@
         <v>73</v>
       </c>
       <c r="H48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I48" s="3">
         <v>8.1</v>
@@ -5739,9 +5739,9 @@
       <c r="BT48" s="2"/>
       <c r="BU48" s="2"/>
     </row>
-    <row r="49" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C49" s="1">
         <v>39876</v>
@@ -5752,7 +5752,7 @@
         <v>75</v>
       </c>
       <c r="H49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I49" s="3">
         <v>8.1</v>
@@ -5864,9 +5864,9 @@
       <c r="BT49" s="2"/>
       <c r="BU49" s="2"/>
     </row>
-    <row r="50" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="1">
         <v>39884</v>
@@ -5877,7 +5877,7 @@
         <v>83</v>
       </c>
       <c r="H50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I50" s="3">
         <v>8.1</v>
@@ -5953,9 +5953,9 @@
       <c r="BT50" s="2"/>
       <c r="BU50" s="2"/>
     </row>
-    <row r="51" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C51" s="1">
         <v>39888</v>
@@ -5966,7 +5966,7 @@
         <v>87</v>
       </c>
       <c r="H51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I51" s="3">
         <v>8.1</v>
@@ -6078,9 +6078,9 @@
       <c r="BT51" s="2"/>
       <c r="BU51" s="2"/>
     </row>
-    <row r="52" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C52" s="1">
         <v>39895</v>
@@ -6091,7 +6091,7 @@
         <v>94</v>
       </c>
       <c r="H52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I52" s="3">
         <v>8.1</v>
@@ -6167,9 +6167,9 @@
       <c r="BT52" s="2"/>
       <c r="BU52" s="2"/>
     </row>
-    <row r="53" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C53" s="1">
         <v>39904</v>
@@ -6180,7 +6180,7 @@
         <v>103</v>
       </c>
       <c r="H53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I53" s="3">
         <v>8.1</v>
@@ -6292,9 +6292,9 @@
       <c r="BT53" s="2"/>
       <c r="BU53" s="2"/>
     </row>
-    <row r="54" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C54" s="1">
         <v>39908</v>
@@ -6305,7 +6305,7 @@
         <v>107</v>
       </c>
       <c r="H54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I54" s="3">
         <v>8.1</v>
@@ -6381,9 +6381,9 @@
       <c r="BT54" s="2"/>
       <c r="BU54" s="2"/>
     </row>
-    <row r="55" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C55" s="1">
         <v>39911</v>
@@ -6394,7 +6394,7 @@
         <v>110</v>
       </c>
       <c r="H55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I55" s="3">
         <v>8.1</v>
@@ -6472,9 +6472,9 @@
       <c r="BT55" s="2"/>
       <c r="BU55" s="2"/>
     </row>
-    <row r="56" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C56" s="1">
         <v>39920</v>
@@ -6485,7 +6485,7 @@
         <v>119</v>
       </c>
       <c r="H56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I56" s="3">
         <v>8.1</v>
@@ -6563,9 +6563,9 @@
       <c r="BT56" s="2"/>
       <c r="BU56" s="2"/>
     </row>
-    <row r="57" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C57" s="1">
         <v>39922</v>
@@ -6574,16 +6574,16 @@
         <v>8</v>
       </c>
       <c r="E57" t="s">
+        <v>79</v>
+      </c>
+      <c r="F57" t="s">
         <v>80</v>
-      </c>
-      <c r="F57" t="s">
-        <v>81</v>
       </c>
       <c r="G57">
         <v>121</v>
       </c>
       <c r="H57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I57" s="3">
         <v>8.1</v>
@@ -6659,9 +6659,9 @@
       <c r="BT57" s="2"/>
       <c r="BU57" s="2"/>
     </row>
-    <row r="58" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C58" s="1">
         <v>39925</v>
@@ -6672,7 +6672,7 @@
         <v>124</v>
       </c>
       <c r="H58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I58" s="3">
         <v>8.1</v>
@@ -6750,9 +6750,9 @@
       <c r="BT58" s="2"/>
       <c r="BU58" s="2"/>
     </row>
-    <row r="59" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C59" s="1">
         <v>39932</v>
@@ -6763,7 +6763,7 @@
         <v>131</v>
       </c>
       <c r="H59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I59" s="3">
         <v>8.1</v>
@@ -6879,9 +6879,9 @@
       <c r="BT59" s="2"/>
       <c r="BU59" s="2"/>
     </row>
-    <row r="60" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C60" s="1">
         <v>39939</v>
@@ -6892,7 +6892,7 @@
         <v>138</v>
       </c>
       <c r="H60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I60" s="3">
         <v>8.1</v>
@@ -6970,9 +6970,9 @@
       <c r="BT60" s="2"/>
       <c r="BU60" s="2"/>
     </row>
-    <row r="61" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C61" s="1">
         <v>39945</v>
@@ -6981,16 +6981,16 @@
         <v>9</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F61" t="s">
         <v>82</v>
-      </c>
-      <c r="F61" t="s">
-        <v>83</v>
       </c>
       <c r="G61">
         <v>144</v>
       </c>
       <c r="H61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I61" s="3">
         <v>8.1</v>
@@ -7066,9 +7066,9 @@
       <c r="BT61" s="2"/>
       <c r="BU61" s="2"/>
     </row>
-    <row r="62" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C62" s="1">
         <v>39946</v>
@@ -7079,7 +7079,7 @@
         <v>145</v>
       </c>
       <c r="H62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I62" s="3">
         <v>8.1</v>
@@ -7157,9 +7157,9 @@
       <c r="BT62" s="2"/>
       <c r="BU62" s="2"/>
     </row>
-    <row r="63" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C63" s="1">
         <v>39954</v>
@@ -7170,7 +7170,7 @@
         <v>153</v>
       </c>
       <c r="H63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I63" s="3">
         <v>8.1</v>
@@ -7248,9 +7248,9 @@
       <c r="BT63" s="2"/>
       <c r="BU63" s="2"/>
     </row>
-    <row r="64" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C64" s="1">
         <v>39960</v>
@@ -7259,16 +7259,16 @@
         <v>10</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F64" t="s">
         <v>84</v>
-      </c>
-      <c r="F64" t="s">
-        <v>85</v>
       </c>
       <c r="G64">
         <v>159</v>
       </c>
       <c r="H64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I64" s="3">
         <v>8.1</v>
@@ -7354,9 +7354,9 @@
       <c r="BT64" s="2"/>
       <c r="BU64" s="2"/>
     </row>
-    <row r="65" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C65" s="1">
         <v>39820</v>
@@ -7365,16 +7365,16 @@
         <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F65" t="s">
         <v>71</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" s="2">
+        <v>0</v>
+      </c>
+      <c r="H65" t="s">
         <v>72</v>
-      </c>
-      <c r="G65" s="2">
-        <v>0</v>
-      </c>
-      <c r="H65" t="s">
-        <v>73</v>
       </c>
       <c r="I65" s="3">
         <v>8.3000000000000007</v>
@@ -7466,9 +7466,9 @@
       <c r="BT65" s="2"/>
       <c r="BU65" s="2"/>
     </row>
-    <row r="66" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C66" s="1">
         <v>39846</v>
@@ -7477,16 +7477,16 @@
         <v>4</v>
       </c>
       <c r="E66" t="s">
+        <v>73</v>
+      </c>
+      <c r="F66" t="s">
         <v>74</v>
-      </c>
-      <c r="F66" t="s">
-        <v>75</v>
       </c>
       <c r="G66">
         <v>26</v>
       </c>
       <c r="H66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I66" s="3">
         <v>8.3000000000000007</v>
@@ -7580,9 +7580,9 @@
       <c r="BT66" s="2"/>
       <c r="BU66" s="2"/>
     </row>
-    <row r="67" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C67" s="1">
         <v>39848</v>
@@ -7593,7 +7593,7 @@
         <v>28</v>
       </c>
       <c r="H67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I67" s="3">
         <v>8.3000000000000007</v>
@@ -7669,9 +7669,9 @@
       <c r="BT67" s="2"/>
       <c r="BU67" s="2"/>
     </row>
-    <row r="68" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C68" s="1">
         <v>39854</v>
@@ -7682,7 +7682,7 @@
         <v>34</v>
       </c>
       <c r="H68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I68" s="3">
         <v>8.3000000000000007</v>
@@ -7758,9 +7758,9 @@
       <c r="BT68" s="2"/>
       <c r="BU68" s="2"/>
     </row>
-    <row r="69" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C69" s="1">
         <v>39860</v>
@@ -7771,7 +7771,7 @@
         <v>40</v>
       </c>
       <c r="H69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I69" s="3">
         <v>8.3000000000000007</v>
@@ -7847,9 +7847,9 @@
       <c r="BT69" s="2"/>
       <c r="BU69" s="2"/>
     </row>
-    <row r="70" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C70" s="1">
         <v>39864</v>
@@ -7860,7 +7860,7 @@
         <v>44</v>
       </c>
       <c r="H70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I70" s="3">
         <v>8.3000000000000007</v>
@@ -7954,9 +7954,9 @@
       <c r="BT70" s="2"/>
       <c r="BU70" s="2"/>
     </row>
-    <row r="71" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C71" s="1">
         <v>39869</v>
@@ -7967,7 +7967,7 @@
         <v>49</v>
       </c>
       <c r="H71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I71" s="3">
         <v>8.3000000000000007</v>
@@ -8043,9 +8043,9 @@
       <c r="BT71" s="2"/>
       <c r="BU71" s="2"/>
     </row>
-    <row r="72" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C72" s="1">
         <v>39874</v>
@@ -8056,7 +8056,7 @@
         <v>54</v>
       </c>
       <c r="H72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I72" s="3">
         <v>8.3000000000000007</v>
@@ -8169,9 +8169,9 @@
       <c r="BT72" s="2"/>
       <c r="BU72" s="2"/>
     </row>
-    <row r="73" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C73" s="1">
         <v>39877</v>
@@ -8180,16 +8180,16 @@
         <v>4</v>
       </c>
       <c r="E73" t="s">
+        <v>75</v>
+      </c>
+      <c r="F73" t="s">
         <v>76</v>
-      </c>
-      <c r="F73" t="s">
-        <v>77</v>
       </c>
       <c r="G73">
         <v>57</v>
       </c>
       <c r="H73" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I73" s="3">
         <v>8.3000000000000007</v>
@@ -8265,9 +8265,9 @@
       <c r="BT73" s="2"/>
       <c r="BU73" s="2"/>
     </row>
-    <row r="74" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C74" s="1">
         <v>39884</v>
@@ -8278,7 +8278,7 @@
         <v>64</v>
       </c>
       <c r="H74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I74" s="3">
         <v>8.3000000000000007</v>
@@ -8354,9 +8354,9 @@
       <c r="BT74" s="2"/>
       <c r="BU74" s="2"/>
     </row>
-    <row r="75" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C75" s="1">
         <v>39890</v>
@@ -8367,7 +8367,7 @@
         <v>70</v>
       </c>
       <c r="H75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I75" s="3">
         <v>8.3000000000000007</v>
@@ -8481,9 +8481,9 @@
       <c r="BT75" s="2"/>
       <c r="BU75" s="2"/>
     </row>
-    <row r="76" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C76" s="1">
         <v>39895</v>
@@ -8494,7 +8494,7 @@
         <v>75</v>
       </c>
       <c r="H76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I76" s="3">
         <v>8.3000000000000007</v>
@@ -8570,9 +8570,9 @@
       <c r="BT76" s="2"/>
       <c r="BU76" s="2"/>
     </row>
-    <row r="77" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C77" s="1">
         <v>39903</v>
@@ -8581,16 +8581,16 @@
         <v>6</v>
       </c>
       <c r="E77" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F77" t="s">
         <v>78</v>
-      </c>
-      <c r="F77" t="s">
-        <v>79</v>
       </c>
       <c r="G77">
         <v>83</v>
       </c>
       <c r="H77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I77" s="3">
         <v>8.3000000000000007</v>
@@ -8704,9 +8704,9 @@
       <c r="BT77" s="2"/>
       <c r="BU77" s="2"/>
     </row>
-    <row r="78" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C78" s="1">
         <v>39911</v>
@@ -8717,7 +8717,7 @@
         <v>91</v>
       </c>
       <c r="H78" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I78" s="3">
         <v>8.3000000000000007</v>
@@ -8793,9 +8793,9 @@
       <c r="BT78" s="2"/>
       <c r="BU78" s="2"/>
     </row>
-    <row r="79" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C79" s="1">
         <v>39919</v>
@@ -8806,7 +8806,7 @@
         <v>99</v>
       </c>
       <c r="H79" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I79" s="3">
         <v>8.3000000000000007</v>
@@ -8918,9 +8918,9 @@
       <c r="BT79" s="2"/>
       <c r="BU79" s="2"/>
     </row>
-    <row r="80" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C80" s="1">
         <v>39928</v>
@@ -8931,7 +8931,7 @@
         <v>108</v>
       </c>
       <c r="H80" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I80" s="3">
         <v>8.3000000000000007</v>
@@ -9007,9 +9007,9 @@
       <c r="BT80" s="2"/>
       <c r="BU80" s="2"/>
     </row>
-    <row r="81" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C81" s="1">
         <v>39938</v>
@@ -9018,16 +9018,16 @@
         <v>8</v>
       </c>
       <c r="E81" t="s">
+        <v>79</v>
+      </c>
+      <c r="F81" t="s">
         <v>80</v>
-      </c>
-      <c r="F81" t="s">
-        <v>81</v>
       </c>
       <c r="G81">
         <v>118</v>
       </c>
       <c r="H81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I81" s="3">
         <v>8.3000000000000007</v>
@@ -9141,9 +9141,9 @@
       <c r="BT81" s="2"/>
       <c r="BU81" s="2"/>
     </row>
-    <row r="82" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C82" s="1">
         <v>39954</v>
@@ -9154,7 +9154,7 @@
         <v>134</v>
       </c>
       <c r="H82" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I82" s="3">
         <v>8.3000000000000007</v>
@@ -9232,9 +9232,9 @@
       <c r="BT82" s="2"/>
       <c r="BU82" s="2"/>
     </row>
-    <row r="83" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C83" s="1">
         <v>39960</v>
@@ -9245,7 +9245,7 @@
         <v>140</v>
       </c>
       <c r="H83" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I83" s="3">
         <v>8.3000000000000007</v>
@@ -9323,9 +9323,9 @@
       <c r="BT83" s="2"/>
       <c r="BU83" s="2"/>
     </row>
-    <row r="84" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C84" s="1">
         <v>39966</v>
@@ -9336,7 +9336,7 @@
         <v>146</v>
       </c>
       <c r="H84" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I84" s="3">
         <v>8.3000000000000007</v>
@@ -9448,9 +9448,9 @@
       <c r="BT84" s="2"/>
       <c r="BU84" s="2"/>
     </row>
-    <row r="85" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C85" s="1">
         <v>39969</v>
@@ -9461,7 +9461,7 @@
         <v>149</v>
       </c>
       <c r="H85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I85" s="3">
         <v>8.3000000000000007</v>
@@ -9539,9 +9539,9 @@
       <c r="BT85" s="2"/>
       <c r="BU85" s="2"/>
     </row>
-    <row r="86" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C86" s="1">
         <v>39974</v>
@@ -9550,16 +9550,16 @@
         <v>9</v>
       </c>
       <c r="E86" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F86" t="s">
         <v>82</v>
-      </c>
-      <c r="F86" t="s">
-        <v>83</v>
       </c>
       <c r="G86">
         <v>154</v>
       </c>
       <c r="H86" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I86" s="3">
         <v>8.3000000000000007</v>
@@ -9635,9 +9635,9 @@
       <c r="BT86" s="2"/>
       <c r="BU86" s="2"/>
     </row>
-    <row r="87" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C87" s="1">
         <v>39976</v>
@@ -9648,7 +9648,7 @@
         <v>156</v>
       </c>
       <c r="H87" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I87" s="3">
         <v>8.3000000000000007</v>
@@ -9726,9 +9726,9 @@
       <c r="BT87" s="2"/>
       <c r="BU87" s="2"/>
     </row>
-    <row r="88" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C88" s="1">
         <v>39983</v>
@@ -9739,7 +9739,7 @@
         <v>163</v>
       </c>
       <c r="H88" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I88" s="3">
         <v>8.3000000000000007</v>
@@ -9817,9 +9817,9 @@
       <c r="BT88" s="2"/>
       <c r="BU88" s="2"/>
     </row>
-    <row r="89" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C89" s="1">
         <v>39990</v>
@@ -9830,7 +9830,7 @@
         <v>170</v>
       </c>
       <c r="H89" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I89" s="3">
         <v>8.3000000000000007</v>
@@ -9908,9 +9908,9 @@
       <c r="BT89" s="2"/>
       <c r="BU89" s="2"/>
     </row>
-    <row r="90" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C90" s="1">
         <v>39994</v>
@@ -9919,16 +9919,16 @@
         <v>10</v>
       </c>
       <c r="E90" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F90" t="s">
         <v>84</v>
-      </c>
-      <c r="F90" t="s">
-        <v>85</v>
       </c>
       <c r="G90">
         <v>174</v>
       </c>
       <c r="H90" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I90" s="3">
         <v>8.3000000000000007</v>
@@ -10010,9 +10010,9 @@
       <c r="BT90" s="2"/>
       <c r="BU90" s="2"/>
     </row>
-    <row r="91" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C91" s="1">
         <v>39995</v>
@@ -10023,7 +10023,7 @@
         <v>175</v>
       </c>
       <c r="H91" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I91" s="3">
         <v>8.3000000000000007</v>
@@ -10101,9 +10101,9 @@
       <c r="BT91" s="2"/>
       <c r="BU91" s="2"/>
     </row>
-    <row r="92" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C92" s="1">
         <v>40895</v>
@@ -10112,16 +10112,16 @@
         <v>1</v>
       </c>
       <c r="E92" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F92" t="s">
         <v>71</v>
       </c>
-      <c r="F92" t="s">
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92" t="s">
         <v>72</v>
-      </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92" t="s">
-        <v>73</v>
       </c>
       <c r="I92" s="3">
         <v>8</v>
@@ -10213,9 +10213,9 @@
       <c r="BT92" s="2"/>
       <c r="BU92" s="2"/>
     </row>
-    <row r="93" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C93" s="1">
         <v>40924</v>
@@ -10224,16 +10224,16 @@
         <v>4</v>
       </c>
       <c r="E93" t="s">
+        <v>73</v>
+      </c>
+      <c r="F93" t="s">
         <v>74</v>
-      </c>
-      <c r="F93" t="s">
-        <v>75</v>
       </c>
       <c r="G93">
         <v>29</v>
       </c>
       <c r="H93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I93" s="3">
         <v>8</v>
@@ -10327,9 +10327,9 @@
       <c r="BT93" s="2"/>
       <c r="BU93" s="2"/>
     </row>
-    <row r="94" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C94" s="1">
         <v>40931</v>
@@ -10340,7 +10340,7 @@
         <v>36</v>
       </c>
       <c r="H94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I94" s="3">
         <v>8</v>
@@ -10416,9 +10416,9 @@
       <c r="BT94" s="2"/>
       <c r="BU94" s="2"/>
     </row>
-    <row r="95" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C95" s="1">
         <v>40938</v>
@@ -10429,7 +10429,7 @@
         <v>43</v>
       </c>
       <c r="H95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I95" s="3">
         <v>8</v>
@@ -10541,9 +10541,9 @@
       <c r="BT95" s="2"/>
       <c r="BU95" s="2"/>
     </row>
-    <row r="96" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C96" s="1">
         <v>40939</v>
@@ -10554,7 +10554,7 @@
         <v>44</v>
       </c>
       <c r="H96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I96" s="3">
         <v>8</v>
@@ -10630,9 +10630,9 @@
       <c r="BT96" s="2"/>
       <c r="BU96" s="2"/>
     </row>
-    <row r="97" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C97" s="1">
         <v>40945</v>
@@ -10641,16 +10641,16 @@
         <v>5</v>
       </c>
       <c r="E97" t="s">
+        <v>75</v>
+      </c>
+      <c r="F97" t="s">
         <v>76</v>
-      </c>
-      <c r="F97" t="s">
-        <v>77</v>
       </c>
       <c r="G97">
         <v>50</v>
       </c>
       <c r="H97" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I97" s="3">
         <v>8</v>
@@ -10764,9 +10764,9 @@
       <c r="BT97" s="2"/>
       <c r="BU97" s="2"/>
     </row>
-    <row r="98" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C98" s="1">
         <v>40948</v>
@@ -10777,7 +10777,7 @@
         <v>53</v>
       </c>
       <c r="H98" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I98" s="3">
         <v>8</v>
@@ -10853,9 +10853,9 @@
       <c r="BT98" s="2"/>
       <c r="BU98" s="2"/>
     </row>
-    <row r="99" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C99" s="1">
         <v>40954</v>
@@ -10866,7 +10866,7 @@
         <v>59</v>
       </c>
       <c r="H99" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I99" s="3">
         <v>8</v>
@@ -10942,9 +10942,9 @@
       <c r="BT99" s="2"/>
       <c r="BU99" s="2"/>
     </row>
-    <row r="100" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C100" s="1">
         <v>40959</v>
@@ -10955,7 +10955,7 @@
         <v>64</v>
       </c>
       <c r="H100" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I100" s="3">
         <v>8</v>
@@ -11067,9 +11067,9 @@
       <c r="BT100" s="2"/>
       <c r="BU100" s="2"/>
     </row>
-    <row r="101" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C101" s="1">
         <v>40960</v>
@@ -11080,7 +11080,7 @@
         <v>65</v>
       </c>
       <c r="H101" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I101" s="3">
         <v>8</v>
@@ -11156,9 +11156,9 @@
       <c r="BT101" s="2"/>
       <c r="BU101" s="2"/>
     </row>
-    <row r="102" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C102" s="1">
         <v>40970</v>
@@ -11169,7 +11169,7 @@
         <v>75</v>
       </c>
       <c r="H102" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I102" s="3">
         <v>8</v>
@@ -11245,9 +11245,9 @@
       <c r="BT102" s="2"/>
       <c r="BU102" s="2"/>
     </row>
-    <row r="103" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C103" s="1">
         <v>40976</v>
@@ -11258,7 +11258,7 @@
         <v>81</v>
       </c>
       <c r="H103" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I103" s="3">
         <v>8</v>
@@ -11334,9 +11334,9 @@
       <c r="BT103" s="2"/>
       <c r="BU103" s="2"/>
     </row>
-    <row r="104" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C104" s="1">
         <v>40980</v>
@@ -11345,16 +11345,16 @@
         <v>6</v>
       </c>
       <c r="E104" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F104" t="s">
         <v>78</v>
-      </c>
-      <c r="F104" t="s">
-        <v>79</v>
       </c>
       <c r="G104">
         <v>85</v>
       </c>
       <c r="H104" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I104" s="3">
         <v>8</v>
@@ -11466,9 +11466,9 @@
       <c r="BT104" s="2"/>
       <c r="BU104" s="2"/>
     </row>
-    <row r="105" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C105" s="1">
         <v>40982</v>
@@ -11479,7 +11479,7 @@
         <v>87</v>
       </c>
       <c r="H105" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I105" s="3">
         <v>8</v>
@@ -11555,9 +11555,9 @@
       <c r="BT105" s="2"/>
       <c r="BU105" s="2"/>
     </row>
-    <row r="106" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C106" s="1">
         <v>40997</v>
@@ -11566,16 +11566,16 @@
         <v>8</v>
       </c>
       <c r="E106" t="s">
+        <v>79</v>
+      </c>
+      <c r="F106" t="s">
         <v>80</v>
-      </c>
-      <c r="F106" t="s">
-        <v>81</v>
       </c>
       <c r="G106">
         <v>102</v>
       </c>
       <c r="H106" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I106" s="3">
         <v>8</v>
@@ -11689,9 +11689,9 @@
       <c r="BT106" s="2"/>
       <c r="BU106" s="2"/>
     </row>
-    <row r="107" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C107" s="1">
         <v>41001</v>
@@ -11702,7 +11702,7 @@
         <v>106</v>
       </c>
       <c r="H107" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I107" s="3">
         <v>8</v>
@@ -11778,9 +11778,9 @@
       <c r="BT107" s="2"/>
       <c r="BU107" s="2"/>
     </row>
-    <row r="108" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C108" s="1">
         <v>41009</v>
@@ -11791,7 +11791,7 @@
         <v>114</v>
       </c>
       <c r="H108" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I108" s="3">
         <v>8</v>
@@ -11869,9 +11869,9 @@
       <c r="BT108" s="2"/>
       <c r="BU108" s="2"/>
     </row>
-    <row r="109" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C109" s="1">
         <v>41018</v>
@@ -11882,7 +11882,7 @@
         <v>123</v>
       </c>
       <c r="H109" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I109" s="3">
         <v>8</v>
@@ -11960,9 +11960,9 @@
       <c r="BT109" s="2"/>
       <c r="BU109" s="2"/>
     </row>
-    <row r="110" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C110" s="1">
         <v>41025</v>
@@ -11971,16 +11971,16 @@
         <v>9</v>
       </c>
       <c r="E110" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F110" t="s">
         <v>82</v>
-      </c>
-      <c r="F110" t="s">
-        <v>83</v>
       </c>
       <c r="G110">
         <v>130</v>
       </c>
       <c r="H110" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I110" s="3">
         <v>8</v>
@@ -12060,9 +12060,9 @@
       <c r="BT110" s="2"/>
       <c r="BU110" s="2"/>
     </row>
-    <row r="111" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C111" s="1">
         <v>41032</v>
@@ -12073,7 +12073,7 @@
         <v>137</v>
       </c>
       <c r="H111" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I111" s="3">
         <v>8</v>
@@ -12151,9 +12151,9 @@
       <c r="BT111" s="2"/>
       <c r="BU111" s="2"/>
     </row>
-    <row r="112" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C112" s="1">
         <v>41038</v>
@@ -12164,7 +12164,7 @@
         <v>143</v>
       </c>
       <c r="H112" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I112" s="3">
         <v>8</v>
@@ -12276,9 +12276,9 @@
       <c r="BT112" s="2"/>
       <c r="BU112" s="2"/>
     </row>
-    <row r="113" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C113" s="1">
         <v>41039</v>
@@ -12289,7 +12289,7 @@
         <v>144</v>
       </c>
       <c r="H113" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I113" s="3">
         <v>8</v>
@@ -12367,9 +12367,9 @@
       <c r="BT113" s="2"/>
       <c r="BU113" s="2"/>
     </row>
-    <row r="114" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C114" s="1">
         <v>41043</v>
@@ -12380,7 +12380,7 @@
         <v>148</v>
       </c>
       <c r="H114" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I114" s="3">
         <v>8</v>
@@ -12458,9 +12458,9 @@
       <c r="BT114" s="2"/>
       <c r="BU114" s="2"/>
     </row>
-    <row r="115" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C115" s="1">
         <v>41050</v>
@@ -12471,7 +12471,7 @@
         <v>155</v>
       </c>
       <c r="H115" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I115" s="3">
         <v>8</v>
@@ -12549,9 +12549,9 @@
       <c r="BT115" s="2"/>
       <c r="BU115" s="2"/>
     </row>
-    <row r="116" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C116" s="1">
         <v>41057</v>
@@ -12562,7 +12562,7 @@
         <v>162</v>
       </c>
       <c r="H116" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I116" s="3">
         <v>8</v>
@@ -12640,9 +12640,9 @@
       <c r="BT116" s="2"/>
       <c r="BU116" s="2"/>
     </row>
-    <row r="117" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C117" s="1">
         <v>41065</v>
@@ -12651,16 +12651,16 @@
         <v>10</v>
       </c>
       <c r="E117" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F117" t="s">
         <v>84</v>
-      </c>
-      <c r="F117" t="s">
-        <v>85</v>
       </c>
       <c r="G117">
         <v>170</v>
       </c>
       <c r="H117" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I117" s="3">
         <v>8</v>
@@ -12742,9 +12742,9 @@
       <c r="BT117" s="2"/>
       <c r="BU117" s="2"/>
     </row>
-    <row r="118" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C118" s="1">
         <v>40912</v>
@@ -12753,16 +12753,16 @@
         <v>1</v>
       </c>
       <c r="E118" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F118" t="s">
         <v>71</v>
       </c>
-      <c r="F118" t="s">
+      <c r="G118">
+        <v>0</v>
+      </c>
+      <c r="H118" t="s">
         <v>72</v>
-      </c>
-      <c r="G118">
-        <v>0</v>
-      </c>
-      <c r="H118" t="s">
-        <v>73</v>
       </c>
       <c r="I118" s="3">
         <v>8</v>
@@ -12854,9 +12854,9 @@
       <c r="BT118" s="2"/>
       <c r="BU118" s="2"/>
     </row>
-    <row r="119" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C119" s="1">
         <v>40945</v>
@@ -12867,7 +12867,7 @@
         <v>33</v>
       </c>
       <c r="H119" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I119" s="3">
         <v>8</v>
@@ -12979,9 +12979,9 @@
       <c r="BT119" s="2"/>
       <c r="BU119" s="2"/>
     </row>
-    <row r="120" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C120" s="1">
         <v>40947</v>
@@ -12990,16 +12990,16 @@
         <v>4</v>
       </c>
       <c r="E120" t="s">
+        <v>73</v>
+      </c>
+      <c r="F120" t="s">
         <v>74</v>
-      </c>
-      <c r="F120" t="s">
-        <v>75</v>
       </c>
       <c r="G120">
         <v>35</v>
       </c>
       <c r="H120" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I120" s="3">
         <v>8</v>
@@ -13075,9 +13075,9 @@
       <c r="BT120" s="2"/>
       <c r="BU120" s="2"/>
     </row>
-    <row r="121" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C121" s="1">
         <v>40956</v>
@@ -13088,7 +13088,7 @@
         <v>44</v>
       </c>
       <c r="H121" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I121" s="3">
         <v>8</v>
@@ -13200,9 +13200,9 @@
       <c r="BT121" s="2"/>
       <c r="BU121" s="2"/>
     </row>
-    <row r="122" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C122" s="1">
         <v>40960</v>
@@ -13213,7 +13213,7 @@
         <v>48</v>
       </c>
       <c r="H122" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I122" s="3">
         <v>8</v>
@@ -13289,9 +13289,9 @@
       <c r="BT122" s="2"/>
       <c r="BU122" s="2"/>
     </row>
-    <row r="123" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C123" s="1">
         <v>40963</v>
@@ -13300,16 +13300,16 @@
         <v>5</v>
       </c>
       <c r="E123" t="s">
+        <v>75</v>
+      </c>
+      <c r="F123" t="s">
         <v>76</v>
-      </c>
-      <c r="F123" t="s">
-        <v>77</v>
       </c>
       <c r="G123">
         <v>51</v>
       </c>
       <c r="H123" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I123" s="3">
         <v>8</v>
@@ -13423,9 +13423,9 @@
       <c r="BT123" s="2"/>
       <c r="BU123" s="2"/>
     </row>
-    <row r="124" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C124" s="1">
         <v>40970</v>
@@ -13436,7 +13436,7 @@
         <v>58</v>
       </c>
       <c r="H124" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I124" s="3">
         <v>8</v>
@@ -13512,9 +13512,9 @@
       <c r="BT124" s="2"/>
       <c r="BU124" s="2"/>
     </row>
-    <row r="125" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C125" s="1">
         <v>40976</v>
@@ -13525,7 +13525,7 @@
         <v>64</v>
       </c>
       <c r="H125" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I125" s="3">
         <v>8</v>
@@ -13601,9 +13601,9 @@
       <c r="BT125" s="2"/>
       <c r="BU125" s="2"/>
     </row>
-    <row r="126" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C126" s="1">
         <v>40980</v>
@@ -13612,16 +13612,16 @@
         <v>6</v>
       </c>
       <c r="E126" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F126" t="s">
         <v>78</v>
-      </c>
-      <c r="F126" t="s">
-        <v>79</v>
       </c>
       <c r="G126">
         <v>68</v>
       </c>
       <c r="H126" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I126" s="3">
         <v>8</v>
@@ -13733,9 +13733,9 @@
       <c r="BT126" s="2"/>
       <c r="BU126" s="2"/>
     </row>
-    <row r="127" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C127" s="1">
         <v>40982</v>
@@ -13746,7 +13746,7 @@
         <v>70</v>
       </c>
       <c r="H127" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I127" s="3">
         <v>8</v>
@@ -13822,9 +13822,9 @@
       <c r="BT127" s="2"/>
       <c r="BU127" s="2"/>
     </row>
-    <row r="128" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C128" s="1">
         <v>40994</v>
@@ -13835,7 +13835,7 @@
         <v>82</v>
       </c>
       <c r="H128" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I128" s="3">
         <v>8</v>
@@ -13911,9 +13911,9 @@
       <c r="BT128" s="2"/>
       <c r="BU128" s="2"/>
     </row>
-    <row r="129" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C129" s="1">
         <v>40998</v>
@@ -13922,16 +13922,16 @@
         <v>8</v>
       </c>
       <c r="E129" t="s">
+        <v>79</v>
+      </c>
+      <c r="F129" t="s">
         <v>80</v>
-      </c>
-      <c r="F129" t="s">
-        <v>81</v>
       </c>
       <c r="G129">
         <v>86</v>
       </c>
       <c r="H129" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I129" s="3">
         <v>8</v>
@@ -14007,9 +14007,9 @@
       <c r="BT129" s="2"/>
       <c r="BU129" s="2"/>
     </row>
-    <row r="130" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C130" s="1">
         <v>41001</v>
@@ -14020,7 +14020,7 @@
         <v>89</v>
       </c>
       <c r="H130" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I130" s="3">
         <v>8</v>
@@ -14096,9 +14096,9 @@
       <c r="BT130" s="2"/>
       <c r="BU130" s="2"/>
     </row>
-    <row r="131" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C131" s="1">
         <v>41011</v>
@@ -14109,7 +14109,7 @@
         <v>99</v>
       </c>
       <c r="H131" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I131" s="3">
         <v>8</v>
@@ -14221,9 +14221,9 @@
       <c r="BT131" s="2"/>
       <c r="BU131" s="2"/>
     </row>
-    <row r="132" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C132" s="1">
         <v>41016</v>
@@ -14234,7 +14234,7 @@
         <v>104</v>
       </c>
       <c r="H132" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I132" s="3">
         <v>8</v>
@@ -14310,9 +14310,9 @@
       <c r="BT132" s="2"/>
       <c r="BU132" s="2"/>
     </row>
-    <row r="133" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C133" s="1">
         <v>41029</v>
@@ -14323,7 +14323,7 @@
         <v>117</v>
       </c>
       <c r="H133" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I133" s="3">
         <v>8</v>
@@ -14435,9 +14435,9 @@
       <c r="BT133" s="2"/>
       <c r="BU133" s="2"/>
     </row>
-    <row r="134" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C134" s="1">
         <v>41043</v>
@@ -14448,7 +14448,7 @@
         <v>131</v>
       </c>
       <c r="H134" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I134" s="3">
         <v>8</v>
@@ -14526,9 +14526,9 @@
       <c r="BT134" s="2"/>
       <c r="BU134" s="2"/>
     </row>
-    <row r="135" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C135" s="1">
         <v>41050</v>
@@ -14539,7 +14539,7 @@
         <v>138</v>
       </c>
       <c r="H135" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I135" s="3">
         <v>8</v>
@@ -14617,9 +14617,9 @@
       <c r="BT135" s="2"/>
       <c r="BU135" s="2"/>
     </row>
-    <row r="136" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C136" s="1">
         <v>41057</v>
@@ -14630,7 +14630,7 @@
         <v>145</v>
       </c>
       <c r="H136" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I136" s="3">
         <v>8</v>
@@ -14708,9 +14708,9 @@
       <c r="BT136" s="2"/>
       <c r="BU136" s="2"/>
     </row>
-    <row r="137" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C137" s="1">
         <v>41064</v>
@@ -14721,7 +14721,7 @@
         <v>152</v>
       </c>
       <c r="H137" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I137" s="3">
         <v>8</v>
@@ -14799,9 +14799,9 @@
       <c r="BT137" s="2"/>
       <c r="BU137" s="2"/>
     </row>
-    <row r="138" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C138" s="1">
         <v>41066</v>
@@ -14812,7 +14812,7 @@
         <v>154</v>
       </c>
       <c r="H138" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I138" s="3">
         <v>8</v>
@@ -14924,9 +14924,9 @@
       <c r="BT138" s="2"/>
       <c r="BU138" s="2"/>
     </row>
-    <row r="139" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C139" s="1">
         <v>41071</v>
@@ -14935,16 +14935,16 @@
         <v>9</v>
       </c>
       <c r="E139" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F139" t="s">
         <v>82</v>
-      </c>
-      <c r="F139" t="s">
-        <v>83</v>
       </c>
       <c r="G139">
         <v>159</v>
       </c>
       <c r="H139" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I139" s="3">
         <v>8</v>
@@ -15020,9 +15020,9 @@
       <c r="BT139" s="2"/>
       <c r="BU139" s="2"/>
     </row>
-    <row r="140" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C140" s="1">
         <v>41072</v>
@@ -15033,7 +15033,7 @@
         <v>160</v>
       </c>
       <c r="H140" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I140" s="3">
         <v>8</v>
@@ -15111,9 +15111,9 @@
       <c r="BT140" s="2"/>
       <c r="BU140" s="2"/>
     </row>
-    <row r="141" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C141" s="1">
         <v>41092</v>
@@ -15124,7 +15124,7 @@
         <v>180</v>
       </c>
       <c r="H141" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I141" s="3">
         <v>8</v>
@@ -15202,9 +15202,9 @@
       <c r="BT141" s="2"/>
       <c r="BU141" s="2"/>
     </row>
-    <row r="142" spans="1:73" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C142" s="1">
         <v>41096</v>
@@ -15213,16 +15213,16 @@
         <v>10</v>
       </c>
       <c r="E142" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F142" t="s">
         <v>84</v>
-      </c>
-      <c r="F142" t="s">
-        <v>85</v>
       </c>
       <c r="G142">
         <v>184</v>
       </c>
       <c r="H142" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I142" s="3">
         <v>8</v>

</xml_diff>

<commit_message>
Fixed capitalisation NConc, chnaged "Fruit" to "Boll"
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CCE800-6E5E-48B8-8C69-D9E505AD1AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C434479A-3B47-4368-BE06-2CF6CE9A4A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="17640" xr2:uid="{FBA18FA7-8D49-4A23-B648-57CB41343816}"/>
   </bookViews>
@@ -170,19 +170,10 @@
     <t>dw_OB</t>
   </si>
   <si>
-    <t>Cotton.Fruit.Nconc</t>
-  </si>
-  <si>
-    <t>Cotton.Fruit.N</t>
-  </si>
-  <si>
     <t>Cotton.AboveGround.Wt</t>
   </si>
   <si>
     <t>Cotton.AboveGround.N</t>
-  </si>
-  <si>
-    <t>Cotton.Fruit.HarvestIndex</t>
   </si>
   <si>
     <t>percent_l</t>
@@ -210,9 +201,6 @@
   </si>
   <si>
     <t>AboveGround.Partitioning.Leaf</t>
-  </si>
-  <si>
-    <t>AboveGround.Partitioning.Fruit</t>
   </si>
   <si>
     <t>Cotton.Sites</t>
@@ -318,6 +306,18 @@
   </si>
   <si>
     <t>Cotton.Leaf.SpecificAreaCanopy</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.NConc</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.N</t>
+  </si>
+  <si>
+    <t>Cotton.Boll.HarvestIndex</t>
+  </si>
+  <si>
+    <t>AboveGround.Partitioning.Boll</t>
   </si>
 </sst>
 </file>
@@ -682,10 +682,10 @@
   <dimension ref="A1:BU142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="P110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="BA2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V118" sqref="V118:V142"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +928,7 @@
         <v>33</v>
       </c>
       <c r="AI1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AJ1" t="s">
         <v>34</v>
@@ -958,96 +958,96 @@
         <v>42</v>
       </c>
       <c r="AS1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX1" t="s">
         <v>91</v>
       </c>
-      <c r="AT1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BE1" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>52</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BI1" t="s">
         <v>54</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BJ1" t="s">
         <v>55</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BK1" t="s">
         <v>56</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BL1" t="s">
         <v>57</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BM1" t="s">
         <v>58</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BN1" t="s">
         <v>59</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BO1" t="s">
         <v>60</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BP1" t="s">
         <v>61</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BQ1" t="s">
         <v>62</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BR1" t="s">
         <v>63</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BS1" t="s">
         <v>64</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BT1" t="s">
         <v>65</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BU1" t="s">
         <v>66</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C2" s="1">
         <v>39783</v>
@@ -1056,16 +1056,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I2" s="3">
         <v>8.3000000000000007</v>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C3" s="1">
         <v>39798</v>
@@ -1178,7 +1178,7 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I3" s="3">
         <v>8.3000000000000007</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C4" s="1">
         <v>39804</v>
@@ -1273,16 +1273,16 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G4">
         <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I4" s="3">
         <v>8.3000000000000007</v>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1">
         <v>39806</v>
@@ -1377,7 +1377,7 @@
         <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I5" s="3">
         <v>8.3000000000000007</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1">
         <v>39813</v>
@@ -1474,7 +1474,7 @@
         <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I6" s="3">
         <v>8.3000000000000007</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1">
         <v>39818</v>
@@ -1571,7 +1571,7 @@
         <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I7" s="3">
         <v>8.3000000000000007</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="8" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C8" s="1">
         <v>39819</v>
@@ -1700,7 +1700,7 @@
         <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I8" s="3">
         <v>8.3000000000000007</v>
@@ -1786,7 +1786,7 @@
     </row>
     <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1">
         <v>39825</v>
@@ -1795,16 +1795,16 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G9">
         <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I9" s="3">
         <v>8.3000000000000007</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="10" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1">
         <v>39827</v>
@@ -1937,7 +1937,7 @@
         <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I10" s="3">
         <v>8.3000000000000007</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="11" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C11" s="1">
         <v>39833</v>
@@ -2034,7 +2034,7 @@
         <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I11" s="3">
         <v>8.3000000000000007</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="12" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C12" s="1">
         <v>39840</v>
@@ -2131,7 +2131,7 @@
         <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I12" s="3">
         <v>8.3000000000000007</v>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="13" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1">
         <v>39841</v>
@@ -2228,7 +2228,7 @@
         <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I13" s="3">
         <v>8.3000000000000007</v>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="14" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C14" s="1">
         <v>39848</v>
@@ -2361,7 +2361,7 @@
         <v>65</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I14" s="3">
         <v>8.3000000000000007</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="15" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C15" s="1">
         <v>39853</v>
@@ -2456,16 +2456,16 @@
         <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G15">
         <v>70</v>
       </c>
       <c r="H15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I15" s="3">
         <v>8.3000000000000007</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="16" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C16" s="1">
         <v>39854</v>
@@ -2598,7 +2598,7 @@
         <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I16" s="3">
         <v>8.3000000000000007</v>
@@ -2684,7 +2684,7 @@
     </row>
     <row r="17" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1">
         <v>39860</v>
@@ -2695,7 +2695,7 @@
         <v>77</v>
       </c>
       <c r="H17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I17" s="3">
         <v>8.3000000000000007</v>
@@ -2781,7 +2781,7 @@
     </row>
     <row r="18" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1">
         <v>39874</v>
@@ -2792,7 +2792,7 @@
         <v>91</v>
       </c>
       <c r="H18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I18" s="3">
         <v>8.3000000000000007</v>
@@ -2878,7 +2878,7 @@
     </row>
     <row r="19" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C19" s="1">
         <v>39875</v>
@@ -2889,7 +2889,7 @@
         <v>92</v>
       </c>
       <c r="H19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I19" s="3">
         <v>8.3000000000000007</v>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="20" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C20" s="1">
         <v>39877</v>
@@ -3020,16 +3020,16 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G20">
         <v>94</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I20" s="3">
         <v>8.3000000000000007</v>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="21" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C21" s="1">
         <v>39884</v>
@@ -3124,7 +3124,7 @@
         <v>101</v>
       </c>
       <c r="H21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I21" s="3">
         <v>8.3000000000000007</v>
@@ -3210,7 +3210,7 @@
     </row>
     <row r="22" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1">
         <v>39889</v>
@@ -3221,7 +3221,7 @@
         <v>106</v>
       </c>
       <c r="H22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I22" s="3">
         <v>8.3000000000000007</v>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="23" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1">
         <v>39895</v>
@@ -3354,7 +3354,7 @@
         <v>112</v>
       </c>
       <c r="H23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I23" s="3">
         <v>8.3000000000000007</v>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="24" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C24" s="1">
         <v>39904</v>
@@ -3451,7 +3451,7 @@
         <v>121</v>
       </c>
       <c r="H24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I24" s="3">
         <v>8.3000000000000007</v>
@@ -3539,7 +3539,7 @@
     </row>
     <row r="25" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1">
         <v>39910</v>
@@ -3550,7 +3550,7 @@
         <v>127</v>
       </c>
       <c r="H25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I25" s="3">
         <v>8.3000000000000007</v>
@@ -3672,7 +3672,7 @@
     </row>
     <row r="26" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1">
         <v>39911</v>
@@ -3683,7 +3683,7 @@
         <v>128</v>
       </c>
       <c r="H26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I26" s="3">
         <v>8.3000000000000007</v>
@@ -3771,7 +3771,7 @@
     </row>
     <row r="27" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C27" s="1">
         <v>39920</v>
@@ -3782,7 +3782,7 @@
         <v>137</v>
       </c>
       <c r="H27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I27" s="3">
         <v>8.3000000000000007</v>
@@ -3870,7 +3870,7 @@
     </row>
     <row r="28" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C28" s="1">
         <v>39925</v>
@@ -3881,7 +3881,7 @@
         <v>142</v>
       </c>
       <c r="H28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I28" s="3">
         <v>8.3000000000000007</v>
@@ -3969,7 +3969,7 @@
     </row>
     <row r="29" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C29" s="1">
         <v>39932</v>
@@ -3980,7 +3980,7 @@
         <v>149</v>
       </c>
       <c r="H29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I29" s="3">
         <v>8.3000000000000007</v>
@@ -4068,7 +4068,7 @@
     </row>
     <row r="30" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C30" s="1">
         <v>39939</v>
@@ -4079,7 +4079,7 @@
         <v>156</v>
       </c>
       <c r="H30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I30" s="3">
         <v>8.3000000000000007</v>
@@ -4167,7 +4167,7 @@
     </row>
     <row r="31" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C31" s="1">
         <v>39946</v>
@@ -4178,7 +4178,7 @@
         <v>163</v>
       </c>
       <c r="H31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I31" s="3">
         <v>8.3000000000000007</v>
@@ -4266,7 +4266,7 @@
     </row>
     <row r="32" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C32" s="1">
         <v>39947</v>
@@ -4275,16 +4275,16 @@
         <v>9</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F32" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G32">
         <v>164</v>
       </c>
       <c r="H32" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I32" s="3">
         <v>8.3000000000000007</v>
@@ -4368,7 +4368,7 @@
     </row>
     <row r="33" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C33" s="1">
         <v>39954</v>
@@ -4379,7 +4379,7 @@
         <v>171</v>
       </c>
       <c r="H33" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I33" s="3">
         <v>8.3000000000000007</v>
@@ -4467,7 +4467,7 @@
     </row>
     <row r="34" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C34" s="1">
         <v>39957</v>
@@ -4476,16 +4476,16 @@
         <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F34" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G34">
         <v>174</v>
       </c>
       <c r="H34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I34" s="3">
         <v>8.3000000000000007</v>
@@ -4577,7 +4577,7 @@
     </row>
     <row r="35" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C35" s="1">
         <v>39960</v>
@@ -4588,7 +4588,7 @@
         <v>177</v>
       </c>
       <c r="H35" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I35" s="3">
         <v>8.3000000000000007</v>
@@ -4676,7 +4676,7 @@
     </row>
     <row r="36" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C36" s="1">
         <v>39801</v>
@@ -4685,16 +4685,16 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G36" s="2">
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I36" s="3">
         <v>8.1</v>
@@ -4796,7 +4796,7 @@
     </row>
     <row r="37" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C37" s="1">
         <v>39819</v>
@@ -4807,7 +4807,7 @@
         <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I37" s="3">
         <v>8.1</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="38" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C38" s="1">
         <v>39820</v>
@@ -4904,7 +4904,7 @@
         <v>19</v>
       </c>
       <c r="H38" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I38" s="3">
         <v>8.1</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="39" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C39" s="1">
         <v>39824</v>
@@ -5017,16 +5017,16 @@
         <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F39" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G39">
         <v>23</v>
       </c>
       <c r="H39" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I39" s="3">
         <v>8.1</v>
@@ -5110,7 +5110,7 @@
     </row>
     <row r="40" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1">
         <v>39827</v>
@@ -5121,7 +5121,7 @@
         <v>26</v>
       </c>
       <c r="H40" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I40" s="3">
         <v>8.1</v>
@@ -5207,7 +5207,7 @@
     </row>
     <row r="41" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C41" s="1">
         <v>39833</v>
@@ -5218,7 +5218,7 @@
         <v>32</v>
       </c>
       <c r="H41" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I41" s="3">
         <v>8.1</v>
@@ -5338,7 +5338,7 @@
     </row>
     <row r="42" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C42" s="1">
         <v>39840</v>
@@ -5349,7 +5349,7 @@
         <v>39</v>
       </c>
       <c r="H42" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I42" s="3">
         <v>8.1</v>
@@ -5435,7 +5435,7 @@
     </row>
     <row r="43" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C43" s="1">
         <v>39848</v>
@@ -5446,7 +5446,7 @@
         <v>47</v>
       </c>
       <c r="H43" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I43" s="3">
         <v>8.1</v>
@@ -5570,7 +5570,7 @@
     </row>
     <row r="44" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C44" s="1">
         <v>39849</v>
@@ -5579,16 +5579,16 @@
         <v>4</v>
       </c>
       <c r="E44" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F44" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G44">
         <v>48</v>
       </c>
       <c r="H44" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I44" s="3">
         <v>8.1</v>
@@ -5672,7 +5672,7 @@
     </row>
     <row r="45" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C45" s="1">
         <v>39854</v>
@@ -5683,7 +5683,7 @@
         <v>53</v>
       </c>
       <c r="H45" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I45" s="3">
         <v>8.1</v>
@@ -5769,7 +5769,7 @@
     </row>
     <row r="46" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C46" s="1">
         <v>39860</v>
@@ -5778,16 +5778,16 @@
         <v>6</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F46" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G46" s="2">
         <v>59</v>
       </c>
       <c r="H46" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I46" s="3">
         <v>8.1</v>
@@ -5911,7 +5911,7 @@
     </row>
     <row r="47" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C47" s="1">
         <v>39869</v>
@@ -5922,7 +5922,7 @@
         <v>68</v>
       </c>
       <c r="H47" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I47" s="3">
         <v>8.1</v>
@@ -6008,7 +6008,7 @@
     </row>
     <row r="48" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C48" s="1">
         <v>39874</v>
@@ -6019,7 +6019,7 @@
         <v>73</v>
       </c>
       <c r="H48" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I48" s="3">
         <v>8.1</v>
@@ -6105,7 +6105,7 @@
     </row>
     <row r="49" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C49" s="1">
         <v>39876</v>
@@ -6116,7 +6116,7 @@
         <v>75</v>
       </c>
       <c r="H49" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I49" s="3">
         <v>8.1</v>
@@ -6238,7 +6238,7 @@
     </row>
     <row r="50" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C50" s="1">
         <v>39884</v>
@@ -6249,7 +6249,7 @@
         <v>83</v>
       </c>
       <c r="H50" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I50" s="3">
         <v>8.1</v>
@@ -6335,7 +6335,7 @@
     </row>
     <row r="51" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C51" s="1">
         <v>39888</v>
@@ -6346,7 +6346,7 @@
         <v>87</v>
       </c>
       <c r="H51" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I51" s="3">
         <v>8.1</v>
@@ -6468,7 +6468,7 @@
     </row>
     <row r="52" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C52" s="1">
         <v>39895</v>
@@ -6479,7 +6479,7 @@
         <v>94</v>
       </c>
       <c r="H52" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I52" s="3">
         <v>8.1</v>
@@ -6565,7 +6565,7 @@
     </row>
     <row r="53" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C53" s="1">
         <v>39904</v>
@@ -6576,7 +6576,7 @@
         <v>103</v>
       </c>
       <c r="H53" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I53" s="3">
         <v>8.1</v>
@@ -6698,7 +6698,7 @@
     </row>
     <row r="54" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C54" s="1">
         <v>39908</v>
@@ -6709,7 +6709,7 @@
         <v>107</v>
       </c>
       <c r="H54" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I54" s="3">
         <v>8.1</v>
@@ -6795,7 +6795,7 @@
     </row>
     <row r="55" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C55" s="1">
         <v>39911</v>
@@ -6806,7 +6806,7 @@
         <v>110</v>
       </c>
       <c r="H55" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I55" s="3">
         <v>8.1</v>
@@ -6894,7 +6894,7 @@
     </row>
     <row r="56" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C56" s="1">
         <v>39920</v>
@@ -6905,7 +6905,7 @@
         <v>119</v>
       </c>
       <c r="H56" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I56" s="3">
         <v>8.1</v>
@@ -6993,7 +6993,7 @@
     </row>
     <row r="57" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C57" s="1">
         <v>39922</v>
@@ -7002,16 +7002,16 @@
         <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F57" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G57">
         <v>121</v>
       </c>
       <c r="H57" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I57" s="3">
         <v>8.1</v>
@@ -7095,7 +7095,7 @@
     </row>
     <row r="58" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C58" s="1">
         <v>39925</v>
@@ -7106,7 +7106,7 @@
         <v>124</v>
       </c>
       <c r="H58" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I58" s="3">
         <v>8.1</v>
@@ -7194,7 +7194,7 @@
     </row>
     <row r="59" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C59" s="1">
         <v>39932</v>
@@ -7205,7 +7205,7 @@
         <v>131</v>
       </c>
       <c r="H59" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I59" s="3">
         <v>8.1</v>
@@ -7331,7 +7331,7 @@
     </row>
     <row r="60" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C60" s="1">
         <v>39939</v>
@@ -7342,7 +7342,7 @@
         <v>138</v>
       </c>
       <c r="H60" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I60" s="3">
         <v>8.1</v>
@@ -7430,7 +7430,7 @@
     </row>
     <row r="61" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C61" s="1">
         <v>39945</v>
@@ -7439,16 +7439,16 @@
         <v>9</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F61" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G61">
         <v>144</v>
       </c>
       <c r="H61" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I61" s="3">
         <v>8.1</v>
@@ -7532,7 +7532,7 @@
     </row>
     <row r="62" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C62" s="1">
         <v>39946</v>
@@ -7543,7 +7543,7 @@
         <v>145</v>
       </c>
       <c r="H62" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I62" s="3">
         <v>8.1</v>
@@ -7631,7 +7631,7 @@
     </row>
     <row r="63" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C63" s="1">
         <v>39954</v>
@@ -7642,7 +7642,7 @@
         <v>153</v>
       </c>
       <c r="H63" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I63" s="3">
         <v>8.1</v>
@@ -7730,7 +7730,7 @@
     </row>
     <row r="64" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C64" s="1">
         <v>39960</v>
@@ -7739,16 +7739,16 @@
         <v>10</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F64" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G64">
         <v>159</v>
       </c>
       <c r="H64" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I64" s="3">
         <v>8.1</v>
@@ -7844,7 +7844,7 @@
     </row>
     <row r="65" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C65" s="1">
         <v>39820</v>
@@ -7853,16 +7853,16 @@
         <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F65" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G65" s="2">
         <v>0</v>
       </c>
       <c r="H65" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I65" s="3">
         <v>8.3000000000000007</v>
@@ -7964,7 +7964,7 @@
     </row>
     <row r="66" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C66" s="1">
         <v>39846</v>
@@ -7973,16 +7973,16 @@
         <v>4</v>
       </c>
       <c r="E66" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F66" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G66">
         <v>26</v>
       </c>
       <c r="H66" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I66" s="3">
         <v>8.3000000000000007</v>
@@ -8084,7 +8084,7 @@
     </row>
     <row r="67" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C67" s="1">
         <v>39848</v>
@@ -8095,7 +8095,7 @@
         <v>28</v>
       </c>
       <c r="H67" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I67" s="3">
         <v>8.3000000000000007</v>
@@ -8181,7 +8181,7 @@
     </row>
     <row r="68" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C68" s="1">
         <v>39854</v>
@@ -8192,7 +8192,7 @@
         <v>34</v>
       </c>
       <c r="H68" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I68" s="3">
         <v>8.3000000000000007</v>
@@ -8278,7 +8278,7 @@
     </row>
     <row r="69" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C69" s="1">
         <v>39860</v>
@@ -8289,7 +8289,7 @@
         <v>40</v>
       </c>
       <c r="H69" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I69" s="3">
         <v>8.3000000000000007</v>
@@ -8375,7 +8375,7 @@
     </row>
     <row r="70" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C70" s="1">
         <v>39864</v>
@@ -8386,7 +8386,7 @@
         <v>44</v>
       </c>
       <c r="H70" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I70" s="3">
         <v>8.3000000000000007</v>
@@ -8490,7 +8490,7 @@
     </row>
     <row r="71" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C71" s="1">
         <v>39869</v>
@@ -8501,7 +8501,7 @@
         <v>49</v>
       </c>
       <c r="H71" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I71" s="3">
         <v>8.3000000000000007</v>
@@ -8587,7 +8587,7 @@
     </row>
     <row r="72" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C72" s="1">
         <v>39874</v>
@@ -8598,7 +8598,7 @@
         <v>54</v>
       </c>
       <c r="H72" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I72" s="3">
         <v>8.3000000000000007</v>
@@ -8721,7 +8721,7 @@
     </row>
     <row r="73" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C73" s="1">
         <v>39877</v>
@@ -8730,16 +8730,16 @@
         <v>4</v>
       </c>
       <c r="E73" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F73" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G73">
         <v>57</v>
       </c>
       <c r="H73" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I73" s="3">
         <v>8.3000000000000007</v>
@@ -8823,7 +8823,7 @@
     </row>
     <row r="74" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C74" s="1">
         <v>39884</v>
@@ -8834,7 +8834,7 @@
         <v>64</v>
       </c>
       <c r="H74" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I74" s="3">
         <v>8.3000000000000007</v>
@@ -8920,7 +8920,7 @@
     </row>
     <row r="75" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C75" s="1">
         <v>39890</v>
@@ -8931,7 +8931,7 @@
         <v>70</v>
       </c>
       <c r="H75" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I75" s="3">
         <v>8.3000000000000007</v>
@@ -9055,7 +9055,7 @@
     </row>
     <row r="76" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C76" s="1">
         <v>39895</v>
@@ -9066,7 +9066,7 @@
         <v>75</v>
       </c>
       <c r="H76" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I76" s="3">
         <v>8.3000000000000007</v>
@@ -9152,7 +9152,7 @@
     </row>
     <row r="77" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C77" s="1">
         <v>39903</v>
@@ -9161,16 +9161,16 @@
         <v>6</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F77" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G77">
         <v>83</v>
       </c>
       <c r="H77" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I77" s="3">
         <v>8.3000000000000007</v>
@@ -9294,7 +9294,7 @@
     </row>
     <row r="78" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C78" s="1">
         <v>39911</v>
@@ -9305,7 +9305,7 @@
         <v>91</v>
       </c>
       <c r="H78" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I78" s="3">
         <v>8.3000000000000007</v>
@@ -9391,7 +9391,7 @@
     </row>
     <row r="79" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C79" s="1">
         <v>39919</v>
@@ -9402,7 +9402,7 @@
         <v>99</v>
       </c>
       <c r="H79" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I79" s="3">
         <v>8.3000000000000007</v>
@@ -9524,7 +9524,7 @@
     </row>
     <row r="80" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C80" s="1">
         <v>39928</v>
@@ -9535,7 +9535,7 @@
         <v>108</v>
       </c>
       <c r="H80" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I80" s="3">
         <v>8.3000000000000007</v>
@@ -9621,7 +9621,7 @@
     </row>
     <row r="81" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C81" s="1">
         <v>39938</v>
@@ -9630,16 +9630,16 @@
         <v>8</v>
       </c>
       <c r="E81" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F81" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G81">
         <v>118</v>
       </c>
       <c r="H81" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I81" s="3">
         <v>8.3000000000000007</v>
@@ -9761,7 +9761,7 @@
     </row>
     <row r="82" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C82" s="1">
         <v>39954</v>
@@ -9772,7 +9772,7 @@
         <v>134</v>
       </c>
       <c r="H82" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I82" s="3">
         <v>8.3000000000000007</v>
@@ -9860,7 +9860,7 @@
     </row>
     <row r="83" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C83" s="1">
         <v>39960</v>
@@ -9871,7 +9871,7 @@
         <v>140</v>
       </c>
       <c r="H83" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I83" s="3">
         <v>8.3000000000000007</v>
@@ -9959,7 +9959,7 @@
     </row>
     <row r="84" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C84" s="1">
         <v>39966</v>
@@ -9970,7 +9970,7 @@
         <v>146</v>
       </c>
       <c r="H84" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I84" s="3">
         <v>8.3000000000000007</v>
@@ -10092,7 +10092,7 @@
     </row>
     <row r="85" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C85" s="1">
         <v>39969</v>
@@ -10103,7 +10103,7 @@
         <v>149</v>
       </c>
       <c r="H85" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I85" s="3">
         <v>8.3000000000000007</v>
@@ -10191,7 +10191,7 @@
     </row>
     <row r="86" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C86" s="1">
         <v>39974</v>
@@ -10200,16 +10200,16 @@
         <v>9</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F86" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G86">
         <v>154</v>
       </c>
       <c r="H86" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I86" s="3">
         <v>8.3000000000000007</v>
@@ -10293,7 +10293,7 @@
     </row>
     <row r="87" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C87" s="1">
         <v>39976</v>
@@ -10304,7 +10304,7 @@
         <v>156</v>
       </c>
       <c r="H87" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I87" s="3">
         <v>8.3000000000000007</v>
@@ -10392,7 +10392,7 @@
     </row>
     <row r="88" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C88" s="1">
         <v>39983</v>
@@ -10403,7 +10403,7 @@
         <v>163</v>
       </c>
       <c r="H88" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I88" s="3">
         <v>8.3000000000000007</v>
@@ -10491,7 +10491,7 @@
     </row>
     <row r="89" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C89" s="1">
         <v>39990</v>
@@ -10502,7 +10502,7 @@
         <v>170</v>
       </c>
       <c r="H89" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I89" s="3">
         <v>8.3000000000000007</v>
@@ -10590,7 +10590,7 @@
     </row>
     <row r="90" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C90" s="1">
         <v>39994</v>
@@ -10599,16 +10599,16 @@
         <v>10</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F90" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G90">
         <v>174</v>
       </c>
       <c r="H90" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I90" s="3">
         <v>8.3000000000000007</v>
@@ -10700,7 +10700,7 @@
     </row>
     <row r="91" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C91" s="1">
         <v>39995</v>
@@ -10711,7 +10711,7 @@
         <v>175</v>
       </c>
       <c r="H91" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I91" s="3">
         <v>8.3000000000000007</v>
@@ -10799,7 +10799,7 @@
     </row>
     <row r="92" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C92" s="1">
         <v>40895</v>
@@ -10808,16 +10808,16 @@
         <v>1</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F92" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G92">
         <v>0</v>
       </c>
       <c r="H92" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I92" s="3">
         <v>8</v>
@@ -10919,7 +10919,7 @@
     </row>
     <row r="93" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C93" s="1">
         <v>40924</v>
@@ -10928,16 +10928,16 @@
         <v>4</v>
       </c>
       <c r="E93" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F93" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G93">
         <v>29</v>
       </c>
       <c r="H93" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I93" s="3">
         <v>8</v>
@@ -11039,7 +11039,7 @@
     </row>
     <row r="94" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C94" s="1">
         <v>40931</v>
@@ -11050,7 +11050,7 @@
         <v>36</v>
       </c>
       <c r="H94" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I94" s="3">
         <v>8</v>
@@ -11136,7 +11136,7 @@
     </row>
     <row r="95" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C95" s="1">
         <v>40938</v>
@@ -11147,7 +11147,7 @@
         <v>43</v>
       </c>
       <c r="H95" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I95" s="3">
         <v>8</v>
@@ -11269,7 +11269,7 @@
     </row>
     <row r="96" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C96" s="1">
         <v>40939</v>
@@ -11280,7 +11280,7 @@
         <v>44</v>
       </c>
       <c r="H96" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I96" s="3">
         <v>8</v>
@@ -11366,7 +11366,7 @@
     </row>
     <row r="97" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C97" s="1">
         <v>40945</v>
@@ -11375,16 +11375,16 @@
         <v>5</v>
       </c>
       <c r="E97" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F97" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G97">
         <v>50</v>
       </c>
       <c r="H97" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I97" s="3">
         <v>8</v>
@@ -11506,7 +11506,7 @@
     </row>
     <row r="98" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C98" s="1">
         <v>40948</v>
@@ -11517,7 +11517,7 @@
         <v>53</v>
       </c>
       <c r="H98" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I98" s="3">
         <v>8</v>
@@ -11603,7 +11603,7 @@
     </row>
     <row r="99" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C99" s="1">
         <v>40954</v>
@@ -11614,7 +11614,7 @@
         <v>59</v>
       </c>
       <c r="H99" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I99" s="3">
         <v>8</v>
@@ -11700,7 +11700,7 @@
     </row>
     <row r="100" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C100" s="1">
         <v>40959</v>
@@ -11711,7 +11711,7 @@
         <v>64</v>
       </c>
       <c r="H100" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I100" s="3">
         <v>8</v>
@@ -11833,7 +11833,7 @@
     </row>
     <row r="101" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C101" s="1">
         <v>40960</v>
@@ -11844,7 +11844,7 @@
         <v>65</v>
       </c>
       <c r="H101" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I101" s="3">
         <v>8</v>
@@ -11930,7 +11930,7 @@
     </row>
     <row r="102" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C102" s="1">
         <v>40970</v>
@@ -11941,7 +11941,7 @@
         <v>75</v>
       </c>
       <c r="H102" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I102" s="3">
         <v>8</v>
@@ -12027,7 +12027,7 @@
     </row>
     <row r="103" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C103" s="1">
         <v>40976</v>
@@ -12038,7 +12038,7 @@
         <v>81</v>
       </c>
       <c r="H103" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I103" s="3">
         <v>8</v>
@@ -12124,7 +12124,7 @@
     </row>
     <row r="104" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C104" s="1">
         <v>40980</v>
@@ -12133,16 +12133,16 @@
         <v>6</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F104" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G104">
         <v>85</v>
       </c>
       <c r="H104" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I104" s="3">
         <v>8</v>
@@ -12264,7 +12264,7 @@
     </row>
     <row r="105" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C105" s="1">
         <v>40982</v>
@@ -12275,7 +12275,7 @@
         <v>87</v>
       </c>
       <c r="H105" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I105" s="3">
         <v>8</v>
@@ -12361,7 +12361,7 @@
     </row>
     <row r="106" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C106" s="1">
         <v>40997</v>
@@ -12370,16 +12370,16 @@
         <v>8</v>
       </c>
       <c r="E106" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F106" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G106">
         <v>102</v>
       </c>
       <c r="H106" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I106" s="3">
         <v>8</v>
@@ -12501,7 +12501,7 @@
     </row>
     <row r="107" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C107" s="1">
         <v>41001</v>
@@ -12512,7 +12512,7 @@
         <v>106</v>
       </c>
       <c r="H107" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I107" s="3">
         <v>8</v>
@@ -12598,7 +12598,7 @@
     </row>
     <row r="108" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C108" s="1">
         <v>41009</v>
@@ -12609,7 +12609,7 @@
         <v>114</v>
       </c>
       <c r="H108" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I108" s="3">
         <v>8</v>
@@ -12697,7 +12697,7 @@
     </row>
     <row r="109" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C109" s="1">
         <v>41018</v>
@@ -12708,7 +12708,7 @@
         <v>123</v>
       </c>
       <c r="H109" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I109" s="3">
         <v>8</v>
@@ -12796,7 +12796,7 @@
     </row>
     <row r="110" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C110" s="1">
         <v>41025</v>
@@ -12805,16 +12805,16 @@
         <v>9</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F110" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G110">
         <v>130</v>
       </c>
       <c r="H110" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I110" s="3">
         <v>8</v>
@@ -12902,7 +12902,7 @@
     </row>
     <row r="111" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C111" s="1">
         <v>41032</v>
@@ -12913,7 +12913,7 @@
         <v>137</v>
       </c>
       <c r="H111" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I111" s="3">
         <v>8</v>
@@ -13001,7 +13001,7 @@
     </row>
     <row r="112" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C112" s="1">
         <v>41038</v>
@@ -13012,7 +13012,7 @@
         <v>143</v>
       </c>
       <c r="H112" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I112" s="3">
         <v>8</v>
@@ -13134,7 +13134,7 @@
     </row>
     <row r="113" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C113" s="1">
         <v>41039</v>
@@ -13145,7 +13145,7 @@
         <v>144</v>
       </c>
       <c r="H113" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I113" s="3">
         <v>8</v>
@@ -13233,7 +13233,7 @@
     </row>
     <row r="114" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C114" s="1">
         <v>41043</v>
@@ -13244,7 +13244,7 @@
         <v>148</v>
       </c>
       <c r="H114" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I114" s="3">
         <v>8</v>
@@ -13332,7 +13332,7 @@
     </row>
     <row r="115" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C115" s="1">
         <v>41050</v>
@@ -13343,7 +13343,7 @@
         <v>155</v>
       </c>
       <c r="H115" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I115" s="3">
         <v>8</v>
@@ -13431,7 +13431,7 @@
     </row>
     <row r="116" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C116" s="1">
         <v>41057</v>
@@ -13442,7 +13442,7 @@
         <v>162</v>
       </c>
       <c r="H116" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I116" s="3">
         <v>8</v>
@@ -13530,7 +13530,7 @@
     </row>
     <row r="117" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C117" s="1">
         <v>41065</v>
@@ -13539,16 +13539,16 @@
         <v>10</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F117" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G117">
         <v>170</v>
       </c>
       <c r="H117" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I117" s="3">
         <v>8</v>
@@ -13640,7 +13640,7 @@
     </row>
     <row r="118" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C118" s="1">
         <v>40912</v>
@@ -13649,16 +13649,16 @@
         <v>1</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F118" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G118">
         <v>0</v>
       </c>
       <c r="H118" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I118" s="3">
         <v>8</v>
@@ -13760,7 +13760,7 @@
     </row>
     <row r="119" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C119" s="1">
         <v>40945</v>
@@ -13771,7 +13771,7 @@
         <v>33</v>
       </c>
       <c r="H119" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I119" s="3">
         <v>8</v>
@@ -13893,7 +13893,7 @@
     </row>
     <row r="120" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C120" s="1">
         <v>40947</v>
@@ -13902,16 +13902,16 @@
         <v>4</v>
       </c>
       <c r="E120" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F120" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G120">
         <v>35</v>
       </c>
       <c r="H120" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I120" s="3">
         <v>8</v>
@@ -13995,7 +13995,7 @@
     </row>
     <row r="121" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C121" s="1">
         <v>40956</v>
@@ -14006,7 +14006,7 @@
         <v>44</v>
       </c>
       <c r="H121" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I121" s="3">
         <v>8</v>
@@ -14128,7 +14128,7 @@
     </row>
     <row r="122" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C122" s="1">
         <v>40960</v>
@@ -14139,7 +14139,7 @@
         <v>48</v>
       </c>
       <c r="H122" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I122" s="3">
         <v>8</v>
@@ -14225,7 +14225,7 @@
     </row>
     <row r="123" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C123" s="1">
         <v>40963</v>
@@ -14234,16 +14234,16 @@
         <v>5</v>
       </c>
       <c r="E123" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F123" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G123">
         <v>51</v>
       </c>
       <c r="H123" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I123" s="3">
         <v>8</v>
@@ -14365,7 +14365,7 @@
     </row>
     <row r="124" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C124" s="1">
         <v>40970</v>
@@ -14376,7 +14376,7 @@
         <v>58</v>
       </c>
       <c r="H124" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I124" s="3">
         <v>8</v>
@@ -14462,7 +14462,7 @@
     </row>
     <row r="125" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C125" s="1">
         <v>40976</v>
@@ -14473,7 +14473,7 @@
         <v>64</v>
       </c>
       <c r="H125" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I125" s="3">
         <v>8</v>
@@ -14559,7 +14559,7 @@
     </row>
     <row r="126" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C126" s="1">
         <v>40980</v>
@@ -14568,16 +14568,16 @@
         <v>6</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F126" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G126">
         <v>68</v>
       </c>
       <c r="H126" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I126" s="3">
         <v>8</v>
@@ -14699,7 +14699,7 @@
     </row>
     <row r="127" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C127" s="1">
         <v>40982</v>
@@ -14710,7 +14710,7 @@
         <v>70</v>
       </c>
       <c r="H127" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I127" s="3">
         <v>8</v>
@@ -14796,7 +14796,7 @@
     </row>
     <row r="128" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C128" s="1">
         <v>40994</v>
@@ -14807,7 +14807,7 @@
         <v>82</v>
       </c>
       <c r="H128" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I128" s="3">
         <v>8</v>
@@ -14893,7 +14893,7 @@
     </row>
     <row r="129" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C129" s="1">
         <v>40998</v>
@@ -14902,16 +14902,16 @@
         <v>8</v>
       </c>
       <c r="E129" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F129" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G129">
         <v>86</v>
       </c>
       <c r="H129" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I129" s="3">
         <v>8</v>
@@ -14995,7 +14995,7 @@
     </row>
     <row r="130" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C130" s="1">
         <v>41001</v>
@@ -15006,7 +15006,7 @@
         <v>89</v>
       </c>
       <c r="H130" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I130" s="3">
         <v>8</v>
@@ -15092,7 +15092,7 @@
     </row>
     <row r="131" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C131" s="1">
         <v>41011</v>
@@ -15103,7 +15103,7 @@
         <v>99</v>
       </c>
       <c r="H131" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I131" s="3">
         <v>8</v>
@@ -15225,7 +15225,7 @@
     </row>
     <row r="132" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C132" s="1">
         <v>41016</v>
@@ -15236,7 +15236,7 @@
         <v>104</v>
       </c>
       <c r="H132" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I132" s="3">
         <v>8</v>
@@ -15322,7 +15322,7 @@
     </row>
     <row r="133" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C133" s="1">
         <v>41029</v>
@@ -15333,7 +15333,7 @@
         <v>117</v>
       </c>
       <c r="H133" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I133" s="3">
         <v>8</v>
@@ -15455,7 +15455,7 @@
     </row>
     <row r="134" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C134" s="1">
         <v>41043</v>
@@ -15466,7 +15466,7 @@
         <v>131</v>
       </c>
       <c r="H134" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I134" s="3">
         <v>8</v>
@@ -15554,7 +15554,7 @@
     </row>
     <row r="135" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C135" s="1">
         <v>41050</v>
@@ -15565,7 +15565,7 @@
         <v>138</v>
       </c>
       <c r="H135" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I135" s="3">
         <v>8</v>
@@ -15653,7 +15653,7 @@
     </row>
     <row r="136" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C136" s="1">
         <v>41057</v>
@@ -15664,7 +15664,7 @@
         <v>145</v>
       </c>
       <c r="H136" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I136" s="3">
         <v>8</v>
@@ -15752,7 +15752,7 @@
     </row>
     <row r="137" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C137" s="1">
         <v>41064</v>
@@ -15763,7 +15763,7 @@
         <v>152</v>
       </c>
       <c r="H137" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I137" s="3">
         <v>8</v>
@@ -15851,7 +15851,7 @@
     </row>
     <row r="138" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C138" s="1">
         <v>41066</v>
@@ -15862,7 +15862,7 @@
         <v>154</v>
       </c>
       <c r="H138" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I138" s="3">
         <v>8</v>
@@ -15984,7 +15984,7 @@
     </row>
     <row r="139" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C139" s="1">
         <v>41071</v>
@@ -15993,16 +15993,16 @@
         <v>9</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F139" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G139">
         <v>159</v>
       </c>
       <c r="H139" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I139" s="3">
         <v>8</v>
@@ -16086,7 +16086,7 @@
     </row>
     <row r="140" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C140" s="1">
         <v>41072</v>
@@ -16097,7 +16097,7 @@
         <v>160</v>
       </c>
       <c r="H140" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I140" s="3">
         <v>8</v>
@@ -16185,7 +16185,7 @@
     </row>
     <row r="141" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C141" s="1">
         <v>41092</v>
@@ -16196,7 +16196,7 @@
         <v>180</v>
       </c>
       <c r="H141" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I141" s="3">
         <v>8</v>
@@ -16284,7 +16284,7 @@
     </row>
     <row r="142" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C142" s="1">
         <v>41096</v>
@@ -16293,16 +16293,16 @@
         <v>10</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F142" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G142">
         <v>184</v>
       </c>
       <c r="H142" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I142" s="3">
         <v>8</v>

</xml_diff>

<commit_message>
Fixed errors in PhenologyObserved tab
</commit_message>
<xml_diff>
--- a/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
+++ b/Tests/UnderReview/Cotton/Observed/BDKObserved.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ApsimX\Tests\UnderReview\Cotton\Observed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE9E524-11BE-43A6-854B-52B6DF496BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AFE82E-8660-449B-946B-D34A0B22EC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{FBA18FA7-8D49-4A23-B648-57CB41343816}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CottonObserved!$A$1:$BM$142</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PhenologyObserved!$A$1:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PhenologyObserved!$A$1:$G$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="84">
   <si>
     <t>SimulationName</t>
   </si>
@@ -275,9 +275,6 @@
   </si>
   <si>
     <t>AboveGround.Partitioning.Boll</t>
-  </si>
-  <si>
-    <t>Cotton.Phenology.EmergenceDAS</t>
   </si>
   <si>
     <t>Cotton.Phenology.SquaringDAS</t>
@@ -14125,23 +14122,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF74C9E2-DF23-4CC5-866C-B668BAF53D64}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14155,137 +14151,217 @@
         <v>80</v>
       </c>
       <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
         <v>81</v>
-      </c>
-      <c r="F1" t="s">
-        <v>84</v>
       </c>
       <c r="G1" t="s">
         <v>82</v>
       </c>
-      <c r="H1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>21</v>
+      </c>
       <c r="C2" s="2">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="E2" s="2">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="F2" s="2">
-        <v>94</v>
+        <v>164</v>
       </c>
       <c r="G2" s="2">
-        <v>164</v>
-      </c>
-      <c r="H2" s="2">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>23</v>
+      </c>
       <c r="C3" s="2">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D3" s="2">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E3" s="2">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="F3" s="2">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="G3" s="2">
-        <v>144</v>
-      </c>
-      <c r="H3" s="2">
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>26</v>
+      </c>
       <c r="C4" s="2">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="E4" s="2">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="F4" s="2">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="G4" s="2">
-        <v>154</v>
-      </c>
-      <c r="H4" s="2">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>29</v>
+      </c>
       <c r="C5" s="2">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D5" s="2">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="E5" s="2">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="F5" s="2">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="G5" s="2">
-        <v>130</v>
-      </c>
-      <c r="H5" s="2">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>35</v>
+      </c>
       <c r="C6" s="2">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D6" s="2">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="F6" s="2">
-        <v>86</v>
+        <v>159</v>
       </c>
       <c r="G6" s="2">
-        <v>159</v>
-      </c>
-      <c r="H6" s="2">
         <v>184</v>
       </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>